<commit_message>
edited the data wrangling sheet, made the summary model tables and addedsome notes to the project notes.
</commit_message>
<xml_diff>
--- a/Figures/summaries_csvs/model_summary.xlsx
+++ b/Figures/summaries_csvs/model_summary.xlsx
@@ -1,35 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunalpalawat/Documents/GitHub/project-harvest-fork/Figures/summaries_csvs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gift/Documents/Rprojects/project-harvest/Figures/summaries_csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7973F3BD-3F20-7B41-9D12-5FA680A5CE02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E70B8FE-F69C-C549-B3F8-6F6254F0A067}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1060" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="2" xr2:uid="{BBA561B4-B8F2-A543-83D5-E4C6EA31C59C}"/>
+    <workbookView xWindow="1040" yWindow="500" windowWidth="27740" windowHeight="17500" activeTab="2" xr2:uid="{BBA561B4-B8F2-A543-83D5-E4C6EA31C59C}"/>
   </bookViews>
   <sheets>
     <sheet name="exceedances" sheetId="1" r:id="rId1"/>
-    <sheet name="PCAs" sheetId="2" r:id="rId2"/>
-    <sheet name="HDS" sheetId="3" r:id="rId3"/>
-    <sheet name="exceedance%_overall" sheetId="4" r:id="rId4"/>
-    <sheet name="exceedance%_com" sheetId="5" r:id="rId5"/>
-    <sheet name="exceedance%_site" sheetId="6" r:id="rId6"/>
-    <sheet name="exceedance%_ssn" sheetId="7" r:id="rId7"/>
+    <sheet name="pli_and_hds_modelling" sheetId="8" r:id="rId2"/>
+    <sheet name="pli only" sheetId="9" r:id="rId3"/>
+    <sheet name="PCAs" sheetId="2" r:id="rId4"/>
+    <sheet name="HDS" sheetId="3" r:id="rId5"/>
+    <sheet name="exceedance%_overall" sheetId="4" r:id="rId6"/>
+    <sheet name="exceedance%_com" sheetId="5" r:id="rId7"/>
+    <sheet name="exceedance%_site" sheetId="6" r:id="rId8"/>
+    <sheet name="exceedance%_ssn" sheetId="7" r:id="rId9"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'exceedance%_com'!$A$1:$H$73</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'exceedance%_overall'!$A$1:$G$19</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'exceedance%_site'!$A$1:$H$2935</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'exceedance%_ssn'!$A$1:$H$37</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">HDS!$K$32:$K$50</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">PCAs!$A$1:$P$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'exceedance%_com'!$A$1:$H$73</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">'exceedance%_overall'!$A$1:$G$19</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'exceedance%_site'!$A$1:$H$2935</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'exceedance%_ssn'!$A$1:$H$37</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">HDS!$K$32:$K$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">PCAs!$A$1:$P$22</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -50,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10582" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10697" uniqueCount="349">
   <si>
     <t>Analyte</t>
   </si>
@@ -1050,6 +1052,72 @@
   <si>
     <t>pH almost signif (p = 0.07); low adj r2</t>
   </si>
+  <si>
+    <t>Infrastructural Factor</t>
+  </si>
+  <si>
+    <t>Model Type</t>
+  </si>
+  <si>
+    <t>Conditional R square</t>
+  </si>
+  <si>
+    <t>Marginal R square</t>
+  </si>
+  <si>
+    <t>Q67: #Do you clean parts of your roof draining system (like the debris filter, gutters, scuppers, etc.)?</t>
+  </si>
+  <si>
+    <t>Q67</t>
+  </si>
+  <si>
+    <t>seasonMonsoon</t>
+  </si>
+  <si>
+    <t>RMSE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">seasonMonsoon </t>
+  </si>
+  <si>
+    <t>Q71: Do you treat or wash your cistern with anything?</t>
+  </si>
+  <si>
+    <t>Q79: Do you ever remove the screen/filter and leave your cistern without the filter?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Linear mixed model </t>
+  </si>
+  <si>
+    <t>Q76: Does your cistern have a first flush?</t>
+  </si>
+  <si>
+    <t>Q77: Does your cistern have a screen/filter for incoming water from down spout on top of the tank?</t>
+  </si>
+  <si>
+    <t>Linear regression</t>
+  </si>
+  <si>
+    <t>No value</t>
+  </si>
+  <si>
+    <t>Hayden-Winklemann</t>
+  </si>
+  <si>
+    <t>Globe</t>
+  </si>
+  <si>
+    <t>prox.normal</t>
+  </si>
+  <si>
+    <t>Reference levels</t>
+  </si>
+  <si>
+    <t>Low R square= Less than 10%</t>
+  </si>
+  <si>
+    <t xml:space="preserve">prox.normal </t>
+  </si>
 </sst>
 </file>
 
@@ -1062,7 +1130,7 @@
     <numFmt numFmtId="167" formatCode="0.000"/>
     <numFmt numFmtId="168" formatCode="0.0"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1085,8 +1153,25 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1141,8 +1226,14 @@
         <bgColor rgb="FF000000"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1335,11 +1426,41 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="thin">
+        <color theme="8"/>
+      </top>
+      <bottom style="medium">
+        <color theme="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="8"/>
+      </left>
+      <right style="thin">
+        <color theme="8"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="92">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -1420,6 +1541,61 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1436,24 +1612,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1468,61 +1626,208 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" quotePrefix="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color theme="8"/>
+        </left>
+        <right style="thin">
+          <color theme="8"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <border outline="0">
+        <left style="thin">
+          <color theme="8"/>
+        </left>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="0"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1533,6 +1838,56 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{332D19AC-328C-4243-9CEE-6380094CC0E5}" name="pli_plus_hds_model" displayName="pli_plus_hds_model" ref="A1:K41" headerRowDxfId="7" dataDxfId="8">
+  <autoFilter ref="A1:K41" xr:uid="{332D19AC-328C-4243-9CEE-6380094CC0E5}"/>
+  <tableColumns count="11">
+    <tableColumn id="1" xr3:uid="{92165279-5B62-5143-99E5-BC33DE6B6F7B}" name="Community" totalsRowLabel="Total" dataDxfId="13" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E8C220B7-0331-1348-8864-7CDC70A233BF}" name="Infrastructural Factor" dataDxfId="12" totalsRowDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{7B0E1DF0-4AE8-8643-9336-E6B7FAAC98B5}" name="Model Type"/>
+    <tableColumn id="4" xr3:uid="{58B4AA9C-B6AF-B447-BC9C-049A219684AF}" name="Levels"/>
+    <tableColumn id="5" xr3:uid="{21A01350-C8E4-1C47-94BA-D5794FE8128E}" name="Estimate"/>
+    <tableColumn id="6" xr3:uid="{BA142DBD-3396-C148-AA91-849E4EF81CA9}" name="Standard Error"/>
+    <tableColumn id="7" xr3:uid="{7B5FF10C-5FBF-AF4A-9BD5-DFB74EF276E6}" name="Conditional R square" dataDxfId="11" totalsRowDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{E9DD9E05-B76E-5B47-85AB-997943D27B54}" name="Marginal R square" dataDxfId="10" totalsRowDxfId="5"/>
+    <tableColumn id="9" xr3:uid="{B6A7AC17-47BA-7F40-B110-1CA6D30C22BD}" name="RMSE" dataDxfId="9" totalsRowDxfId="6"/>
+    <tableColumn id="10" xr3:uid="{16F95216-CD61-AB4C-A209-F074E1F74973}" name="p-value"/>
+    <tableColumn id="11" xr3:uid="{18A203FA-0D11-2049-B943-15415D57623B}" name="Reference levels" totalsRowFunction="count"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight20" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{33E07BFC-D947-F846-9235-68D258BB4795}" name="Table5" displayName="Table5" ref="A1:J11" totalsRowShown="0" headerRowDxfId="0" tableBorderDxfId="1">
+  <autoFilter ref="A1:J11" xr:uid="{33E07BFC-D947-F846-9235-68D258BB4795}">
+    <filterColumn colId="0" hiddenButton="1"/>
+    <filterColumn colId="1" hiddenButton="1"/>
+    <filterColumn colId="2" hiddenButton="1"/>
+    <filterColumn colId="3" hiddenButton="1"/>
+    <filterColumn colId="4" hiddenButton="1"/>
+    <filterColumn colId="5" hiddenButton="1"/>
+    <filterColumn colId="6" hiddenButton="1"/>
+    <filterColumn colId="7" hiddenButton="1"/>
+    <filterColumn colId="8" hiddenButton="1"/>
+    <filterColumn colId="9" hiddenButton="1"/>
+  </autoFilter>
+  <tableColumns count="10">
+    <tableColumn id="1" xr3:uid="{094D909F-012F-DB46-9CF6-5662BAB45E5B}" name="Community" dataCellStyle="Normal"/>
+    <tableColumn id="2" xr3:uid="{28A00A5D-0CE1-214C-ACED-D9C7E8E91C9F}" name="Model Type" dataCellStyle="Normal"/>
+    <tableColumn id="3" xr3:uid="{E5136E0C-70AF-7140-B1C3-7B3A1FE5232F}" name="Levels" dataCellStyle="Normal"/>
+    <tableColumn id="4" xr3:uid="{D32C054E-0831-BE41-AB7A-0801AAF5855F}" name="Estimate" dataCellStyle="Normal"/>
+    <tableColumn id="5" xr3:uid="{2C556E22-11F9-E54A-B84D-0B0E092606F3}" name="Standard Error" dataCellStyle="Normal"/>
+    <tableColumn id="6" xr3:uid="{499AE85D-55DD-2249-A5FD-4E8F1B98B124}" name="Conditional R square" dataCellStyle="Normal"/>
+    <tableColumn id="7" xr3:uid="{444468D3-0ABF-9E44-889D-2CFBCFF5DBB3}" name="Marginal R square"/>
+    <tableColumn id="8" xr3:uid="{6B4B36B8-72B1-B84C-AAB7-355A56F0EAF8}" name="RMSE"/>
+    <tableColumn id="9" xr3:uid="{241F30D3-1798-5D40-9911-B4896D381D16}" name="p-value"/>
+    <tableColumn id="10" xr3:uid="{91231617-62C7-F748-811D-B41C183C3A6D}" name="Reference levels"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight18" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1834,8 +2189,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF0D4DAB-8658-6540-A6EF-06375FD0FCC4}">
   <dimension ref="A1:AU100"/>
   <sheetViews>
-    <sheetView topLeftCell="AH82" zoomScale="75" workbookViewId="0">
-      <selection activeCell="AT89" sqref="AT89:AT91"/>
+    <sheetView topLeftCell="AG80" zoomScale="75" workbookViewId="0">
+      <selection activeCell="AP88" sqref="AP88:AU88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2287,27 +2642,27 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M31" s="63" t="s">
+      <c r="M31" s="73" t="s">
         <v>65</v>
       </c>
-      <c r="N31" s="63"/>
-      <c r="O31" s="63"/>
-      <c r="P31" s="63"/>
-      <c r="Q31" s="63"/>
+      <c r="N31" s="73"/>
+      <c r="O31" s="73"/>
+      <c r="P31" s="73"/>
+      <c r="Q31" s="73"/>
     </row>
     <row r="32" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="M32" s="64" t="s">
+      <c r="M32" s="74" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="62" t="s">
+      <c r="N32" s="72" t="s">
         <v>53</v>
       </c>
-      <c r="O32" s="62"/>
-      <c r="P32" s="62"/>
-      <c r="Q32" s="62"/>
+      <c r="O32" s="72"/>
+      <c r="P32" s="72"/>
+      <c r="Q32" s="72"/>
     </row>
     <row r="33" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="M33" s="61"/>
+      <c r="M33" s="65"/>
       <c r="N33" s="13" t="s">
         <v>21</v>
       </c>
@@ -2381,29 +2736,29 @@
       </c>
     </row>
     <row r="44" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="Y44" s="57" t="s">
+      <c r="Y44" s="78" t="s">
         <v>77</v>
       </c>
-      <c r="Z44" s="57"/>
-      <c r="AA44" s="57"/>
-      <c r="AB44" s="57"/>
-      <c r="AC44" s="57"/>
+      <c r="Z44" s="78"/>
+      <c r="AA44" s="78"/>
+      <c r="AB44" s="78"/>
+      <c r="AC44" s="78"/>
     </row>
     <row r="45" spans="13:29" x14ac:dyDescent="0.2">
       <c r="Y45" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="Z45" s="58" t="s">
+      <c r="Z45" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="AA45" s="58"/>
-      <c r="AB45" s="58"/>
+      <c r="AA45" s="79"/>
+      <c r="AB45" s="79"/>
       <c r="AC45" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="46" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="Y46" s="59" t="s">
+      <c r="Y46" s="63" t="s">
         <v>67</v>
       </c>
       <c r="Z46" s="8" t="s">
@@ -2417,7 +2772,7 @@
       </c>
     </row>
     <row r="47" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="Y47" s="60"/>
+      <c r="Y47" s="64"/>
       <c r="Z47" s="8">
         <v>0</v>
       </c>
@@ -2429,7 +2784,7 @@
       </c>
     </row>
     <row r="48" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="Y48" s="60"/>
+      <c r="Y48" s="64"/>
       <c r="Z48" s="8">
         <v>0.5</v>
       </c>
@@ -2441,7 +2796,7 @@
       </c>
     </row>
     <row r="49" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y49" s="60"/>
+      <c r="Y49" s="64"/>
       <c r="Z49" s="8">
         <v>1</v>
       </c>
@@ -2453,7 +2808,7 @@
       </c>
     </row>
     <row r="50" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y50" s="60"/>
+      <c r="Y50" s="64"/>
       <c r="Z50" s="8">
         <v>1.5</v>
       </c>
@@ -2465,7 +2820,7 @@
       </c>
     </row>
     <row r="51" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y51" s="61"/>
+      <c r="Y51" s="65"/>
       <c r="Z51" s="11">
         <v>2</v>
       </c>
@@ -2478,7 +2833,7 @@
       <c r="AC51" s="13"/>
     </row>
     <row r="52" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y52" s="59" t="s">
+      <c r="Y52" s="63" t="s">
         <v>69</v>
       </c>
       <c r="Z52" s="1" t="s">
@@ -2487,62 +2842,62 @@
       <c r="AA52" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AC52" s="54" t="s">
+      <c r="AC52" s="75" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="53" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y53" s="60"/>
+      <c r="Y53" s="64"/>
       <c r="Z53" s="1">
         <v>0</v>
       </c>
       <c r="AA53" s="34">
         <v>6.1733623452348702E-2</v>
       </c>
-      <c r="AC53" s="56"/>
+      <c r="AC53" s="77"/>
     </row>
     <row r="54" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y54" s="60"/>
+      <c r="Y54" s="64"/>
       <c r="Z54" s="1">
         <v>2</v>
       </c>
       <c r="AA54" s="34">
         <v>1.20772053410085E-2</v>
       </c>
-      <c r="AC54" s="56"/>
+      <c r="AC54" s="77"/>
     </row>
     <row r="55" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y55" s="60"/>
+      <c r="Y55" s="64"/>
       <c r="Z55" s="1">
         <v>4</v>
       </c>
       <c r="AA55" s="31">
         <v>2.2662402083130201E-3</v>
       </c>
-      <c r="AC55" s="56"/>
+      <c r="AC55" s="77"/>
     </row>
     <row r="56" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y56" s="60"/>
+      <c r="Y56" s="64"/>
       <c r="Z56" s="1">
         <v>6</v>
       </c>
       <c r="AA56" s="28">
         <v>4.2184786680835203E-4</v>
       </c>
-      <c r="AC56" s="56"/>
+      <c r="AC56" s="77"/>
     </row>
     <row r="57" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y57" s="60"/>
+      <c r="Y57" s="64"/>
       <c r="Z57" s="1">
         <v>8</v>
       </c>
       <c r="AA57" s="28">
         <v>7.8406646322768398E-5</v>
       </c>
-      <c r="AC57" s="56"/>
+      <c r="AC57" s="77"/>
     </row>
     <row r="58" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y58" s="61"/>
+      <c r="Y58" s="65"/>
       <c r="Z58" s="13">
         <v>10</v>
       </c>
@@ -2550,10 +2905,10 @@
         <v>1.4568956039108299E-5</v>
       </c>
       <c r="AB58" s="13"/>
-      <c r="AC58" s="55"/>
+      <c r="AC58" s="76"/>
     </row>
     <row r="59" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y59" s="59" t="s">
+      <c r="Y59" s="63" t="s">
         <v>73</v>
       </c>
       <c r="Z59" s="1" t="s">
@@ -2562,72 +2917,72 @@
       <c r="AA59" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AC59" s="54" t="s">
+      <c r="AC59" s="75" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="60" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y60" s="60"/>
+      <c r="Y60" s="64"/>
       <c r="Z60" s="1">
         <v>0</v>
       </c>
       <c r="AA60" s="34">
         <v>4.213704983443E-2</v>
       </c>
-      <c r="AC60" s="56"/>
+      <c r="AC60" s="77"/>
     </row>
     <row r="61" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y61" s="60"/>
+      <c r="Y61" s="64"/>
       <c r="Z61" s="1">
         <v>4</v>
       </c>
       <c r="AA61" s="36">
         <v>0.70383460067707004</v>
       </c>
-      <c r="AC61" s="56"/>
+      <c r="AC61" s="77"/>
     </row>
     <row r="62" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y62" s="60"/>
+      <c r="Y62" s="64"/>
       <c r="Z62" s="1">
         <v>8</v>
       </c>
       <c r="AA62" s="36">
         <v>0.99227108557330002</v>
       </c>
-      <c r="AC62" s="56"/>
+      <c r="AC62" s="77"/>
     </row>
     <row r="63" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y63" s="60"/>
+      <c r="Y63" s="64"/>
       <c r="Z63" s="1">
         <v>12</v>
       </c>
       <c r="AA63" s="37">
         <v>0.99985583826317304</v>
       </c>
-      <c r="AC63" s="56"/>
+      <c r="AC63" s="77"/>
     </row>
     <row r="64" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y64" s="60"/>
+      <c r="Y64" s="64"/>
       <c r="Z64" s="1">
         <v>16</v>
       </c>
       <c r="AA64" s="37">
         <v>0.99999733107778499</v>
       </c>
-      <c r="AC64" s="56"/>
+      <c r="AC64" s="77"/>
     </row>
     <row r="65" spans="25:36" x14ac:dyDescent="0.2">
-      <c r="Y65" s="60"/>
+      <c r="Y65" s="64"/>
       <c r="Z65" s="1">
         <v>20</v>
       </c>
       <c r="AA65" s="37">
         <v>0.99999995059606805</v>
       </c>
-      <c r="AC65" s="56"/>
+      <c r="AC65" s="77"/>
     </row>
     <row r="66" spans="25:36" x14ac:dyDescent="0.2">
-      <c r="Y66" s="61"/>
+      <c r="Y66" s="65"/>
       <c r="Z66" s="13">
         <v>24</v>
       </c>
@@ -2635,7 +2990,7 @@
         <v>0.99999999908549497</v>
       </c>
       <c r="AB66" s="13"/>
-      <c r="AC66" s="55"/>
+      <c r="AC66" s="76"/>
     </row>
     <row r="71" spans="25:36" x14ac:dyDescent="0.2">
       <c r="AD71" s="1" t="s">
@@ -2684,7 +3039,7 @@
       </c>
     </row>
     <row r="74" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD74" s="54" t="s">
+      <c r="AD74" s="75" t="s">
         <v>9</v>
       </c>
       <c r="AE74" s="48" t="s">
@@ -2704,7 +3059,7 @@
       </c>
     </row>
     <row r="75" spans="25:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="AD75" s="55"/>
+      <c r="AD75" s="76"/>
       <c r="AE75" s="49" t="s">
         <v>13</v>
       </c>
@@ -2722,7 +3077,7 @@
       </c>
     </row>
     <row r="76" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD76" s="54" t="s">
+      <c r="AD76" s="75" t="s">
         <v>10</v>
       </c>
       <c r="AE76" s="48" t="s">
@@ -2742,7 +3097,7 @@
       </c>
     </row>
     <row r="77" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD77" s="56"/>
+      <c r="AD77" s="77"/>
       <c r="AE77" s="50" t="s">
         <v>17</v>
       </c>
@@ -2760,7 +3115,7 @@
       </c>
     </row>
     <row r="78" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD78" s="55"/>
+      <c r="AD78" s="76"/>
       <c r="AE78" s="49" t="s">
         <v>12</v>
       </c>
@@ -2778,7 +3133,7 @@
       </c>
     </row>
     <row r="79" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD79" s="54" t="s">
+      <c r="AD79" s="75" t="s">
         <v>11</v>
       </c>
       <c r="AE79" s="48" t="s">
@@ -2798,7 +3153,7 @@
       </c>
     </row>
     <row r="80" spans="25:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="AD80" s="56"/>
+      <c r="AD80" s="77"/>
       <c r="AE80" s="50" t="s">
         <v>19</v>
       </c>
@@ -2816,7 +3171,7 @@
       </c>
     </row>
     <row r="81" spans="30:47" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD81" s="56"/>
+      <c r="AD81" s="77"/>
       <c r="AE81" s="50" t="s">
         <v>13</v>
       </c>
@@ -2834,7 +3189,7 @@
       </c>
     </row>
     <row r="82" spans="30:47" ht="34" x14ac:dyDescent="0.2">
-      <c r="AD82" s="55"/>
+      <c r="AD82" s="76"/>
       <c r="AE82" s="49" t="s">
         <v>15</v>
       </c>
@@ -2852,369 +3207,358 @@
       </c>
     </row>
     <row r="87" spans="30:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AL87" s="63" t="s">
+      <c r="AL87" s="73" t="s">
         <v>274</v>
       </c>
-      <c r="AM87" s="63"/>
-      <c r="AN87" s="63"/>
-      <c r="AO87" s="63"/>
-      <c r="AP87" s="63"/>
-      <c r="AQ87" s="63"/>
-      <c r="AR87" s="63"/>
-      <c r="AS87" s="63"/>
-      <c r="AT87" s="63"/>
-      <c r="AU87" s="63"/>
+      <c r="AM87" s="73"/>
+      <c r="AN87" s="73"/>
+      <c r="AO87" s="73"/>
+      <c r="AP87" s="73"/>
+      <c r="AQ87" s="73"/>
+      <c r="AR87" s="73"/>
+      <c r="AS87" s="73"/>
+      <c r="AT87" s="73"/>
+      <c r="AU87" s="73"/>
     </row>
     <row r="88" spans="30:47" ht="35" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="AL88" s="70" t="s">
+      <c r="AL88" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="AM88" s="70" t="s">
+      <c r="AM88" s="55" t="s">
         <v>275</v>
       </c>
-      <c r="AN88" s="70" t="s">
-        <v>0</v>
-      </c>
-      <c r="AO88" s="70" t="s">
+      <c r="AN88" s="55" t="s">
+        <v>0</v>
+      </c>
+      <c r="AO88" s="55" t="s">
         <v>276</v>
       </c>
-      <c r="AP88" s="71" t="s">
+      <c r="AP88" s="56" t="s">
         <v>298</v>
       </c>
-      <c r="AQ88" s="70" t="s">
+      <c r="AQ88" s="55" t="s">
         <v>281</v>
       </c>
-      <c r="AR88" s="70" t="s">
+      <c r="AR88" s="55" t="s">
         <v>282</v>
       </c>
-      <c r="AS88" s="70" t="s">
+      <c r="AS88" s="55" t="s">
         <v>283</v>
       </c>
-      <c r="AT88" s="70" t="s">
+      <c r="AT88" s="55" t="s">
         <v>303</v>
       </c>
-      <c r="AU88" s="70" t="s">
+      <c r="AU88" s="55" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="89" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL89" s="72" t="s">
+      <c r="AL89" s="69" t="s">
         <v>9</v>
       </c>
-      <c r="AM89" s="73" t="s">
+      <c r="AM89" s="66" t="s">
         <v>279</v>
       </c>
-      <c r="AN89" s="59" t="s">
+      <c r="AN89" s="63" t="s">
         <v>13</v>
       </c>
       <c r="AO89" s="40" t="s">
         <v>284</v>
       </c>
-      <c r="AP89" s="74">
+      <c r="AP89" s="57">
         <v>-2.0699999999999998</v>
       </c>
-      <c r="AQ89" s="74">
+      <c r="AQ89" s="57">
         <v>0.372</v>
       </c>
-      <c r="AR89" s="74">
+      <c r="AR89" s="57">
         <v>-5.57</v>
       </c>
-      <c r="AS89" s="74" t="s">
+      <c r="AS89" s="57" t="s">
         <v>288</v>
       </c>
-      <c r="AT89" s="72" t="s">
+      <c r="AT89" s="69" t="s">
         <v>287</v>
       </c>
-      <c r="AU89" s="73" t="s">
+      <c r="AU89" s="66" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="90" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL90" s="75"/>
-      <c r="AM90" s="76"/>
-      <c r="AN90" s="77"/>
-      <c r="AO90" s="78" t="s">
+      <c r="AL90" s="70"/>
+      <c r="AM90" s="67"/>
+      <c r="AN90" s="64"/>
+      <c r="AO90" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AP90" s="79">
+      <c r="AP90" s="58">
         <v>-0.82199999999999995</v>
       </c>
-      <c r="AQ90" s="79">
+      <c r="AQ90" s="58">
         <v>0.25700000000000001</v>
       </c>
-      <c r="AR90" s="79">
+      <c r="AR90" s="58">
         <v>-3.19</v>
       </c>
-      <c r="AS90" s="79">
+      <c r="AS90" s="58">
         <v>1E-3</v>
       </c>
-      <c r="AT90" s="75"/>
-      <c r="AU90" s="76"/>
+      <c r="AT90" s="70"/>
+      <c r="AU90" s="67"/>
     </row>
     <row r="91" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL91" s="80"/>
-      <c r="AM91" s="81"/>
-      <c r="AN91" s="61"/>
+      <c r="AL91" s="71"/>
+      <c r="AM91" s="68"/>
+      <c r="AN91" s="65"/>
       <c r="AO91" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="AP91" s="82" t="s">
+      <c r="AP91" s="59" t="s">
         <v>290</v>
       </c>
-      <c r="AQ91" s="82">
+      <c r="AQ91" s="59">
         <v>0.503</v>
       </c>
-      <c r="AR91" s="82">
+      <c r="AR91" s="59">
         <v>3.78</v>
       </c>
-      <c r="AS91" s="82">
+      <c r="AS91" s="59">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="AT91" s="80"/>
-      <c r="AU91" s="81"/>
+      <c r="AT91" s="71"/>
+      <c r="AU91" s="68"/>
     </row>
     <row r="92" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL92" s="72" t="s">
+      <c r="AL92" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="AM92" s="72" t="s">
+      <c r="AM92" s="69" t="s">
         <v>280</v>
       </c>
-      <c r="AN92" s="59" t="s">
+      <c r="AN92" s="63" t="s">
         <v>12</v>
       </c>
       <c r="AO92" s="40" t="s">
         <v>284</v>
       </c>
-      <c r="AP92" s="74">
+      <c r="AP92" s="57">
         <v>-2.57</v>
       </c>
-      <c r="AQ92" s="74">
+      <c r="AQ92" s="57">
         <v>0.51400000000000001</v>
       </c>
-      <c r="AR92" s="74" t="s">
+      <c r="AR92" s="57" t="s">
         <v>289</v>
       </c>
-      <c r="AS92" s="74" t="s">
+      <c r="AS92" s="57" t="s">
         <v>288</v>
       </c>
-      <c r="AT92" s="72" t="s">
+      <c r="AT92" s="69" t="s">
         <v>287</v>
       </c>
-      <c r="AU92" s="73" t="s">
+      <c r="AU92" s="66" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="93" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL93" s="75"/>
-      <c r="AM93" s="75"/>
-      <c r="AN93" s="77"/>
-      <c r="AO93" s="78" t="s">
+      <c r="AL93" s="70"/>
+      <c r="AM93" s="70"/>
+      <c r="AN93" s="64"/>
+      <c r="AO93" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AP93" s="79">
+      <c r="AP93" s="58">
         <v>-1.39</v>
       </c>
-      <c r="AQ93" s="79">
+      <c r="AQ93" s="58">
         <v>0.497</v>
       </c>
-      <c r="AR93" s="79">
+      <c r="AR93" s="58">
         <v>-2.79</v>
       </c>
-      <c r="AS93" s="79">
+      <c r="AS93" s="58">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AT93" s="75"/>
-      <c r="AU93" s="76"/>
+      <c r="AT93" s="70"/>
+      <c r="AU93" s="67"/>
     </row>
     <row r="94" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL94" s="75"/>
-      <c r="AM94" s="75"/>
-      <c r="AN94" s="77"/>
-      <c r="AO94" s="78" t="s">
+      <c r="AL94" s="70"/>
+      <c r="AM94" s="70"/>
+      <c r="AN94" s="64"/>
+      <c r="AO94" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="AP94" s="79">
+      <c r="AP94" s="58">
         <v>2.0699999999999998</v>
       </c>
-      <c r="AQ94" s="79">
+      <c r="AQ94" s="58">
         <v>0.68400000000000005</v>
       </c>
-      <c r="AR94" s="79">
+      <c r="AR94" s="58">
         <v>3.0310000000000001</v>
       </c>
-      <c r="AS94" s="79">
+      <c r="AS94" s="58">
         <v>2E-3</v>
       </c>
-      <c r="AT94" s="75"/>
-      <c r="AU94" s="76"/>
+      <c r="AT94" s="70"/>
+      <c r="AU94" s="67"/>
     </row>
     <row r="95" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL95" s="75"/>
-      <c r="AM95" s="76" t="s">
+      <c r="AL95" s="70"/>
+      <c r="AM95" s="67" t="s">
         <v>279</v>
       </c>
-      <c r="AN95" s="77" t="s">
+      <c r="AN95" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="AO95" s="83" t="s">
+      <c r="AO95" t="s">
         <v>284</v>
       </c>
-      <c r="AP95" s="79">
+      <c r="AP95" s="58">
         <v>-3.36</v>
       </c>
-      <c r="AQ95" s="79">
+      <c r="AQ95" s="58">
         <v>0.68600000000000005</v>
       </c>
-      <c r="AR95" s="79" t="s">
+      <c r="AR95" s="58" t="s">
         <v>292</v>
       </c>
-      <c r="AS95" s="79" t="s">
+      <c r="AS95" s="58" t="s">
         <v>288</v>
       </c>
-      <c r="AT95" s="75" t="s">
+      <c r="AT95" s="70" t="s">
         <v>287</v>
       </c>
-      <c r="AU95" s="76" t="s">
+      <c r="AU95" s="67" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="96" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL96" s="75"/>
-      <c r="AM96" s="76"/>
-      <c r="AN96" s="77"/>
-      <c r="AO96" s="78" t="s">
+      <c r="AL96" s="70"/>
+      <c r="AM96" s="67"/>
+      <c r="AN96" s="64"/>
+      <c r="AO96" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AP96" s="79">
+      <c r="AP96" s="58">
         <v>-1.91</v>
       </c>
-      <c r="AQ96" s="79">
+      <c r="AQ96" s="58">
         <v>0.63200000000000001</v>
       </c>
-      <c r="AR96" s="79" t="s">
+      <c r="AR96" s="58" t="s">
         <v>293</v>
       </c>
-      <c r="AS96" s="79">
+      <c r="AS96" s="58">
         <v>2E-3</v>
       </c>
-      <c r="AT96" s="75"/>
-      <c r="AU96" s="76"/>
+      <c r="AT96" s="70"/>
+      <c r="AU96" s="67"/>
     </row>
     <row r="97" spans="38:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL97" s="80"/>
-      <c r="AM97" s="81"/>
-      <c r="AN97" s="61"/>
+      <c r="AL97" s="71"/>
+      <c r="AM97" s="68"/>
+      <c r="AN97" s="65"/>
       <c r="AO97" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="AP97" s="82">
+      <c r="AP97" s="59">
         <v>3.31</v>
       </c>
-      <c r="AQ97" s="82">
+      <c r="AQ97" s="59">
         <v>0.84199999999999997</v>
       </c>
-      <c r="AR97" s="82" t="s">
+      <c r="AR97" s="59" t="s">
         <v>294</v>
       </c>
-      <c r="AS97" s="82" t="s">
+      <c r="AS97" s="59" t="s">
         <v>288</v>
       </c>
-      <c r="AT97" s="80"/>
-      <c r="AU97" s="81"/>
+      <c r="AT97" s="71"/>
+      <c r="AU97" s="68"/>
     </row>
     <row r="98" spans="38:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL98" s="72" t="s">
+      <c r="AL98" s="69" t="s">
         <v>11</v>
       </c>
-      <c r="AM98" s="73" t="s">
+      <c r="AM98" s="66" t="s">
         <v>279</v>
       </c>
-      <c r="AN98" s="59" t="s">
+      <c r="AN98" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="AO98" s="84" t="s">
+      <c r="AO98" s="60" t="s">
         <v>284</v>
       </c>
-      <c r="AP98" s="74">
+      <c r="AP98" s="57">
         <v>-3.67</v>
       </c>
-      <c r="AQ98" s="74">
+      <c r="AQ98" s="57">
         <v>0.434</v>
       </c>
-      <c r="AR98" s="74" t="s">
+      <c r="AR98" s="57" t="s">
         <v>295</v>
       </c>
-      <c r="AS98" s="74" t="s">
+      <c r="AS98" s="57" t="s">
         <v>288</v>
       </c>
-      <c r="AT98" s="72" t="s">
+      <c r="AT98" s="69" t="s">
         <v>287</v>
       </c>
-      <c r="AU98" s="73" t="s">
+      <c r="AU98" s="66" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="99" spans="38:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL99" s="75"/>
-      <c r="AM99" s="76"/>
-      <c r="AN99" s="77"/>
-      <c r="AO99" s="78" t="s">
+      <c r="AL99" s="70"/>
+      <c r="AM99" s="67"/>
+      <c r="AN99" s="64"/>
+      <c r="AO99" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="AP99" s="79">
+      <c r="AP99" s="58">
         <v>-0.56299999999999994</v>
       </c>
-      <c r="AQ99" s="79">
+      <c r="AQ99" s="58">
         <v>0.27700000000000002</v>
       </c>
-      <c r="AR99" s="79" t="s">
+      <c r="AR99" s="58" t="s">
         <v>296</v>
       </c>
-      <c r="AS99" s="79">
+      <c r="AS99" s="58">
         <v>0.04</v>
       </c>
-      <c r="AT99" s="75"/>
-      <c r="AU99" s="76"/>
+      <c r="AT99" s="70"/>
+      <c r="AU99" s="67"/>
     </row>
     <row r="100" spans="38:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL100" s="80"/>
-      <c r="AM100" s="81"/>
-      <c r="AN100" s="61"/>
+      <c r="AL100" s="71"/>
+      <c r="AM100" s="68"/>
+      <c r="AN100" s="65"/>
       <c r="AO100" s="13" t="s">
         <v>286</v>
       </c>
-      <c r="AP100" s="82" t="s">
+      <c r="AP100" s="59" t="s">
         <v>291</v>
       </c>
-      <c r="AQ100" s="82">
+      <c r="AQ100" s="59">
         <v>0.502</v>
       </c>
-      <c r="AR100" s="82" t="s">
+      <c r="AR100" s="59" t="s">
         <v>297</v>
       </c>
-      <c r="AS100" s="82" t="s">
+      <c r="AS100" s="59" t="s">
         <v>288</v>
       </c>
-      <c r="AT100" s="80"/>
-      <c r="AU100" s="81"/>
+      <c r="AT100" s="71"/>
+      <c r="AU100" s="68"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="AN98:AN100"/>
-    <mergeCell ref="AM98:AM100"/>
-    <mergeCell ref="AL98:AL100"/>
-    <mergeCell ref="AL92:AL97"/>
-    <mergeCell ref="AM92:AM94"/>
-    <mergeCell ref="AM95:AM97"/>
-    <mergeCell ref="AN92:AN94"/>
-    <mergeCell ref="AN95:AN97"/>
-    <mergeCell ref="AT92:AT94"/>
-    <mergeCell ref="AU92:AU94"/>
-    <mergeCell ref="AU95:AU97"/>
-    <mergeCell ref="AT95:AT97"/>
-    <mergeCell ref="AT98:AT100"/>
-    <mergeCell ref="AU98:AU100"/>
+    <mergeCell ref="Y59:Y66"/>
+    <mergeCell ref="AC52:AC58"/>
+    <mergeCell ref="AC59:AC66"/>
     <mergeCell ref="N32:Q32"/>
     <mergeCell ref="M31:Q31"/>
     <mergeCell ref="M32:M33"/>
@@ -3231,15 +3575,1149 @@
     <mergeCell ref="Z45:AB45"/>
     <mergeCell ref="Y46:Y51"/>
     <mergeCell ref="Y52:Y58"/>
-    <mergeCell ref="Y59:Y66"/>
-    <mergeCell ref="AC52:AC58"/>
-    <mergeCell ref="AC59:AC66"/>
+    <mergeCell ref="AT92:AT94"/>
+    <mergeCell ref="AU92:AU94"/>
+    <mergeCell ref="AU95:AU97"/>
+    <mergeCell ref="AT95:AT97"/>
+    <mergeCell ref="AT98:AT100"/>
+    <mergeCell ref="AU98:AU100"/>
+    <mergeCell ref="AN98:AN100"/>
+    <mergeCell ref="AM98:AM100"/>
+    <mergeCell ref="AL98:AL100"/>
+    <mergeCell ref="AL92:AL97"/>
+    <mergeCell ref="AM92:AM94"/>
+    <mergeCell ref="AM95:AM97"/>
+    <mergeCell ref="AN92:AN94"/>
+    <mergeCell ref="AN95:AN97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{877C8987-74F6-7E41-A66F-F19286D2B850}">
+  <dimension ref="A1:L41"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="85.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" ht="18" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="88" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="90" t="s">
+        <v>327</v>
+      </c>
+      <c r="C1" s="88" t="s">
+        <v>328</v>
+      </c>
+      <c r="D1" s="88" t="s">
+        <v>276</v>
+      </c>
+      <c r="E1" s="91" t="s">
+        <v>277</v>
+      </c>
+      <c r="F1" s="92" t="s">
+        <v>281</v>
+      </c>
+      <c r="G1" s="92" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" s="88" t="s">
+        <v>330</v>
+      </c>
+      <c r="I1" s="88" t="s">
+        <v>334</v>
+      </c>
+      <c r="J1" s="92" t="s">
+        <v>283</v>
+      </c>
+      <c r="K1" s="92" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="93" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="89" t="s">
+        <v>331</v>
+      </c>
+      <c r="C2" t="s">
+        <v>338</v>
+      </c>
+      <c r="D2" t="s">
+        <v>333</v>
+      </c>
+      <c r="E2">
+        <v>0.50477000000000005</v>
+      </c>
+      <c r="F2">
+        <v>8.8419999999999999E-2</v>
+      </c>
+      <c r="G2" s="99">
+        <v>0.35199999999999998</v>
+      </c>
+      <c r="H2" s="94">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="I2" s="94">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="J2">
+        <v>4.6899999999999997E-2</v>
+      </c>
+      <c r="K2" s="99" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="93"/>
+      <c r="B3" s="89"/>
+      <c r="D3" t="s">
+        <v>332</v>
+      </c>
+      <c r="E3">
+        <v>0.25013999999999997</v>
+      </c>
+      <c r="F3">
+        <v>0.123</v>
+      </c>
+      <c r="G3" s="94"/>
+      <c r="H3" s="94"/>
+      <c r="I3" s="94"/>
+      <c r="J3" s="87">
+        <v>4.66E-8</v>
+      </c>
+      <c r="K3" s="94"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A4" s="93"/>
+      <c r="B4" s="89" t="s">
+        <v>336</v>
+      </c>
+      <c r="C4" s="94" t="s">
+        <v>338</v>
+      </c>
+      <c r="D4" s="94" t="s">
+        <v>335</v>
+      </c>
+      <c r="E4">
+        <v>0.50731999999999999</v>
+      </c>
+      <c r="F4">
+        <v>8.8739999999999999E-2</v>
+      </c>
+      <c r="G4" s="94">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="H4" s="94">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="I4" s="94">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="J4" s="98">
+        <v>4.5300000000000002E-8</v>
+      </c>
+      <c r="K4" s="94" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A5" s="93"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="94"/>
+      <c r="D5" s="94"/>
+      <c r="G5" s="94"/>
+      <c r="H5" s="94"/>
+      <c r="I5" s="94"/>
+      <c r="J5" s="98"/>
+      <c r="K5" s="94"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A6" s="93"/>
+      <c r="B6" s="96" t="s">
+        <v>337</v>
+      </c>
+      <c r="C6" s="97" t="s">
+        <v>338</v>
+      </c>
+      <c r="D6" s="97" t="s">
+        <v>335</v>
+      </c>
+      <c r="E6" s="97">
+        <v>0.88880000000000003</v>
+      </c>
+      <c r="F6" s="97">
+        <v>0.22620000000000001</v>
+      </c>
+      <c r="G6" s="100">
+        <v>0.24199999999999999</v>
+      </c>
+      <c r="H6" s="97">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="I6" s="97">
+        <v>1.4279999999999999</v>
+      </c>
+      <c r="J6" s="97">
+        <v>1.193E-4</v>
+      </c>
+      <c r="K6" s="97" t="s">
+        <v>262</v>
+      </c>
+      <c r="L6" s="95" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A7" s="93"/>
+      <c r="B7" s="96"/>
+      <c r="C7" s="97"/>
+      <c r="D7" s="97"/>
+      <c r="E7" s="97"/>
+      <c r="F7" s="97"/>
+      <c r="G7" s="100"/>
+      <c r="H7" s="97"/>
+      <c r="I7" s="97"/>
+      <c r="J7" s="97"/>
+      <c r="K7" s="97"/>
+      <c r="L7" s="95"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A8" s="93"/>
+      <c r="B8" s="96" t="s">
+        <v>339</v>
+      </c>
+      <c r="C8" s="97" t="s">
+        <v>338</v>
+      </c>
+      <c r="D8" s="97" t="s">
+        <v>333</v>
+      </c>
+      <c r="E8" s="97">
+        <v>0.87319999999999998</v>
+      </c>
+      <c r="F8" s="97">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="G8" s="100">
+        <v>0.245</v>
+      </c>
+      <c r="H8" s="97">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="I8" s="97">
+        <v>1.4379999999999999</v>
+      </c>
+      <c r="J8" s="97">
+        <v>2.32E-4</v>
+      </c>
+      <c r="K8" s="97" t="s">
+        <v>262</v>
+      </c>
+      <c r="L8" s="95"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A9" s="93"/>
+      <c r="B9" s="96"/>
+      <c r="C9" s="97"/>
+      <c r="D9" s="97"/>
+      <c r="E9" s="97"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="100"/>
+      <c r="H9" s="97"/>
+      <c r="I9" s="97"/>
+      <c r="J9" s="97"/>
+      <c r="K9" s="97"/>
+      <c r="L9" s="95"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A10" s="93"/>
+      <c r="B10" s="96" t="s">
+        <v>340</v>
+      </c>
+      <c r="C10" s="97" t="s">
+        <v>338</v>
+      </c>
+      <c r="D10" s="97" t="s">
+        <v>333</v>
+      </c>
+      <c r="E10" s="97">
+        <v>0.87319999999999998</v>
+      </c>
+      <c r="F10" s="97">
+        <v>0.23230000000000001</v>
+      </c>
+      <c r="G10" s="100">
+        <v>0.245</v>
+      </c>
+      <c r="H10" s="97">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="I10" s="97">
+        <v>1.4379999999999999</v>
+      </c>
+      <c r="J10" s="97">
+        <v>2.32E-4</v>
+      </c>
+      <c r="K10" s="97"/>
+      <c r="L10" s="95"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A11" s="93"/>
+      <c r="B11" s="96"/>
+      <c r="C11" s="97"/>
+      <c r="D11" s="97"/>
+      <c r="E11" s="97"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="100"/>
+      <c r="H11" s="97"/>
+      <c r="I11" s="97"/>
+      <c r="J11" s="97"/>
+      <c r="K11" s="97"/>
+      <c r="L11" s="95"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A12" s="93" t="s">
+        <v>21</v>
+      </c>
+      <c r="B12" s="89" t="s">
+        <v>331</v>
+      </c>
+      <c r="C12" t="s">
+        <v>341</v>
+      </c>
+      <c r="D12" t="s">
+        <v>333</v>
+      </c>
+      <c r="E12">
+        <v>0.68569999999999998</v>
+      </c>
+      <c r="F12">
+        <v>0.2172</v>
+      </c>
+      <c r="G12" s="94">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="H12">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="I12">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="J12">
+        <v>2.6700000000000001E-3</v>
+      </c>
+      <c r="K12" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A13" s="93"/>
+      <c r="B13" s="89"/>
+      <c r="G13" s="94"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A14" s="93"/>
+      <c r="B14" s="89" t="s">
+        <v>336</v>
+      </c>
+      <c r="C14" s="94" t="s">
+        <v>342</v>
+      </c>
+      <c r="D14" s="94"/>
+      <c r="E14" s="94"/>
+      <c r="F14" s="94"/>
+      <c r="G14" s="94"/>
+      <c r="H14" s="94"/>
+      <c r="I14" s="94"/>
+      <c r="J14" s="94"/>
+      <c r="K14" s="94"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A15" s="93"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="94"/>
+      <c r="D15" s="94"/>
+      <c r="E15" s="94"/>
+      <c r="F15" s="94"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="94"/>
+      <c r="I15" s="94"/>
+      <c r="J15" s="94"/>
+      <c r="K15" s="94"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A16" s="93"/>
+      <c r="B16" s="89" t="s">
+        <v>337</v>
+      </c>
+      <c r="C16" t="s">
+        <v>341</v>
+      </c>
+      <c r="E16">
+        <v>0.68569999999999998</v>
+      </c>
+      <c r="F16">
+        <v>0.2172</v>
+      </c>
+      <c r="G16" s="94">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="H16" s="94">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="I16" s="94">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="J16">
+        <v>2.6700000000000001E-3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A17" s="93"/>
+      <c r="B17" s="89"/>
+      <c r="G17" s="94"/>
+      <c r="H17" s="94"/>
+      <c r="I17" s="94"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A18" s="93"/>
+      <c r="B18" s="89" t="s">
+        <v>339</v>
+      </c>
+      <c r="C18" s="94" t="s">
+        <v>342</v>
+      </c>
+      <c r="D18" s="94"/>
+      <c r="E18" s="94"/>
+      <c r="F18" s="94"/>
+      <c r="G18" s="94"/>
+      <c r="H18" s="94"/>
+      <c r="I18" s="94"/>
+      <c r="J18" s="94"/>
+      <c r="K18" s="94"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A19" s="93"/>
+      <c r="B19" s="89"/>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="94"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A20" s="93"/>
+      <c r="B20" s="89" t="s">
+        <v>340</v>
+      </c>
+      <c r="C20" t="s">
+        <v>341</v>
+      </c>
+      <c r="D20" t="s">
+        <v>335</v>
+      </c>
+      <c r="E20">
+        <v>0.68569999999999998</v>
+      </c>
+      <c r="F20">
+        <v>0.2172</v>
+      </c>
+      <c r="G20">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="H20">
+        <v>0.14699999999999999</v>
+      </c>
+      <c r="I20">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="K20" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A21" s="93"/>
+      <c r="B21" s="89"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A22" s="93" t="s">
+        <v>343</v>
+      </c>
+      <c r="B22" s="89" t="s">
+        <v>331</v>
+      </c>
+      <c r="C22" s="94" t="s">
+        <v>342</v>
+      </c>
+      <c r="D22" s="94"/>
+      <c r="E22" s="94"/>
+      <c r="F22" s="94"/>
+      <c r="G22" s="94"/>
+      <c r="H22" s="94"/>
+      <c r="I22" s="94"/>
+      <c r="J22" s="94"/>
+      <c r="K22" s="94"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A23" s="93"/>
+      <c r="B23" s="89"/>
+      <c r="C23" s="94"/>
+      <c r="D23" s="94"/>
+      <c r="E23" s="94"/>
+      <c r="F23" s="94"/>
+      <c r="G23" s="94"/>
+      <c r="H23" s="94"/>
+      <c r="I23" s="94"/>
+      <c r="J23" s="94"/>
+      <c r="K23" s="94"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A24" s="93"/>
+      <c r="B24" s="89" t="s">
+        <v>336</v>
+      </c>
+      <c r="C24" s="94"/>
+      <c r="D24" s="94"/>
+      <c r="E24" s="94"/>
+      <c r="F24" s="94"/>
+      <c r="G24" s="94"/>
+      <c r="H24" s="94"/>
+      <c r="I24" s="94"/>
+      <c r="J24" s="94"/>
+      <c r="K24" s="94"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A25" s="93"/>
+      <c r="B25" s="89"/>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A26" s="93"/>
+      <c r="B26" s="89" t="s">
+        <v>337</v>
+      </c>
+      <c r="C26" t="s">
+        <v>341</v>
+      </c>
+      <c r="D26" t="s">
+        <v>335</v>
+      </c>
+      <c r="E26">
+        <v>0.65056000000000003</v>
+      </c>
+      <c r="F26">
+        <v>0.23355000000000001</v>
+      </c>
+      <c r="G26">
+        <v>0.153</v>
+      </c>
+      <c r="H26">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="I26">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="J26">
+        <v>7.92E-3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A27" s="93"/>
+      <c r="B27" s="89"/>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A28" s="93"/>
+      <c r="B28" s="89" t="s">
+        <v>339</v>
+      </c>
+      <c r="C28" s="94" t="s">
+        <v>342</v>
+      </c>
+      <c r="D28" s="94"/>
+      <c r="E28" s="94"/>
+      <c r="F28" s="94"/>
+      <c r="G28" s="94"/>
+      <c r="H28" s="94"/>
+      <c r="I28" s="94"/>
+      <c r="J28" s="94"/>
+      <c r="K28" s="94"/>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A29" s="93"/>
+      <c r="B29" s="89"/>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A30" s="93"/>
+      <c r="B30" s="89" t="s">
+        <v>340</v>
+      </c>
+      <c r="C30" t="s">
+        <v>341</v>
+      </c>
+      <c r="D30" t="s">
+        <v>335</v>
+      </c>
+      <c r="E30">
+        <v>0.69269999999999998</v>
+      </c>
+      <c r="F30">
+        <v>0.27929999999999999</v>
+      </c>
+      <c r="G30">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="H30">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="I30">
+        <v>0.82699999999999996</v>
+      </c>
+      <c r="J30">
+        <v>1.78E-2</v>
+      </c>
+      <c r="K30" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A31" s="93"/>
+      <c r="B31" s="89"/>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A32" s="93" t="s">
+        <v>344</v>
+      </c>
+      <c r="B32" s="89" t="s">
+        <v>331</v>
+      </c>
+      <c r="C32" t="s">
+        <v>338</v>
+      </c>
+      <c r="D32" t="s">
+        <v>335</v>
+      </c>
+      <c r="E32">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="F32">
+        <v>0.1234</v>
+      </c>
+      <c r="G32" s="94">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H32" s="94">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="I32" s="94">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="J32" s="87">
+        <v>6.9200000000000001E-9</v>
+      </c>
+      <c r="K32" s="94" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A33" s="93"/>
+      <c r="B33" s="89"/>
+      <c r="D33" t="s">
+        <v>345</v>
+      </c>
+      <c r="E33">
+        <v>-0.45540000000000003</v>
+      </c>
+      <c r="F33">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G33" s="94"/>
+      <c r="H33" s="94"/>
+      <c r="I33" s="94"/>
+      <c r="J33">
+        <v>2.3400000000000001E-3</v>
+      </c>
+      <c r="K33" s="94"/>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A34" s="93"/>
+      <c r="B34" s="89" t="s">
+        <v>336</v>
+      </c>
+      <c r="C34" t="s">
+        <v>338</v>
+      </c>
+      <c r="D34" t="s">
+        <v>335</v>
+      </c>
+      <c r="E34">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="F34">
+        <v>0.1234</v>
+      </c>
+      <c r="G34" s="94">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H34" s="94">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="I34" s="94">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="J34" s="87">
+        <v>6.9210000000000004E-9</v>
+      </c>
+      <c r="K34" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A35" s="93"/>
+      <c r="B35" s="89"/>
+      <c r="D35" t="s">
+        <v>345</v>
+      </c>
+      <c r="E35">
+        <v>-0.45540000000000003</v>
+      </c>
+      <c r="F35">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G35" s="94"/>
+      <c r="H35" s="94"/>
+      <c r="I35" s="94"/>
+      <c r="J35">
+        <v>2.3410000000000002E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A36" s="93"/>
+      <c r="B36" s="89" t="s">
+        <v>337</v>
+      </c>
+      <c r="C36" t="s">
+        <v>338</v>
+      </c>
+      <c r="D36" t="s">
+        <v>335</v>
+      </c>
+      <c r="E36">
+        <v>0.74550000000000005</v>
+      </c>
+      <c r="F36">
+        <v>0.12</v>
+      </c>
+      <c r="G36" s="94">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="H36" s="94">
+        <v>0.245</v>
+      </c>
+      <c r="I36" s="94">
+        <v>0.56999999999999995</v>
+      </c>
+      <c r="J36" s="87">
+        <v>1.2E-8</v>
+      </c>
+      <c r="K36" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A37" s="93"/>
+      <c r="B37" s="89"/>
+      <c r="D37" t="s">
+        <v>345</v>
+      </c>
+      <c r="E37">
+        <v>-0.3422</v>
+      </c>
+      <c r="F37">
+        <v>0.1298</v>
+      </c>
+      <c r="G37" s="94"/>
+      <c r="H37" s="94"/>
+      <c r="I37" s="94"/>
+      <c r="J37">
+        <v>1.38E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A38" s="93"/>
+      <c r="B38" s="89" t="s">
+        <v>339</v>
+      </c>
+      <c r="C38" t="s">
+        <v>338</v>
+      </c>
+      <c r="D38" t="s">
+        <v>335</v>
+      </c>
+      <c r="E38">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="F38">
+        <v>0.1234</v>
+      </c>
+      <c r="G38" s="94">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H38" s="94">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="I38" s="94">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="J38" s="87">
+        <v>6.9200000000000001E-9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A39" s="93"/>
+      <c r="B39" s="89"/>
+      <c r="D39" t="s">
+        <v>345</v>
+      </c>
+      <c r="E39">
+        <v>-0.45540000000000003</v>
+      </c>
+      <c r="F39">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G39" s="94"/>
+      <c r="H39" s="94"/>
+      <c r="I39" s="94"/>
+      <c r="J39">
+        <v>2.3400000000000001E-3</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A40" s="93"/>
+      <c r="B40" s="89" t="s">
+        <v>340</v>
+      </c>
+      <c r="C40" t="s">
+        <v>338</v>
+      </c>
+      <c r="D40" t="s">
+        <v>335</v>
+      </c>
+      <c r="E40">
+        <v>0.79139999999999999</v>
+      </c>
+      <c r="F40">
+        <v>0.1234</v>
+      </c>
+      <c r="G40" s="94">
+        <v>0.61499999999999999</v>
+      </c>
+      <c r="H40" s="94">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="I40" s="94">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="J40" s="87">
+        <v>6.9200000000000001E-9</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="D41" t="s">
+        <v>345</v>
+      </c>
+      <c r="E41">
+        <v>-0.45540000000000003</v>
+      </c>
+      <c r="F41">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G41" s="94"/>
+      <c r="H41" s="94"/>
+      <c r="I41" s="94"/>
+      <c r="J41">
+        <v>2.3400000000000001E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="L6:L11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CF5BA507-4B43-AC4E-B08A-3A1E127153A8}">
+  <dimension ref="A1:J10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K18" sqref="K18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
+        <v>328</v>
+      </c>
+      <c r="C1" t="s">
+        <v>276</v>
+      </c>
+      <c r="D1" t="s">
+        <v>277</v>
+      </c>
+      <c r="E1" t="s">
+        <v>281</v>
+      </c>
+      <c r="F1" t="s">
+        <v>329</v>
+      </c>
+      <c r="G1" s="101" t="s">
+        <v>330</v>
+      </c>
+      <c r="H1" s="101" t="s">
+        <v>334</v>
+      </c>
+      <c r="I1" s="102" t="s">
+        <v>283</v>
+      </c>
+      <c r="J1" s="102" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
+        <v>338</v>
+      </c>
+      <c r="C2" t="s">
+        <v>333</v>
+      </c>
+      <c r="D2">
+        <v>0.43160999999999999</v>
+      </c>
+      <c r="E2">
+        <v>8.9249999999999996E-2</v>
+      </c>
+      <c r="F2">
+        <v>0.433</v>
+      </c>
+      <c r="G2">
+        <v>0.16400000000000001</v>
+      </c>
+      <c r="H2">
+        <v>0.48299999999999998</v>
+      </c>
+      <c r="I2" s="87">
+        <v>2.4399999999999999E-6</v>
+      </c>
+      <c r="J2" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="88"/>
+      <c r="C3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D3">
+        <v>0.26634000000000002</v>
+      </c>
+      <c r="E3">
+        <v>5.5309999999999998E-2</v>
+      </c>
+      <c r="I3" s="87">
+        <v>2.52E-6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="88" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" t="s">
+        <v>333</v>
+      </c>
+      <c r="D4">
+        <v>0.63912000000000002</v>
+      </c>
+      <c r="E4">
+        <v>0.23122999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="G4">
+        <v>0.124</v>
+      </c>
+      <c r="H4">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="I4">
+        <v>8.1899999999999994E-3</v>
+      </c>
+      <c r="J4" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="88"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="88" t="s">
+        <v>343</v>
+      </c>
+      <c r="B6" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" t="s">
+        <v>333</v>
+      </c>
+      <c r="D6">
+        <v>1.06124</v>
+      </c>
+      <c r="E6">
+        <v>0.19517000000000001</v>
+      </c>
+      <c r="F6">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="G6">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="H6">
+        <v>0.71499999999999997</v>
+      </c>
+      <c r="I6" s="87">
+        <v>6.1500000000000004E-7</v>
+      </c>
+      <c r="J6" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="88"/>
+      <c r="C7" t="s">
+        <v>348</v>
+      </c>
+      <c r="D7">
+        <v>-0.38041000000000003</v>
+      </c>
+      <c r="E7">
+        <v>8.6220000000000005E-2</v>
+      </c>
+      <c r="I7" s="87">
+        <v>3.2799999999999998E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="88" t="s">
+        <v>344</v>
+      </c>
+      <c r="B8" t="s">
+        <v>338</v>
+      </c>
+      <c r="C8" t="s">
+        <v>333</v>
+      </c>
+      <c r="D8">
+        <v>0.73280000000000001</v>
+      </c>
+      <c r="E8">
+        <v>0.13619999999999999</v>
+      </c>
+      <c r="F8">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="G8">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="H8">
+        <v>0.58199999999999996</v>
+      </c>
+      <c r="I8" s="87">
+        <v>5.7199999999999999E-7</v>
+      </c>
+      <c r="J8" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="88"/>
+      <c r="C9" t="s">
+        <v>348</v>
+      </c>
+      <c r="D9">
+        <v>-0.33360000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.13020000000000001</v>
+      </c>
+      <c r="I9">
+        <v>1.6400000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="88"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B92E129-2BB0-994E-845F-07E029B53A76}">
   <dimension ref="A1:P25"/>
   <sheetViews>
@@ -3253,35 +4731,35 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A1" s="68" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="67" t="s">
+      <c r="A1" s="83" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="82" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="65"/>
-      <c r="D1" s="66"/>
-      <c r="E1" s="65" t="s">
+      <c r="C1" s="80"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="65"/>
-      <c r="G1" s="65"/>
-      <c r="H1" s="66"/>
-      <c r="I1" s="67" t="s">
+      <c r="F1" s="80"/>
+      <c r="G1" s="80"/>
+      <c r="H1" s="81"/>
+      <c r="I1" s="82" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="65"/>
-      <c r="K1" s="65"/>
-      <c r="L1" s="66"/>
-      <c r="M1" s="67" t="s">
+      <c r="J1" s="80"/>
+      <c r="K1" s="80"/>
+      <c r="L1" s="81"/>
+      <c r="M1" s="82" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="65"/>
-      <c r="O1" s="65"/>
-      <c r="P1" s="66"/>
+      <c r="N1" s="80"/>
+      <c r="O1" s="80"/>
+      <c r="P1" s="81"/>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="A2" s="69"/>
+      <c r="A2" s="84"/>
       <c r="B2" s="5" t="s">
         <v>30</v>
       </c>
@@ -3935,19 +5413,19 @@
       <c r="B15" s="3">
         <v>6.88750127946237E-2</v>
       </c>
-      <c r="C15" s="78">
+      <c r="C15" s="1">
         <v>0</v>
       </c>
       <c r="D15" s="4">
         <v>0</v>
       </c>
-      <c r="E15" s="86">
+      <c r="E15" s="22">
         <v>0.34445449610162798</v>
       </c>
-      <c r="F15" s="78">
-        <v>0</v>
-      </c>
-      <c r="G15" s="78">
+      <c r="F15" s="1">
+        <v>0</v>
+      </c>
+      <c r="G15" s="1">
         <v>0</v>
       </c>
       <c r="H15" s="4">
@@ -3956,10 +5434,10 @@
       <c r="I15" s="7">
         <v>-6.5705100000000002E-2</v>
       </c>
-      <c r="J15" s="85">
-        <v>0</v>
-      </c>
-      <c r="K15" s="85">
+      <c r="J15" s="8">
+        <v>0</v>
+      </c>
+      <c r="K15" s="8">
         <v>0</v>
       </c>
       <c r="L15" s="9">
@@ -3968,10 +5446,10 @@
       <c r="M15" s="7">
         <v>-9.7653299999999998E-2</v>
       </c>
-      <c r="N15" s="85">
-        <v>0</v>
-      </c>
-      <c r="O15" s="85">
+      <c r="N15" s="8">
+        <v>0</v>
+      </c>
+      <c r="O15" s="8">
         <v>0</v>
       </c>
       <c r="P15" s="9">
@@ -4085,19 +5563,19 @@
       <c r="B18" s="3">
         <v>0</v>
       </c>
-      <c r="C18" s="78">
+      <c r="C18" s="1">
         <v>0.86459871719232595</v>
       </c>
       <c r="D18" s="4">
         <v>0</v>
       </c>
-      <c r="E18" s="78">
+      <c r="E18" s="1">
         <v>4.2584655578084003E-2</v>
       </c>
-      <c r="F18" s="78">
-        <v>0</v>
-      </c>
-      <c r="G18" s="78">
+      <c r="F18" s="1">
+        <v>0</v>
+      </c>
+      <c r="G18" s="1">
         <v>0</v>
       </c>
       <c r="H18" s="4">
@@ -4106,10 +5584,10 @@
       <c r="I18" s="7">
         <v>-1.3967000000000001E-3</v>
       </c>
-      <c r="J18" s="85">
-        <v>0</v>
-      </c>
-      <c r="K18" s="85">
+      <c r="J18" s="8">
+        <v>0</v>
+      </c>
+      <c r="K18" s="8">
         <v>1</v>
       </c>
       <c r="L18" s="9">
@@ -4118,10 +5596,10 @@
       <c r="M18" s="24">
         <v>-0.30111870000000002</v>
       </c>
-      <c r="N18" s="85">
+      <c r="N18" s="8">
         <v>-0.7172444</v>
       </c>
-      <c r="O18" s="85">
+      <c r="O18" s="8">
         <v>0</v>
       </c>
       <c r="P18" s="9">
@@ -4135,19 +5613,19 @@
       <c r="B19" s="21">
         <v>0.38345987651346702</v>
       </c>
-      <c r="C19" s="78">
+      <c r="C19" s="1">
         <v>0</v>
       </c>
       <c r="D19" s="4">
         <v>0</v>
       </c>
-      <c r="E19" s="86">
+      <c r="E19" s="22">
         <v>0.228119921464676</v>
       </c>
-      <c r="F19" s="78">
+      <c r="F19" s="1">
         <v>-3.5890256591688999E-2</v>
       </c>
-      <c r="G19" s="78">
+      <c r="G19" s="1">
         <v>0</v>
       </c>
       <c r="H19" s="4">
@@ -4156,10 +5634,10 @@
       <c r="I19" s="7">
         <v>0</v>
       </c>
-      <c r="J19" s="85">
-        <v>0</v>
-      </c>
-      <c r="K19" s="85">
+      <c r="J19" s="8">
+        <v>0</v>
+      </c>
+      <c r="K19" s="8">
         <v>0</v>
       </c>
       <c r="L19" s="9">
@@ -4168,10 +5646,10 @@
       <c r="M19" s="7">
         <v>-0.1587258</v>
       </c>
-      <c r="N19" s="85">
+      <c r="N19" s="8">
         <v>0.45095255000000001</v>
       </c>
-      <c r="O19" s="85">
+      <c r="O19" s="8">
         <v>0</v>
       </c>
       <c r="P19" s="9">
@@ -4420,12 +5898,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E119337B-178C-1641-8548-9AE40C5AB899}">
   <dimension ref="B2:T88"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G61" workbookViewId="0">
-      <selection activeCell="P71" sqref="P71"/>
+    <sheetView topLeftCell="G28" workbookViewId="0">
+      <selection activeCell="O31" sqref="O31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4441,15 +5919,15 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="73" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="63"/>
-      <c r="D2" s="63"/>
-      <c r="E2" s="63"/>
-      <c r="F2" s="63"/>
-      <c r="G2" s="63"/>
-      <c r="H2" s="91"/>
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B3" s="13" t="s">
@@ -4470,10 +5948,9 @@
       <c r="G3" s="13" t="s">
         <v>74</v>
       </c>
-      <c r="H3" s="78"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="63" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="40" t="s">
@@ -4485,10 +5962,9 @@
       <c r="E4" s="40"/>
       <c r="F4" s="40"/>
       <c r="G4" s="40"/>
-      <c r="H4" s="78"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="60"/>
+      <c r="B5" s="64"/>
       <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
@@ -4497,7 +5973,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="60"/>
+      <c r="B6" s="64"/>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
@@ -4506,7 +5982,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="60"/>
+      <c r="B7" s="64"/>
       <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
@@ -4515,7 +5991,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="61"/>
+      <c r="B8" s="65"/>
       <c r="C8" s="13" t="s">
         <v>42</v>
       </c>
@@ -4525,10 +6001,9 @@
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
       <c r="G8" s="13"/>
-      <c r="H8" s="78"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="63" t="s">
         <v>80</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -4540,10 +6015,9 @@
       <c r="E9" s="40"/>
       <c r="F9" s="40"/>
       <c r="G9" s="40"/>
-      <c r="H9" s="78"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="60"/>
+      <c r="B10" s="64"/>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
@@ -4555,7 +6029,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="60"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
@@ -4567,7 +6041,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="60"/>
+      <c r="B12" s="64"/>
       <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
@@ -4576,7 +6050,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="61"/>
+      <c r="B13" s="65"/>
       <c r="C13" s="13" t="s">
         <v>42</v>
       </c>
@@ -4586,10 +6060,9 @@
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="78"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="59" t="s">
+      <c r="B14" s="63" t="s">
         <v>81</v>
       </c>
       <c r="C14" s="41" t="s">
@@ -4603,10 +6076,9 @@
       </c>
       <c r="F14" s="40"/>
       <c r="G14" s="40"/>
-      <c r="H14" s="78"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="60"/>
+      <c r="B15" s="64"/>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
@@ -4618,7 +6090,7 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="60"/>
+      <c r="B16" s="64"/>
       <c r="C16" s="1" t="s">
         <v>37</v>
       </c>
@@ -4633,7 +6105,7 @@
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B17" s="60"/>
+      <c r="B17" s="64"/>
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
@@ -4645,7 +6117,7 @@
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B18" s="61"/>
+      <c r="B18" s="65"/>
       <c r="C18" s="13" t="s">
         <v>13</v>
       </c>
@@ -4657,10 +6129,9 @@
       </c>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="78"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B19" s="60" t="s">
+      <c r="B19" s="64" t="s">
         <v>82</v>
       </c>
       <c r="C19" s="39" t="s">
@@ -4671,7 +6142,7 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B20" s="60"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
@@ -4680,7 +6151,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B21" s="60"/>
+      <c r="B21" s="64"/>
       <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
@@ -4689,7 +6160,7 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="60"/>
+      <c r="B22" s="64"/>
       <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
@@ -4698,7 +6169,7 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B23" s="61"/>
+      <c r="B23" s="65"/>
       <c r="C23" s="13" t="s">
         <v>15</v>
       </c>
@@ -4708,62 +6179,61 @@
       </c>
       <c r="F23" s="13"/>
       <c r="G23" s="13"/>
-      <c r="H23" s="78"/>
     </row>
     <row r="30" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J30" s="63" t="s">
+      <c r="J30" s="73" t="s">
         <v>274</v>
       </c>
-      <c r="K30" s="63"/>
-      <c r="L30" s="63"/>
-      <c r="M30" s="63"/>
-      <c r="N30" s="63"/>
-      <c r="O30" s="63"/>
-      <c r="P30" s="63"/>
-      <c r="Q30" s="63"/>
-      <c r="R30" s="63"/>
-      <c r="S30" s="63"/>
+      <c r="K30" s="73"/>
+      <c r="L30" s="73"/>
+      <c r="M30" s="73"/>
+      <c r="N30" s="73"/>
+      <c r="O30" s="73"/>
+      <c r="P30" s="73"/>
+      <c r="Q30" s="73"/>
+      <c r="R30" s="73"/>
+      <c r="S30" s="73"/>
     </row>
     <row r="31" spans="2:20" ht="18" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="J31" s="70" t="s">
+      <c r="J31" s="55" t="s">
         <v>53</v>
       </c>
-      <c r="K31" s="70" t="s">
+      <c r="K31" s="55" t="s">
         <v>275</v>
       </c>
-      <c r="L31" s="70" t="s">
+      <c r="L31" s="55" t="s">
         <v>307</v>
       </c>
-      <c r="M31" s="70" t="s">
+      <c r="M31" s="55" t="s">
         <v>276</v>
       </c>
-      <c r="N31" s="71" t="s">
+      <c r="N31" s="56" t="s">
         <v>277</v>
       </c>
-      <c r="O31" s="70" t="s">
+      <c r="O31" s="55" t="s">
         <v>281</v>
       </c>
-      <c r="P31" s="70" t="s">
+      <c r="P31" s="55" t="s">
         <v>282</v>
       </c>
-      <c r="Q31" s="70" t="s">
+      <c r="Q31" s="55" t="s">
         <v>283</v>
       </c>
-      <c r="R31" s="70" t="s">
+      <c r="R31" s="55" t="s">
         <v>285</v>
       </c>
-      <c r="S31" s="70" t="s">
+      <c r="S31" s="55" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J32" s="89" t="s">
+      <c r="J32" s="85" t="s">
         <v>79</v>
       </c>
       <c r="K32" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="M32" s="87" t="s">
+      <c r="M32" s="61" t="s">
         <v>273</v>
       </c>
       <c r="T32" s="1" t="s">
@@ -4771,16 +6241,16 @@
       </c>
     </row>
     <row r="33" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J33" s="90"/>
+      <c r="J33" s="86"/>
       <c r="K33" s="14" t="s">
         <v>16</v>
       </c>
-      <c r="M33" s="87" t="s">
+      <c r="M33" s="61" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="34" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J34" s="90"/>
+      <c r="J34" s="86"/>
       <c r="K34" s="14" t="s">
         <v>17</v>
       </c>
@@ -4789,7 +6259,7 @@
       </c>
     </row>
     <row r="35" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J35" s="90"/>
+      <c r="J35" s="86"/>
       <c r="K35" s="14" t="s">
         <v>34</v>
       </c>
@@ -4798,16 +6268,16 @@
       </c>
     </row>
     <row r="36" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J36" s="90"/>
+      <c r="J36" s="86"/>
       <c r="K36" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="M36" s="87" t="s">
+      <c r="M36" s="61" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="37" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J37" s="90"/>
+      <c r="J37" s="86"/>
       <c r="K37" s="14" t="s">
         <v>18</v>
       </c>
@@ -4819,7 +6289,7 @@
       </c>
     </row>
     <row r="38" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J38" s="90"/>
+      <c r="J38" s="86"/>
       <c r="K38" s="14" t="s">
         <v>37</v>
       </c>
@@ -4828,20 +6298,20 @@
       </c>
     </row>
     <row r="39" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J39" s="90"/>
+      <c r="J39" s="86"/>
       <c r="K39" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="M39" s="87" t="s">
+      <c r="M39" s="61" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="40" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J40" s="90"/>
+      <c r="J40" s="86"/>
       <c r="K40" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M40" s="87" t="s">
+      <c r="M40" s="61" t="s">
         <v>273</v>
       </c>
       <c r="T40" s="1" t="s">
@@ -4849,11 +6319,11 @@
       </c>
     </row>
     <row r="41" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J41" s="90"/>
+      <c r="J41" s="86"/>
       <c r="K41" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M41" s="87" t="s">
+      <c r="M41" s="61" t="s">
         <v>273</v>
       </c>
       <c r="T41" s="1" t="s">
@@ -4861,7 +6331,7 @@
       </c>
     </row>
     <row r="42" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="90"/>
+      <c r="J42" s="86"/>
       <c r="K42" s="14" t="s">
         <v>13</v>
       </c>
@@ -4873,7 +6343,7 @@
       </c>
     </row>
     <row r="43" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J43" s="90"/>
+      <c r="J43" s="86"/>
       <c r="K43" s="14" t="s">
         <v>14</v>
       </c>
@@ -4882,7 +6352,7 @@
       </c>
     </row>
     <row r="44" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J44" s="90"/>
+      <c r="J44" s="86"/>
       <c r="K44" s="14" t="s">
         <v>38</v>
       </c>
@@ -4891,7 +6361,7 @@
       </c>
     </row>
     <row r="45" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J45" s="90"/>
+      <c r="J45" s="86"/>
       <c r="K45" s="14" t="s">
         <v>20</v>
       </c>
@@ -4903,20 +6373,20 @@
       </c>
     </row>
     <row r="46" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J46" s="90"/>
+      <c r="J46" s="86"/>
       <c r="K46" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M46" s="87" t="s">
+      <c r="M46" s="61" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="47" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J47" s="90"/>
+      <c r="J47" s="86"/>
       <c r="K47" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="L47" s="88" t="s">
+      <c r="L47" s="62" t="s">
         <v>305</v>
       </c>
       <c r="M47" s="1" t="s">
@@ -4924,16 +6394,16 @@
       </c>
     </row>
     <row r="48" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J48" s="90"/>
+      <c r="J48" s="86"/>
       <c r="K48" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="M48" s="87" t="s">
+      <c r="M48" s="61" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="49" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J49" s="90"/>
+      <c r="J49" s="86"/>
       <c r="K49" s="14" t="s">
         <v>42</v>
       </c>
@@ -4942,27 +6412,27 @@
       </c>
     </row>
     <row r="50" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J50" s="90"/>
+      <c r="J50" s="86"/>
       <c r="K50" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="M50" s="87" t="s">
+      <c r="M50" s="61" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="51" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J51" s="89" t="s">
+      <c r="J51" s="85" t="s">
         <v>80</v>
       </c>
       <c r="K51" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="M51" s="87" t="s">
+      <c r="M51" s="61" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="52" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J52" s="90"/>
+      <c r="J52" s="86"/>
       <c r="K52" s="14" t="s">
         <v>16</v>
       </c>
@@ -4971,7 +6441,7 @@
       </c>
     </row>
     <row r="53" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J53" s="90"/>
+      <c r="J53" s="86"/>
       <c r="K53" s="14" t="s">
         <v>17</v>
       </c>
@@ -4980,7 +6450,7 @@
       </c>
     </row>
     <row r="54" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J54" s="90"/>
+      <c r="J54" s="86"/>
       <c r="K54" s="14" t="s">
         <v>34</v>
       </c>
@@ -4989,7 +6459,7 @@
       </c>
     </row>
     <row r="55" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J55" s="90"/>
+      <c r="J55" s="86"/>
       <c r="K55" s="14" t="s">
         <v>35</v>
       </c>
@@ -4998,7 +6468,7 @@
       </c>
     </row>
     <row r="56" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J56" s="90"/>
+      <c r="J56" s="86"/>
       <c r="K56" s="14" t="s">
         <v>18</v>
       </c>
@@ -5007,7 +6477,7 @@
       </c>
     </row>
     <row r="57" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J57" s="90"/>
+      <c r="J57" s="86"/>
       <c r="K57" s="14" t="s">
         <v>37</v>
       </c>
@@ -5019,7 +6489,7 @@
       </c>
     </row>
     <row r="58" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J58" s="90"/>
+      <c r="J58" s="86"/>
       <c r="K58" s="14" t="s">
         <v>36</v>
       </c>
@@ -5028,7 +6498,7 @@
       </c>
     </row>
     <row r="59" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J59" s="90"/>
+      <c r="J59" s="86"/>
       <c r="K59" s="14" t="s">
         <v>12</v>
       </c>
@@ -5040,16 +6510,16 @@
       </c>
     </row>
     <row r="60" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J60" s="90"/>
+      <c r="J60" s="86"/>
       <c r="K60" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="M60" s="87" t="s">
+      <c r="M60" s="61" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="61" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J61" s="90"/>
+      <c r="J61" s="86"/>
       <c r="K61" s="14" t="s">
         <v>13</v>
       </c>
@@ -5061,7 +6531,7 @@
       </c>
     </row>
     <row r="62" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J62" s="90"/>
+      <c r="J62" s="86"/>
       <c r="K62" s="14" t="s">
         <v>14</v>
       </c>
@@ -5070,7 +6540,7 @@
       </c>
     </row>
     <row r="63" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J63" s="90"/>
+      <c r="J63" s="86"/>
       <c r="K63" s="14" t="s">
         <v>38</v>
       </c>
@@ -5082,7 +6552,7 @@
       </c>
     </row>
     <row r="64" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J64" s="90"/>
+      <c r="J64" s="86"/>
       <c r="K64" s="14" t="s">
         <v>20</v>
       </c>
@@ -5094,11 +6564,11 @@
       </c>
     </row>
     <row r="65" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J65" s="90"/>
+      <c r="J65" s="86"/>
       <c r="K65" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="M65" s="87" t="s">
+      <c r="M65" s="61" t="s">
         <v>273</v>
       </c>
       <c r="T65" s="1" t="s">
@@ -5106,11 +6576,11 @@
       </c>
     </row>
     <row r="66" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J66" s="90"/>
+      <c r="J66" s="86"/>
       <c r="K66" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="M66" s="87" t="s">
+      <c r="M66" s="61" t="s">
         <v>273</v>
       </c>
       <c r="T66" s="1" t="s">
@@ -5118,7 +6588,7 @@
       </c>
     </row>
     <row r="67" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J67" s="90"/>
+      <c r="J67" s="86"/>
       <c r="K67" s="14" t="s">
         <v>41</v>
       </c>
@@ -5127,7 +6597,7 @@
       </c>
     </row>
     <row r="68" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J68" s="90"/>
+      <c r="J68" s="86"/>
       <c r="K68" s="14" t="s">
         <v>42</v>
       </c>
@@ -5139,7 +6609,7 @@
       </c>
     </row>
     <row r="69" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J69" s="90"/>
+      <c r="J69" s="86"/>
       <c r="K69" s="15" t="s">
         <v>15</v>
       </c>
@@ -5148,13 +6618,13 @@
       </c>
     </row>
     <row r="70" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J70" s="89" t="s">
+      <c r="J70" s="85" t="s">
         <v>81</v>
       </c>
       <c r="K70" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="M70" s="87" t="s">
+      <c r="M70" s="61" t="s">
         <v>273</v>
       </c>
       <c r="T70" s="1" t="s">
@@ -5162,7 +6632,7 @@
       </c>
     </row>
     <row r="71" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J71" s="90"/>
+      <c r="J71" s="86"/>
       <c r="K71" s="14" t="s">
         <v>16</v>
       </c>
@@ -5171,7 +6641,7 @@
       </c>
     </row>
     <row r="72" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J72" s="90"/>
+      <c r="J72" s="86"/>
       <c r="K72" s="14" t="s">
         <v>17</v>
       </c>
@@ -5183,7 +6653,7 @@
       </c>
     </row>
     <row r="73" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J73" s="90"/>
+      <c r="J73" s="86"/>
       <c r="K73" s="14" t="s">
         <v>34</v>
       </c>
@@ -5192,16 +6662,16 @@
       </c>
     </row>
     <row r="74" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J74" s="90"/>
+      <c r="J74" s="86"/>
       <c r="K74" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="M74" s="87" t="s">
+      <c r="M74" s="61" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="75" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J75" s="90"/>
+      <c r="J75" s="86"/>
       <c r="K75" s="14" t="s">
         <v>18</v>
       </c>
@@ -5213,7 +6683,7 @@
       </c>
     </row>
     <row r="76" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J76" s="90"/>
+      <c r="J76" s="86"/>
       <c r="K76" s="14" t="s">
         <v>37</v>
       </c>
@@ -5222,7 +6692,7 @@
       </c>
     </row>
     <row r="77" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J77" s="90"/>
+      <c r="J77" s="86"/>
       <c r="K77" s="14" t="s">
         <v>36</v>
       </c>
@@ -5234,7 +6704,7 @@
       </c>
     </row>
     <row r="78" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J78" s="90"/>
+      <c r="J78" s="86"/>
       <c r="K78" s="14" t="s">
         <v>12</v>
       </c>
@@ -5243,7 +6713,7 @@
       </c>
     </row>
     <row r="79" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J79" s="90"/>
+      <c r="J79" s="86"/>
       <c r="K79" s="14" t="s">
         <v>19</v>
       </c>
@@ -5255,7 +6725,7 @@
       </c>
     </row>
     <row r="80" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J80" s="90"/>
+      <c r="J80" s="86"/>
       <c r="K80" s="14" t="s">
         <v>13</v>
       </c>
@@ -5267,7 +6737,7 @@
       </c>
     </row>
     <row r="81" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J81" s="90"/>
+      <c r="J81" s="86"/>
       <c r="K81" s="14" t="s">
         <v>14</v>
       </c>
@@ -5279,7 +6749,7 @@
       </c>
     </row>
     <row r="82" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J82" s="90"/>
+      <c r="J82" s="86"/>
       <c r="K82" s="14" t="s">
         <v>38</v>
       </c>
@@ -5294,7 +6764,7 @@
       </c>
     </row>
     <row r="83" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J83" s="90"/>
+      <c r="J83" s="86"/>
       <c r="K83" s="14" t="s">
         <v>20</v>
       </c>
@@ -5303,7 +6773,7 @@
       </c>
     </row>
     <row r="84" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J84" s="90"/>
+      <c r="J84" s="86"/>
       <c r="K84" s="14" t="s">
         <v>33</v>
       </c>
@@ -5312,7 +6782,7 @@
       </c>
     </row>
     <row r="85" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J85" s="90"/>
+      <c r="J85" s="86"/>
       <c r="K85" s="14" t="s">
         <v>39</v>
       </c>
@@ -5321,7 +6791,7 @@
       </c>
     </row>
     <row r="86" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J86" s="90"/>
+      <c r="J86" s="86"/>
       <c r="K86" s="14" t="s">
         <v>41</v>
       </c>
@@ -5336,7 +6806,7 @@
       </c>
     </row>
     <row r="87" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J87" s="90"/>
+      <c r="J87" s="86"/>
       <c r="K87" s="14" t="s">
         <v>42</v>
       </c>
@@ -5345,7 +6815,7 @@
       </c>
     </row>
     <row r="88" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J88" s="90"/>
+      <c r="J88" s="86"/>
       <c r="K88" s="15" t="s">
         <v>15</v>
       </c>
@@ -5372,7 +6842,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C9F63A6-D668-3143-8DC9-34686F6E9D3E}">
   <dimension ref="A1:G19"/>
   <sheetViews>
@@ -5825,11 +7295,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF3FD98D-D316-FD42-8674-38FD19B76A16}">
   <dimension ref="A1:H73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A75" workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
@@ -7739,7 +9209,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5386430B-DFB3-A74D-968B-1486CE660634}">
   <dimension ref="A1:H2935"/>
   <sheetViews>
@@ -84065,7 +85535,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D694EB28-269F-0D4D-97A6-F8C5DD4D1896}">
   <dimension ref="A1:H37"/>
   <sheetViews>

</xml_diff>

<commit_message>
gift monday jan-29-2024 Made effect_plots for pli and pli_hds
</commit_message>
<xml_diff>
--- a/Figures/summaries_csvs/model_summary.xlsx
+++ b/Figures/summaries_csvs/model_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunalpalawat/Documents/GitHub/project-harvest-fork/Figures/summaries_csvs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Gift/Documents/Rprojects/project-harvest/Figures/summaries_csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{847446FD-ABC8-554C-AB18-9E513150B36A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2BAD892-502B-214D-8DCE-38607608E188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1140" yWindow="500" windowWidth="27660" windowHeight="17500" activeTab="3" xr2:uid="{BBA561B4-B8F2-A543-83D5-E4C6EA31C59C}"/>
+    <workbookView xWindow="5220" yWindow="660" windowWidth="27660" windowHeight="17500" activeTab="1" xr2:uid="{BBA561B4-B8F2-A543-83D5-E4C6EA31C59C}"/>
   </bookViews>
   <sheets>
     <sheet name="exceedances" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11689" uniqueCount="449">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11688" uniqueCount="448">
   <si>
     <t>Analyte</t>
   </si>
@@ -1338,9 +1338,6 @@
     <t>Q771</t>
   </si>
   <si>
-    <t>seasonMonsoon:Q771</t>
-  </si>
-  <si>
     <t>run effect plot</t>
   </si>
   <si>
@@ -2127,7 +2124,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="180">
+  <cellXfs count="181">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -2437,14 +2434,17 @@
     <xf numFmtId="167" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -2456,31 +2456,28 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -2491,6 +2488,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2499,12 +2502,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -2523,6 +2520,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2728,8 +2728,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{754A9160-A031-164E-8DDE-1E700AF4C60A}" name="Table2" displayName="Table2" ref="B3:N132" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
-  <autoFilter ref="B3:N132" xr:uid="{754A9160-A031-164E-8DDE-1E700AF4C60A}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{754A9160-A031-164E-8DDE-1E700AF4C60A}" name="Table2" displayName="Table2" ref="B3:N130" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14" tableBorderDxfId="13">
+  <autoFilter ref="B3:N130" xr:uid="{754A9160-A031-164E-8DDE-1E700AF4C60A}"/>
   <tableColumns count="13">
     <tableColumn id="1" xr3:uid="{A4139E18-F49A-ED4E-AC32-363B2A2EF243}" name="Column1" dataDxfId="12"/>
     <tableColumn id="2" xr3:uid="{6F5B0609-FC24-5244-8C65-143CDFC6C64F}" name="Column2" dataDxfId="11"/>
@@ -3501,27 +3501,27 @@
       </c>
     </row>
     <row r="31" spans="1:17" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="M31" s="164" t="s">
+      <c r="M31" s="152" t="s">
         <v>65</v>
       </c>
-      <c r="N31" s="164"/>
-      <c r="O31" s="164"/>
-      <c r="P31" s="164"/>
-      <c r="Q31" s="164"/>
+      <c r="N31" s="152"/>
+      <c r="O31" s="152"/>
+      <c r="P31" s="152"/>
+      <c r="Q31" s="152"/>
     </row>
     <row r="32" spans="1:17" ht="17" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="M32" s="165" t="s">
+      <c r="M32" s="153" t="s">
         <v>64</v>
       </c>
-      <c r="N32" s="163" t="s">
+      <c r="N32" s="151" t="s">
         <v>53</v>
       </c>
-      <c r="O32" s="163"/>
-      <c r="P32" s="163"/>
-      <c r="Q32" s="163"/>
+      <c r="O32" s="151"/>
+      <c r="P32" s="151"/>
+      <c r="Q32" s="151"/>
     </row>
     <row r="33" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="M33" s="159"/>
+      <c r="M33" s="154"/>
       <c r="N33" s="13" t="s">
         <v>21</v>
       </c>
@@ -3617,7 +3617,7 @@
       </c>
     </row>
     <row r="46" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="Y46" s="157" t="s">
+      <c r="Y46" s="161" t="s">
         <v>67</v>
       </c>
       <c r="Z46" s="8" t="s">
@@ -3631,7 +3631,7 @@
       </c>
     </row>
     <row r="47" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="Y47" s="158"/>
+      <c r="Y47" s="162"/>
       <c r="Z47" s="8">
         <v>0</v>
       </c>
@@ -3643,7 +3643,7 @@
       </c>
     </row>
     <row r="48" spans="13:29" x14ac:dyDescent="0.2">
-      <c r="Y48" s="158"/>
+      <c r="Y48" s="162"/>
       <c r="Z48" s="8">
         <v>0.5</v>
       </c>
@@ -3655,7 +3655,7 @@
       </c>
     </row>
     <row r="49" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y49" s="158"/>
+      <c r="Y49" s="162"/>
       <c r="Z49" s="8">
         <v>1</v>
       </c>
@@ -3667,7 +3667,7 @@
       </c>
     </row>
     <row r="50" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y50" s="158"/>
+      <c r="Y50" s="162"/>
       <c r="Z50" s="8">
         <v>1.5</v>
       </c>
@@ -3679,7 +3679,7 @@
       </c>
     </row>
     <row r="51" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y51" s="159"/>
+      <c r="Y51" s="154"/>
       <c r="Z51" s="11">
         <v>2</v>
       </c>
@@ -3692,7 +3692,7 @@
       <c r="AC51" s="13"/>
     </row>
     <row r="52" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y52" s="157" t="s">
+      <c r="Y52" s="161" t="s">
         <v>69</v>
       </c>
       <c r="Z52" s="1" t="s">
@@ -3701,62 +3701,62 @@
       <c r="AA52" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AC52" s="160" t="s">
+      <c r="AC52" s="163" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="53" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y53" s="158"/>
+      <c r="Y53" s="162"/>
       <c r="Z53" s="1">
         <v>0</v>
       </c>
       <c r="AA53" s="34">
         <v>6.1733623452348702E-2</v>
       </c>
-      <c r="AC53" s="161"/>
+      <c r="AC53" s="165"/>
     </row>
     <row r="54" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y54" s="158"/>
+      <c r="Y54" s="162"/>
       <c r="Z54" s="1">
         <v>2</v>
       </c>
       <c r="AA54" s="34">
         <v>1.20772053410085E-2</v>
       </c>
-      <c r="AC54" s="161"/>
+      <c r="AC54" s="165"/>
     </row>
     <row r="55" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y55" s="158"/>
+      <c r="Y55" s="162"/>
       <c r="Z55" s="1">
         <v>4</v>
       </c>
       <c r="AA55" s="31">
         <v>2.2662402083130201E-3</v>
       </c>
-      <c r="AC55" s="161"/>
+      <c r="AC55" s="165"/>
     </row>
     <row r="56" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y56" s="158"/>
+      <c r="Y56" s="162"/>
       <c r="Z56" s="1">
         <v>6</v>
       </c>
       <c r="AA56" s="28">
         <v>4.2184786680835203E-4</v>
       </c>
-      <c r="AC56" s="161"/>
+      <c r="AC56" s="165"/>
     </row>
     <row r="57" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y57" s="158"/>
+      <c r="Y57" s="162"/>
       <c r="Z57" s="1">
         <v>8</v>
       </c>
       <c r="AA57" s="28">
         <v>7.8406646322768398E-5</v>
       </c>
-      <c r="AC57" s="161"/>
+      <c r="AC57" s="165"/>
     </row>
     <row r="58" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y58" s="159"/>
+      <c r="Y58" s="154"/>
       <c r="Z58" s="13">
         <v>10</v>
       </c>
@@ -3764,10 +3764,10 @@
         <v>1.4568956039108299E-5</v>
       </c>
       <c r="AB58" s="13"/>
-      <c r="AC58" s="162"/>
+      <c r="AC58" s="164"/>
     </row>
     <row r="59" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y59" s="157" t="s">
+      <c r="Y59" s="161" t="s">
         <v>73</v>
       </c>
       <c r="Z59" s="1" t="s">
@@ -3776,72 +3776,72 @@
       <c r="AA59" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="AC59" s="160" t="s">
+      <c r="AC59" s="163" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="60" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y60" s="158"/>
+      <c r="Y60" s="162"/>
       <c r="Z60" s="1">
         <v>0</v>
       </c>
       <c r="AA60" s="34">
         <v>4.213704983443E-2</v>
       </c>
-      <c r="AC60" s="161"/>
+      <c r="AC60" s="165"/>
     </row>
     <row r="61" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y61" s="158"/>
+      <c r="Y61" s="162"/>
       <c r="Z61" s="1">
         <v>4</v>
       </c>
       <c r="AA61" s="36">
         <v>0.70383460067707004</v>
       </c>
-      <c r="AC61" s="161"/>
+      <c r="AC61" s="165"/>
     </row>
     <row r="62" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y62" s="158"/>
+      <c r="Y62" s="162"/>
       <c r="Z62" s="1">
         <v>8</v>
       </c>
       <c r="AA62" s="36">
         <v>0.99227108557330002</v>
       </c>
-      <c r="AC62" s="161"/>
+      <c r="AC62" s="165"/>
     </row>
     <row r="63" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y63" s="158"/>
+      <c r="Y63" s="162"/>
       <c r="Z63" s="1">
         <v>12</v>
       </c>
       <c r="AA63" s="37">
         <v>0.99985583826317304</v>
       </c>
-      <c r="AC63" s="161"/>
+      <c r="AC63" s="165"/>
     </row>
     <row r="64" spans="25:29" x14ac:dyDescent="0.2">
-      <c r="Y64" s="158"/>
+      <c r="Y64" s="162"/>
       <c r="Z64" s="1">
         <v>16</v>
       </c>
       <c r="AA64" s="37">
         <v>0.99999733107778499</v>
       </c>
-      <c r="AC64" s="161"/>
+      <c r="AC64" s="165"/>
     </row>
     <row r="65" spans="25:36" x14ac:dyDescent="0.2">
-      <c r="Y65" s="158"/>
+      <c r="Y65" s="162"/>
       <c r="Z65" s="1">
         <v>20</v>
       </c>
       <c r="AA65" s="37">
         <v>0.99999995059606805</v>
       </c>
-      <c r="AC65" s="161"/>
+      <c r="AC65" s="165"/>
     </row>
     <row r="66" spans="25:36" x14ac:dyDescent="0.2">
-      <c r="Y66" s="159"/>
+      <c r="Y66" s="154"/>
       <c r="Z66" s="13">
         <v>24</v>
       </c>
@@ -3849,7 +3849,7 @@
         <v>0.99999999908549497</v>
       </c>
       <c r="AB66" s="13"/>
-      <c r="AC66" s="162"/>
+      <c r="AC66" s="164"/>
     </row>
     <row r="71" spans="25:36" x14ac:dyDescent="0.2">
       <c r="AD71" s="1" t="s">
@@ -3898,7 +3898,7 @@
       </c>
     </row>
     <row r="74" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD74" s="160" t="s">
+      <c r="AD74" s="163" t="s">
         <v>9</v>
       </c>
       <c r="AE74" s="48" t="s">
@@ -3918,7 +3918,7 @@
       </c>
     </row>
     <row r="75" spans="25:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="AD75" s="162"/>
+      <c r="AD75" s="164"/>
       <c r="AE75" s="49" t="s">
         <v>13</v>
       </c>
@@ -3936,7 +3936,7 @@
       </c>
     </row>
     <row r="76" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD76" s="160" t="s">
+      <c r="AD76" s="163" t="s">
         <v>10</v>
       </c>
       <c r="AE76" s="48" t="s">
@@ -3956,7 +3956,7 @@
       </c>
     </row>
     <row r="77" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD77" s="161"/>
+      <c r="AD77" s="165"/>
       <c r="AE77" s="50" t="s">
         <v>17</v>
       </c>
@@ -3974,7 +3974,7 @@
       </c>
     </row>
     <row r="78" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD78" s="162"/>
+      <c r="AD78" s="164"/>
       <c r="AE78" s="49" t="s">
         <v>12</v>
       </c>
@@ -3992,7 +3992,7 @@
       </c>
     </row>
     <row r="79" spans="25:36" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD79" s="160" t="s">
+      <c r="AD79" s="163" t="s">
         <v>11</v>
       </c>
       <c r="AE79" s="48" t="s">
@@ -4012,7 +4012,7 @@
       </c>
     </row>
     <row r="80" spans="25:36" ht="34" x14ac:dyDescent="0.2">
-      <c r="AD80" s="161"/>
+      <c r="AD80" s="165"/>
       <c r="AE80" s="50" t="s">
         <v>19</v>
       </c>
@@ -4030,7 +4030,7 @@
       </c>
     </row>
     <row r="81" spans="30:47" ht="17" x14ac:dyDescent="0.2">
-      <c r="AD81" s="161"/>
+      <c r="AD81" s="165"/>
       <c r="AE81" s="50" t="s">
         <v>13</v>
       </c>
@@ -4048,7 +4048,7 @@
       </c>
     </row>
     <row r="82" spans="30:47" ht="34" x14ac:dyDescent="0.2">
-      <c r="AD82" s="162"/>
+      <c r="AD82" s="164"/>
       <c r="AE82" s="49" t="s">
         <v>15</v>
       </c>
@@ -4066,18 +4066,18 @@
       </c>
     </row>
     <row r="87" spans="30:47" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AL87" s="164" t="s">
+      <c r="AL87" s="152" t="s">
         <v>274</v>
       </c>
-      <c r="AM87" s="164"/>
-      <c r="AN87" s="164"/>
-      <c r="AO87" s="164"/>
-      <c r="AP87" s="164"/>
-      <c r="AQ87" s="164"/>
-      <c r="AR87" s="164"/>
-      <c r="AS87" s="164"/>
-      <c r="AT87" s="164"/>
-      <c r="AU87" s="164"/>
+      <c r="AM87" s="152"/>
+      <c r="AN87" s="152"/>
+      <c r="AO87" s="152"/>
+      <c r="AP87" s="152"/>
+      <c r="AQ87" s="152"/>
+      <c r="AR87" s="152"/>
+      <c r="AS87" s="152"/>
+      <c r="AT87" s="152"/>
+      <c r="AU87" s="152"/>
     </row>
     <row r="88" spans="30:47" ht="35" thickTop="1" x14ac:dyDescent="0.2">
       <c r="AL88" s="55" t="s">
@@ -4112,13 +4112,13 @@
       </c>
     </row>
     <row r="89" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL89" s="154" t="s">
+      <c r="AL89" s="155" t="s">
         <v>9</v>
       </c>
-      <c r="AM89" s="151" t="s">
+      <c r="AM89" s="158" t="s">
         <v>279</v>
       </c>
-      <c r="AN89" s="157" t="s">
+      <c r="AN89" s="161" t="s">
         <v>13</v>
       </c>
       <c r="AO89" s="40" t="s">
@@ -4136,17 +4136,17 @@
       <c r="AS89" s="57" t="s">
         <v>288</v>
       </c>
-      <c r="AT89" s="154" t="s">
+      <c r="AT89" s="155" t="s">
         <v>287</v>
       </c>
-      <c r="AU89" s="151" t="s">
+      <c r="AU89" s="158" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="90" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL90" s="155"/>
-      <c r="AM90" s="152"/>
-      <c r="AN90" s="158"/>
+      <c r="AL90" s="156"/>
+      <c r="AM90" s="159"/>
+      <c r="AN90" s="162"/>
       <c r="AO90" s="1" t="s">
         <v>68</v>
       </c>
@@ -4162,13 +4162,13 @@
       <c r="AS90" s="58">
         <v>1E-3</v>
       </c>
-      <c r="AT90" s="155"/>
-      <c r="AU90" s="152"/>
+      <c r="AT90" s="156"/>
+      <c r="AU90" s="159"/>
     </row>
     <row r="91" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL91" s="156"/>
-      <c r="AM91" s="153"/>
-      <c r="AN91" s="159"/>
+      <c r="AL91" s="157"/>
+      <c r="AM91" s="160"/>
+      <c r="AN91" s="154"/>
       <c r="AO91" s="13" t="s">
         <v>286</v>
       </c>
@@ -4184,17 +4184,17 @@
       <c r="AS91" s="59">
         <v>2.0000000000000001E-4</v>
       </c>
-      <c r="AT91" s="156"/>
-      <c r="AU91" s="153"/>
+      <c r="AT91" s="157"/>
+      <c r="AU91" s="160"/>
     </row>
     <row r="92" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL92" s="154" t="s">
+      <c r="AL92" s="155" t="s">
         <v>10</v>
       </c>
-      <c r="AM92" s="154" t="s">
+      <c r="AM92" s="155" t="s">
         <v>280</v>
       </c>
-      <c r="AN92" s="157" t="s">
+      <c r="AN92" s="161" t="s">
         <v>12</v>
       </c>
       <c r="AO92" s="40" t="s">
@@ -4212,17 +4212,17 @@
       <c r="AS92" s="57" t="s">
         <v>288</v>
       </c>
-      <c r="AT92" s="154" t="s">
+      <c r="AT92" s="155" t="s">
         <v>287</v>
       </c>
-      <c r="AU92" s="151" t="s">
+      <c r="AU92" s="158" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="93" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL93" s="155"/>
-      <c r="AM93" s="155"/>
-      <c r="AN93" s="158"/>
+      <c r="AL93" s="156"/>
+      <c r="AM93" s="156"/>
+      <c r="AN93" s="162"/>
       <c r="AO93" s="1" t="s">
         <v>68</v>
       </c>
@@ -4238,13 +4238,13 @@
       <c r="AS93" s="58">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="AT93" s="155"/>
-      <c r="AU93" s="152"/>
+      <c r="AT93" s="156"/>
+      <c r="AU93" s="159"/>
     </row>
     <row r="94" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL94" s="155"/>
-      <c r="AM94" s="155"/>
-      <c r="AN94" s="158"/>
+      <c r="AL94" s="156"/>
+      <c r="AM94" s="156"/>
+      <c r="AN94" s="162"/>
       <c r="AO94" s="1" t="s">
         <v>286</v>
       </c>
@@ -4260,15 +4260,15 @@
       <c r="AS94" s="58">
         <v>2E-3</v>
       </c>
-      <c r="AT94" s="155"/>
-      <c r="AU94" s="152"/>
+      <c r="AT94" s="156"/>
+      <c r="AU94" s="159"/>
     </row>
     <row r="95" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL95" s="155"/>
-      <c r="AM95" s="152" t="s">
+      <c r="AL95" s="156"/>
+      <c r="AM95" s="159" t="s">
         <v>279</v>
       </c>
-      <c r="AN95" s="158" t="s">
+      <c r="AN95" s="162" t="s">
         <v>17</v>
       </c>
       <c r="AO95" t="s">
@@ -4286,17 +4286,17 @@
       <c r="AS95" s="58" t="s">
         <v>288</v>
       </c>
-      <c r="AT95" s="155" t="s">
+      <c r="AT95" s="156" t="s">
         <v>287</v>
       </c>
-      <c r="AU95" s="152" t="s">
+      <c r="AU95" s="159" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="96" spans="30:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL96" s="155"/>
-      <c r="AM96" s="152"/>
-      <c r="AN96" s="158"/>
+      <c r="AL96" s="156"/>
+      <c r="AM96" s="159"/>
+      <c r="AN96" s="162"/>
       <c r="AO96" s="1" t="s">
         <v>68</v>
       </c>
@@ -4312,13 +4312,13 @@
       <c r="AS96" s="58">
         <v>2E-3</v>
       </c>
-      <c r="AT96" s="155"/>
-      <c r="AU96" s="152"/>
+      <c r="AT96" s="156"/>
+      <c r="AU96" s="159"/>
     </row>
     <row r="97" spans="38:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL97" s="156"/>
-      <c r="AM97" s="153"/>
-      <c r="AN97" s="159"/>
+      <c r="AL97" s="157"/>
+      <c r="AM97" s="160"/>
+      <c r="AN97" s="154"/>
       <c r="AO97" s="13" t="s">
         <v>286</v>
       </c>
@@ -4334,17 +4334,17 @@
       <c r="AS97" s="59" t="s">
         <v>288</v>
       </c>
-      <c r="AT97" s="156"/>
-      <c r="AU97" s="153"/>
+      <c r="AT97" s="157"/>
+      <c r="AU97" s="160"/>
     </row>
     <row r="98" spans="38:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL98" s="154" t="s">
+      <c r="AL98" s="155" t="s">
         <v>11</v>
       </c>
-      <c r="AM98" s="151" t="s">
+      <c r="AM98" s="158" t="s">
         <v>279</v>
       </c>
-      <c r="AN98" s="157" t="s">
+      <c r="AN98" s="161" t="s">
         <v>13</v>
       </c>
       <c r="AO98" s="60" t="s">
@@ -4362,17 +4362,17 @@
       <c r="AS98" s="57" t="s">
         <v>288</v>
       </c>
-      <c r="AT98" s="154" t="s">
+      <c r="AT98" s="155" t="s">
         <v>287</v>
       </c>
-      <c r="AU98" s="151" t="s">
+      <c r="AU98" s="158" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="99" spans="38:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL99" s="155"/>
-      <c r="AM99" s="152"/>
-      <c r="AN99" s="158"/>
+      <c r="AL99" s="156"/>
+      <c r="AM99" s="159"/>
+      <c r="AN99" s="162"/>
       <c r="AO99" s="1" t="s">
         <v>68</v>
       </c>
@@ -4388,13 +4388,13 @@
       <c r="AS99" s="58">
         <v>0.04</v>
       </c>
-      <c r="AT99" s="155"/>
-      <c r="AU99" s="152"/>
+      <c r="AT99" s="156"/>
+      <c r="AU99" s="159"/>
     </row>
     <row r="100" spans="38:47" ht="30" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="AL100" s="156"/>
-      <c r="AM100" s="153"/>
-      <c r="AN100" s="159"/>
+      <c r="AL100" s="157"/>
+      <c r="AM100" s="160"/>
+      <c r="AN100" s="154"/>
       <c r="AO100" s="13" t="s">
         <v>286</v>
       </c>
@@ -4410,11 +4410,28 @@
       <c r="AS100" s="59" t="s">
         <v>288</v>
       </c>
-      <c r="AT100" s="156"/>
-      <c r="AU100" s="153"/>
+      <c r="AT100" s="157"/>
+      <c r="AU100" s="160"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="AM98:AM100"/>
+    <mergeCell ref="AL98:AL100"/>
+    <mergeCell ref="AL92:AL97"/>
+    <mergeCell ref="AM92:AM94"/>
+    <mergeCell ref="AM95:AM97"/>
+    <mergeCell ref="AU95:AU97"/>
+    <mergeCell ref="AT95:AT97"/>
+    <mergeCell ref="AT98:AT100"/>
+    <mergeCell ref="AU98:AU100"/>
+    <mergeCell ref="AN98:AN100"/>
+    <mergeCell ref="AN95:AN97"/>
+    <mergeCell ref="Y59:Y66"/>
+    <mergeCell ref="AC52:AC58"/>
+    <mergeCell ref="AC59:AC66"/>
+    <mergeCell ref="AT92:AT94"/>
+    <mergeCell ref="AU92:AU94"/>
+    <mergeCell ref="AN92:AN94"/>
     <mergeCell ref="N32:Q32"/>
     <mergeCell ref="M31:Q31"/>
     <mergeCell ref="M32:M33"/>
@@ -4431,23 +4448,6 @@
     <mergeCell ref="Z45:AB45"/>
     <mergeCell ref="Y46:Y51"/>
     <mergeCell ref="Y52:Y58"/>
-    <mergeCell ref="Y59:Y66"/>
-    <mergeCell ref="AC52:AC58"/>
-    <mergeCell ref="AC59:AC66"/>
-    <mergeCell ref="AT92:AT94"/>
-    <mergeCell ref="AU92:AU94"/>
-    <mergeCell ref="AN92:AN94"/>
-    <mergeCell ref="AU95:AU97"/>
-    <mergeCell ref="AT95:AT97"/>
-    <mergeCell ref="AT98:AT100"/>
-    <mergeCell ref="AU98:AU100"/>
-    <mergeCell ref="AN98:AN100"/>
-    <mergeCell ref="AN95:AN97"/>
-    <mergeCell ref="AM98:AM100"/>
-    <mergeCell ref="AL98:AL100"/>
-    <mergeCell ref="AL92:AL97"/>
-    <mergeCell ref="AM92:AM94"/>
-    <mergeCell ref="AM95:AM97"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5435,8 +5435,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7C301AE6-CC50-864C-827E-D25EEF6A22D3}">
   <dimension ref="A2:AN151"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C118" sqref="C118"/>
+    <sheetView tabSelected="1" topLeftCell="A102" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C134" sqref="C134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5468,43 +5468,43 @@
     <row r="3" spans="1:14" ht="17" hidden="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="89"/>
       <c r="B3" s="146" t="s">
+        <v>427</v>
+      </c>
+      <c r="C3" s="146" t="s">
         <v>428</v>
       </c>
-      <c r="C3" s="146" t="s">
+      <c r="D3" s="146" t="s">
         <v>429</v>
       </c>
-      <c r="D3" s="146" t="s">
+      <c r="E3" s="146" t="s">
         <v>430</v>
       </c>
-      <c r="E3" s="146" t="s">
+      <c r="F3" s="146" t="s">
         <v>431</v>
       </c>
-      <c r="F3" s="146" t="s">
+      <c r="G3" s="146" t="s">
         <v>432</v>
       </c>
-      <c r="G3" s="146" t="s">
+      <c r="H3" s="146" t="s">
         <v>433</v>
       </c>
-      <c r="H3" s="146" t="s">
+      <c r="I3" s="146" t="s">
         <v>434</v>
       </c>
-      <c r="I3" s="146" t="s">
+      <c r="J3" s="146" t="s">
         <v>435</v>
       </c>
-      <c r="J3" s="146" t="s">
+      <c r="K3" s="146" t="s">
         <v>436</v>
       </c>
-      <c r="K3" s="146" t="s">
+      <c r="L3" s="146" t="s">
         <v>437</v>
       </c>
-      <c r="L3" s="146" t="s">
+      <c r="M3" s="146" t="s">
         <v>438</v>
       </c>
-      <c r="M3" s="146" t="s">
-        <v>439</v>
-      </c>
       <c r="N3" s="146" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="18" thickTop="1" x14ac:dyDescent="0.2">
@@ -7550,7 +7550,7 @@
     <row r="80" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B80" s="123"/>
       <c r="C80" s="34" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="D80" s="34">
         <v>1.40262</v>
@@ -8553,7 +8553,7 @@
     <row r="117" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B117" s="127"/>
       <c r="C117" s="150" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D117" s="112">
         <v>1.9009999999999999E-2</v>
@@ -8580,7 +8580,7 @@
     <row r="118" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B118" s="127"/>
       <c r="C118" s="150" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="D118" s="112">
         <v>-1.66638</v>
@@ -8607,7 +8607,7 @@
     <row r="119" spans="2:14" ht="17" x14ac:dyDescent="0.2">
       <c r="B119" s="127"/>
       <c r="C119" s="150" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D119" s="112">
         <v>-1.91638</v>
@@ -8783,25 +8783,25 @@
       <c r="M125" s="142"/>
       <c r="N125" s="143"/>
     </row>
-    <row r="126" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="126" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B126" s="127"/>
       <c r="C126" s="139" t="s">
         <v>370</v>
       </c>
       <c r="D126" s="34">
-        <v>1.0812999999999999</v>
+        <v>0.84911000000000003</v>
       </c>
       <c r="E126" s="34">
-        <v>0.21307000000000001</v>
+        <v>0.22067999999999999</v>
       </c>
       <c r="F126" s="34">
-        <v>23.65663</v>
+        <v>23.22897</v>
       </c>
       <c r="G126" s="34">
-        <v>5.0750000000000002</v>
+        <v>3.8479999999999999</v>
       </c>
       <c r="H126" s="34">
-        <v>3.5800000000000003E-5</v>
+        <v>8.0900000000000004E-4</v>
       </c>
       <c r="I126" s="34">
         <v>3393.069</v>
@@ -8826,19 +8826,19 @@
         <v>328</v>
       </c>
       <c r="D127" s="34">
-        <v>0.35282999999999998</v>
+        <v>0.88075999999999999</v>
       </c>
       <c r="E127" s="34">
-        <v>4.9750000000000003E-2</v>
+        <v>2.7009999999999999E-2</v>
       </c>
       <c r="F127" s="34">
-        <v>2044.2178699999999</v>
+        <v>2039.4976999999999</v>
       </c>
       <c r="G127" s="34">
-        <v>7.093</v>
-      </c>
-      <c r="H127" s="34">
-        <v>1.81E-12</v>
+        <v>32.613</v>
+      </c>
+      <c r="H127" s="34" t="s">
+        <v>371</v>
       </c>
       <c r="I127" s="34"/>
       <c r="J127" s="34"/>
@@ -8849,23 +8849,23 @@
     </row>
     <row r="128" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B128" s="127"/>
-      <c r="C128" s="150" t="s">
+      <c r="C128" s="180" t="s">
         <v>410</v>
       </c>
       <c r="D128" s="34">
-        <v>-0.52864999999999995</v>
+        <v>-0.23485</v>
       </c>
       <c r="E128" s="34">
-        <v>0.26839000000000002</v>
+        <v>0.27795999999999998</v>
       </c>
       <c r="F128" s="34">
-        <v>23.369250000000001</v>
+        <v>22.944400000000002</v>
       </c>
       <c r="G128" s="34">
-        <v>-1.97</v>
+        <v>-0.84499999999999997</v>
       </c>
       <c r="H128" s="34">
-        <v>6.0835E-2</v>
+        <v>0.406893</v>
       </c>
       <c r="I128" s="34"/>
       <c r="J128" s="34"/>
@@ -8874,25 +8874,25 @@
       <c r="M128" s="34"/>
       <c r="N128" s="108"/>
     </row>
-    <row r="129" spans="2:14" ht="17" x14ac:dyDescent="0.2">
+    <row r="129" spans="2:14" x14ac:dyDescent="0.2">
       <c r="B129" s="127"/>
       <c r="C129" s="139" t="s">
         <v>389</v>
       </c>
       <c r="D129" s="34">
-        <v>-0.35528999999999999</v>
+        <v>-0.35688999999999999</v>
       </c>
       <c r="E129" s="34">
-        <v>0.13358999999999999</v>
+        <v>0.13889000000000001</v>
       </c>
       <c r="F129" s="34">
-        <v>23.406179999999999</v>
+        <v>23.33747</v>
       </c>
       <c r="G129" s="34">
-        <v>-2.66</v>
+        <v>-2.57</v>
       </c>
       <c r="H129" s="34">
-        <v>1.3885E-2</v>
+        <v>1.7024000000000001E-2</v>
       </c>
       <c r="I129" s="34"/>
       <c r="J129" s="34"/>
@@ -8907,19 +8907,19 @@
         <v>372</v>
       </c>
       <c r="D130" s="34">
-        <v>-0.56728000000000001</v>
+        <v>-0.55330000000000001</v>
       </c>
       <c r="E130" s="34">
-        <v>0.13436999999999999</v>
+        <v>0.13969000000000001</v>
       </c>
       <c r="F130" s="34">
-        <v>23.951989999999999</v>
+        <v>23.87529</v>
       </c>
       <c r="G130" s="34">
-        <v>-4.2220000000000004</v>
+        <v>-3.9609999999999999</v>
       </c>
       <c r="H130" s="34">
-        <v>3.01E-4</v>
+        <v>5.8600000000000004E-4</v>
       </c>
       <c r="I130" s="34"/>
       <c r="J130" s="34"/>
@@ -8928,69 +8928,28 @@
       <c r="M130" s="34"/>
       <c r="N130" s="108"/>
     </row>
-    <row r="131" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B131" s="127"/>
-      <c r="C131" s="150" t="s">
-        <v>411</v>
-      </c>
-      <c r="D131" s="34">
-        <v>0.70560999999999996</v>
-      </c>
-      <c r="E131" s="34">
-        <v>5.6649999999999999E-2</v>
-      </c>
-      <c r="F131" s="34">
-        <v>2037.85367</v>
-      </c>
-      <c r="G131" s="34">
-        <v>12.455</v>
-      </c>
-      <c r="H131" s="34" t="s">
-        <v>371</v>
-      </c>
-      <c r="I131" s="34"/>
-      <c r="J131" s="34"/>
-      <c r="K131" s="34"/>
-      <c r="L131" s="34"/>
-      <c r="M131" s="34"/>
-      <c r="N131" s="108"/>
-    </row>
+    <row r="131" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="132" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B132" s="127"/>
-      <c r="C132" s="34"/>
-      <c r="D132" s="34"/>
-      <c r="E132" s="34"/>
-      <c r="F132" s="34"/>
-      <c r="G132" s="34"/>
-      <c r="H132" s="34"/>
-      <c r="I132" s="34"/>
-      <c r="J132" s="34"/>
-      <c r="K132" s="34"/>
-      <c r="L132" s="34"/>
-      <c r="M132" s="34"/>
-      <c r="N132" s="108"/>
-    </row>
-    <row r="134" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C134" s="19"/>
+      <c r="C132" s="19"/>
     </row>
     <row r="135" spans="2:14" ht="21" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="136" spans="2:14" ht="16" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="C140" s="25"/>
-    </row>
-    <row r="141" spans="2:14" x14ac:dyDescent="0.2">
-      <c r="B141" s="90"/>
-      <c r="D141" s="25"/>
-      <c r="E141" s="25"/>
-      <c r="F141" s="25"/>
-      <c r="G141" s="25"/>
-      <c r="H141" s="25"/>
-      <c r="I141" s="25"/>
-      <c r="J141" s="25"/>
-      <c r="K141" s="25"/>
-      <c r="L141" s="25"/>
-      <c r="M141" s="25"/>
-      <c r="N141" s="25"/>
+    <row r="138" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="C138" s="25"/>
+    </row>
+    <row r="139" spans="2:14" x14ac:dyDescent="0.2">
+      <c r="B139" s="90"/>
+      <c r="D139" s="25"/>
+      <c r="E139" s="25"/>
+      <c r="F139" s="25"/>
+      <c r="G139" s="25"/>
+      <c r="H139" s="25"/>
+      <c r="I139" s="25"/>
+      <c r="J139" s="25"/>
+      <c r="K139" s="25"/>
+      <c r="L139" s="25"/>
+      <c r="M139" s="25"/>
+      <c r="N139" s="25"/>
     </row>
     <row r="151" spans="2:40" s="25" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B151" s="89"/>
@@ -9854,7 +9813,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6964B3A-A93B-A24A-8DF2-4AA66B6335FC}">
   <dimension ref="B3:AN237"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="146" workbookViewId="0">
+    <sheetView zoomScale="146" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
@@ -9890,26 +9849,26 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="164" t="s">
+      <c r="B3" s="152" t="s">
         <v>274</v>
       </c>
-      <c r="C3" s="164"/>
-      <c r="D3" s="164"/>
-      <c r="E3" s="164"/>
-      <c r="F3" s="164"/>
-      <c r="G3" s="164"/>
-      <c r="H3" s="164"/>
-      <c r="I3" s="164"/>
-      <c r="J3" s="164"/>
-      <c r="K3" s="164"/>
-      <c r="L3" s="164"/>
-      <c r="M3" s="164"/>
-      <c r="N3" s="164"/>
-      <c r="O3" s="164"/>
-      <c r="P3" s="164"/>
-      <c r="Q3" s="164"/>
-      <c r="R3" s="164"/>
-      <c r="S3" s="164"/>
+      <c r="C3" s="152"/>
+      <c r="D3" s="152"/>
+      <c r="E3" s="152"/>
+      <c r="F3" s="152"/>
+      <c r="G3" s="152"/>
+      <c r="H3" s="152"/>
+      <c r="I3" s="152"/>
+      <c r="J3" s="152"/>
+      <c r="K3" s="152"/>
+      <c r="L3" s="152"/>
+      <c r="M3" s="152"/>
+      <c r="N3" s="152"/>
+      <c r="O3" s="152"/>
+      <c r="P3" s="152"/>
+      <c r="Q3" s="152"/>
+      <c r="R3" s="152"/>
+      <c r="S3" s="152"/>
       <c r="T3" s="54"/>
     </row>
     <row r="4" spans="2:20" ht="60" thickTop="1" x14ac:dyDescent="0.2">
@@ -9920,19 +9879,19 @@
         <v>358</v>
       </c>
       <c r="D4" s="13" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="E4" s="13" t="s">
         <v>276</v>
       </c>
       <c r="F4" s="26" t="s">
+        <v>425</v>
+      </c>
+      <c r="G4" s="26" t="s">
         <v>426</v>
       </c>
-      <c r="G4" s="26" t="s">
-        <v>427</v>
-      </c>
       <c r="H4" s="26" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="I4" s="13" t="s">
         <v>341</v>
@@ -9950,26 +9909,26 @@
         <v>377</v>
       </c>
       <c r="N4" s="13" t="s">
+        <v>418</v>
+      </c>
+      <c r="O4" s="26" t="s">
+        <v>421</v>
+      </c>
+      <c r="P4" s="26" t="s">
+        <v>422</v>
+      </c>
+      <c r="Q4" s="13" t="s">
         <v>419</v>
       </c>
-      <c r="O4" s="26" t="s">
-        <v>422</v>
-      </c>
-      <c r="P4" s="26" t="s">
-        <v>423</v>
-      </c>
-      <c r="Q4" s="13" t="s">
+      <c r="R4" s="13" t="s">
         <v>420</v>
-      </c>
-      <c r="R4" s="13" t="s">
-        <v>421</v>
       </c>
       <c r="S4" s="13" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="5" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B5" s="169" t="s">
+      <c r="B5" s="171" t="s">
         <v>79</v>
       </c>
       <c r="C5" s="85" t="s">
@@ -9983,7 +9942,7 @@
       </c>
     </row>
     <row r="6" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B6" s="170"/>
+      <c r="B6" s="172"/>
       <c r="C6" s="85" t="s">
         <v>16</v>
       </c>
@@ -9995,8 +9954,8 @@
       </c>
     </row>
     <row r="7" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B7" s="170"/>
-      <c r="C7" s="172" t="s">
+      <c r="B7" s="172"/>
+      <c r="C7" s="169" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="1" t="s">
@@ -10048,8 +10007,8 @@
       <c r="T7" s="25"/>
     </row>
     <row r="8" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B8" s="170"/>
-      <c r="C8" s="172"/>
+      <c r="B8" s="172"/>
+      <c r="C8" s="169"/>
       <c r="E8" s="77" t="s">
         <v>263</v>
       </c>
@@ -10078,8 +10037,8 @@
       <c r="R8" s="36"/>
     </row>
     <row r="9" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B9" s="170"/>
-      <c r="C9" s="172" t="s">
+      <c r="B9" s="172"/>
+      <c r="C9" s="169" t="s">
         <v>34</v>
       </c>
       <c r="D9" s="1" t="s">
@@ -10127,8 +10086,8 @@
       </c>
     </row>
     <row r="10" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B10" s="170"/>
-      <c r="C10" s="172"/>
+      <c r="B10" s="172"/>
+      <c r="C10" s="169"/>
       <c r="E10" s="84" t="s">
         <v>263</v>
       </c>
@@ -10155,8 +10114,8 @@
       <c r="R10" s="36"/>
     </row>
     <row r="11" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B11" s="170"/>
-      <c r="C11" s="172"/>
+      <c r="B11" s="172"/>
+      <c r="C11" s="169"/>
       <c r="E11" s="77" t="s">
         <v>32</v>
       </c>
@@ -10183,7 +10142,7 @@
       <c r="R11" s="36"/>
     </row>
     <row r="12" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B12" s="170"/>
+      <c r="B12" s="172"/>
       <c r="C12" s="85" t="s">
         <v>35</v>
       </c>
@@ -10208,8 +10167,8 @@
       <c r="R12" s="36"/>
     </row>
     <row r="13" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B13" s="170"/>
-      <c r="C13" s="172" t="s">
+      <c r="B13" s="172"/>
+      <c r="C13" s="169" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="1" t="s">
@@ -10257,8 +10216,8 @@
       </c>
     </row>
     <row r="14" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B14" s="170"/>
-      <c r="C14" s="172"/>
+      <c r="B14" s="172"/>
+      <c r="C14" s="169"/>
       <c r="E14" s="77" t="s">
         <v>263</v>
       </c>
@@ -10285,8 +10244,8 @@
       <c r="R14" s="36"/>
     </row>
     <row r="15" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B15" s="170"/>
-      <c r="C15" s="172" t="s">
+      <c r="B15" s="172"/>
+      <c r="C15" s="169" t="s">
         <v>37</v>
       </c>
       <c r="D15" s="1" t="s">
@@ -10334,8 +10293,8 @@
       </c>
     </row>
     <row r="16" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B16" s="170"/>
-      <c r="C16" s="172"/>
+      <c r="B16" s="172"/>
+      <c r="C16" s="169"/>
       <c r="E16" s="77" t="s">
         <v>263</v>
       </c>
@@ -10362,7 +10321,7 @@
       <c r="R16" s="36"/>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B17" s="170"/>
+      <c r="B17" s="172"/>
       <c r="C17" s="85" t="s">
         <v>36</v>
       </c>
@@ -10387,7 +10346,7 @@
       <c r="R17" s="36"/>
     </row>
     <row r="18" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B18" s="170"/>
+      <c r="B18" s="172"/>
       <c r="C18" s="85" t="s">
         <v>12</v>
       </c>
@@ -10412,8 +10371,8 @@
       <c r="R18" s="36"/>
     </row>
     <row r="19" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B19" s="170"/>
-      <c r="C19" s="172" t="s">
+      <c r="B19" s="172"/>
+      <c r="C19" s="169" t="s">
         <v>19</v>
       </c>
       <c r="D19" s="1" t="s">
@@ -10463,8 +10422,8 @@
       </c>
     </row>
     <row r="20" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B20" s="170"/>
-      <c r="C20" s="172"/>
+      <c r="B20" s="172"/>
+      <c r="C20" s="169"/>
       <c r="E20" s="84" t="s">
         <v>263</v>
       </c>
@@ -10495,8 +10454,8 @@
       <c r="R20" s="36"/>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B21" s="170"/>
-      <c r="C21" s="172" t="s">
+      <c r="B21" s="172"/>
+      <c r="C21" s="169" t="s">
         <v>13</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -10544,8 +10503,8 @@
       </c>
     </row>
     <row r="22" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B22" s="170"/>
-      <c r="C22" s="172"/>
+      <c r="B22" s="172"/>
+      <c r="C22" s="169"/>
       <c r="E22" s="77" t="s">
         <v>263</v>
       </c>
@@ -10572,8 +10531,8 @@
       <c r="R22" s="36"/>
     </row>
     <row r="23" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B23" s="170"/>
-      <c r="C23" s="172" t="s">
+      <c r="B23" s="172"/>
+      <c r="C23" s="169" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -10619,8 +10578,8 @@
       </c>
     </row>
     <row r="24" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B24" s="170"/>
-      <c r="C24" s="172"/>
+      <c r="B24" s="172"/>
+      <c r="C24" s="169"/>
       <c r="E24" s="77" t="s">
         <v>32</v>
       </c>
@@ -10647,8 +10606,8 @@
       <c r="R24" s="36"/>
     </row>
     <row r="25" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B25" s="170"/>
-      <c r="C25" s="172" t="s">
+      <c r="B25" s="172"/>
+      <c r="C25" s="169" t="s">
         <v>38</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -10696,8 +10655,8 @@
       </c>
     </row>
     <row r="26" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B26" s="170"/>
-      <c r="C26" s="172"/>
+      <c r="B26" s="172"/>
+      <c r="C26" s="169"/>
       <c r="E26" s="77" t="s">
         <v>263</v>
       </c>
@@ -10724,7 +10683,7 @@
       <c r="R26" s="36"/>
     </row>
     <row r="27" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B27" s="170"/>
+      <c r="B27" s="172"/>
       <c r="C27" s="85" t="s">
         <v>20</v>
       </c>
@@ -10749,7 +10708,7 @@
       <c r="R27" s="36"/>
     </row>
     <row r="28" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B28" s="170"/>
+      <c r="B28" s="172"/>
       <c r="C28" s="85" t="s">
         <v>33</v>
       </c>
@@ -10774,8 +10733,8 @@
       <c r="R28" s="36"/>
     </row>
     <row r="29" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B29" s="170"/>
-      <c r="C29" s="172" t="s">
+      <c r="B29" s="172"/>
+      <c r="C29" s="169" t="s">
         <v>39</v>
       </c>
       <c r="D29" s="39" t="s">
@@ -10821,8 +10780,8 @@
       </c>
     </row>
     <row r="30" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B30" s="170"/>
-      <c r="C30" s="172"/>
+      <c r="B30" s="172"/>
+      <c r="C30" s="169"/>
       <c r="D30" s="39"/>
       <c r="E30" s="77" t="s">
         <v>32</v>
@@ -10850,7 +10809,7 @@
       <c r="R30" s="36"/>
     </row>
     <row r="31" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B31" s="170"/>
+      <c r="B31" s="172"/>
       <c r="C31" s="85" t="s">
         <v>41</v>
       </c>
@@ -10875,8 +10834,8 @@
       <c r="R31" s="36"/>
     </row>
     <row r="32" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B32" s="170"/>
-      <c r="C32" s="172" t="s">
+      <c r="B32" s="172"/>
+      <c r="C32" s="169" t="s">
         <v>42</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -10924,8 +10883,8 @@
       </c>
     </row>
     <row r="33" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B33" s="170"/>
-      <c r="C33" s="172"/>
+      <c r="B33" s="172"/>
+      <c r="C33" s="169"/>
       <c r="E33" s="77" t="s">
         <v>263</v>
       </c>
@@ -10952,8 +10911,8 @@
       <c r="R33" s="36"/>
     </row>
     <row r="34" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B34" s="170"/>
-      <c r="C34" s="172"/>
+      <c r="B34" s="172"/>
+      <c r="C34" s="169"/>
       <c r="E34" s="77" t="s">
         <v>32</v>
       </c>
@@ -10980,7 +10939,7 @@
       <c r="R34" s="36"/>
     </row>
     <row r="35" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B35" s="170"/>
+      <c r="B35" s="172"/>
       <c r="C35" s="86" t="s">
         <v>15</v>
       </c>
@@ -11005,7 +10964,7 @@
       <c r="R35" s="36"/>
     </row>
     <row r="36" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B36" s="169" t="s">
+      <c r="B36" s="171" t="s">
         <v>80</v>
       </c>
       <c r="C36" s="174" t="s">
@@ -11031,7 +10990,7 @@
         <v>5.1799999999999997E-3</v>
       </c>
       <c r="K36" s="36" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="L36" s="36">
         <v>-552.79278274914202</v>
@@ -11056,10 +11015,10 @@
       </c>
     </row>
     <row r="37" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B37" s="170"/>
-      <c r="C37" s="172"/>
+      <c r="B37" s="172"/>
+      <c r="C37" s="169"/>
       <c r="E37" s="84" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="F37" s="36">
         <v>0.75480000000000003</v>
@@ -11084,10 +11043,10 @@
       <c r="R37" s="36"/>
     </row>
     <row r="38" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B38" s="170"/>
-      <c r="C38" s="172"/>
+      <c r="B38" s="172"/>
+      <c r="C38" s="169"/>
       <c r="E38" s="84" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="F38" s="36">
         <v>0.55800000000000005</v>
@@ -11112,8 +11071,8 @@
       <c r="R38" s="36"/>
     </row>
     <row r="39" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B39" s="170"/>
-      <c r="C39" s="172"/>
+      <c r="B39" s="172"/>
+      <c r="C39" s="169"/>
       <c r="E39" s="84" t="s">
         <v>32</v>
       </c>
@@ -11140,8 +11099,8 @@
       <c r="R39" s="36"/>
     </row>
     <row r="40" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B40" s="170"/>
-      <c r="C40" s="172" t="s">
+      <c r="B40" s="172"/>
+      <c r="C40" s="169" t="s">
         <v>16</v>
       </c>
       <c r="D40" s="1" t="s">
@@ -11189,8 +11148,8 @@
       </c>
     </row>
     <row r="41" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B41" s="170"/>
-      <c r="C41" s="172"/>
+      <c r="B41" s="172"/>
+      <c r="C41" s="169"/>
       <c r="E41" s="77" t="s">
         <v>335</v>
       </c>
@@ -11219,8 +11178,8 @@
       <c r="R41" s="36"/>
     </row>
     <row r="42" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B42" s="170"/>
-      <c r="C42" s="172" t="s">
+      <c r="B42" s="172"/>
+      <c r="C42" s="169" t="s">
         <v>17</v>
       </c>
       <c r="D42" s="1" t="s">
@@ -11268,8 +11227,8 @@
       </c>
     </row>
     <row r="43" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B43" s="170"/>
-      <c r="C43" s="172"/>
+      <c r="B43" s="172"/>
+      <c r="C43" s="169"/>
       <c r="E43" s="77" t="s">
         <v>263</v>
       </c>
@@ -11296,8 +11255,8 @@
       <c r="R43" s="36"/>
     </row>
     <row r="44" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B44" s="170"/>
-      <c r="C44" s="172"/>
+      <c r="B44" s="172"/>
+      <c r="C44" s="169"/>
       <c r="E44" s="77" t="s">
         <v>32</v>
       </c>
@@ -11324,8 +11283,8 @@
       <c r="R44" s="36"/>
     </row>
     <row r="45" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B45" s="170"/>
-      <c r="C45" s="172"/>
+      <c r="B45" s="172"/>
+      <c r="C45" s="169"/>
       <c r="E45" s="77" t="s">
         <v>335</v>
       </c>
@@ -11352,8 +11311,8 @@
       <c r="R45" s="36"/>
     </row>
     <row r="46" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B46" s="170"/>
-      <c r="C46" s="172" t="s">
+      <c r="B46" s="172"/>
+      <c r="C46" s="169" t="s">
         <v>34</v>
       </c>
       <c r="D46" s="1" t="s">
@@ -11403,8 +11362,8 @@
       </c>
     </row>
     <row r="47" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B47" s="170"/>
-      <c r="C47" s="172"/>
+      <c r="B47" s="172"/>
+      <c r="C47" s="169"/>
       <c r="E47" s="77" t="s">
         <v>263</v>
       </c>
@@ -11433,8 +11392,8 @@
       <c r="R47" s="36"/>
     </row>
     <row r="48" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B48" s="170"/>
-      <c r="C48" s="172"/>
+      <c r="B48" s="172"/>
+      <c r="C48" s="169"/>
       <c r="E48" s="77" t="s">
         <v>335</v>
       </c>
@@ -11463,8 +11422,8 @@
       <c r="R48" s="36"/>
     </row>
     <row r="49" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B49" s="170"/>
-      <c r="C49" s="172"/>
+      <c r="B49" s="172"/>
+      <c r="C49" s="169"/>
       <c r="E49" s="77" t="s">
         <v>32</v>
       </c>
@@ -11493,8 +11452,8 @@
       <c r="R49" s="36"/>
     </row>
     <row r="50" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B50" s="170"/>
-      <c r="C50" s="172" t="s">
+      <c r="B50" s="172"/>
+      <c r="C50" s="169" t="s">
         <v>35</v>
       </c>
       <c r="D50" s="1" t="s">
@@ -11544,8 +11503,8 @@
       </c>
     </row>
     <row r="51" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B51" s="170"/>
-      <c r="C51" s="172"/>
+      <c r="B51" s="172"/>
+      <c r="C51" s="169"/>
       <c r="E51" s="77" t="s">
         <v>263</v>
       </c>
@@ -11574,8 +11533,8 @@
       <c r="R51" s="36"/>
     </row>
     <row r="52" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B52" s="170"/>
-      <c r="C52" s="172"/>
+      <c r="B52" s="172"/>
+      <c r="C52" s="169"/>
       <c r="E52" s="77" t="s">
         <v>335</v>
       </c>
@@ -11604,8 +11563,8 @@
       <c r="R52" s="36"/>
     </row>
     <row r="53" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B53" s="170"/>
-      <c r="C53" s="172" t="s">
+      <c r="B53" s="172"/>
+      <c r="C53" s="169" t="s">
         <v>18</v>
       </c>
       <c r="D53" s="1" t="s">
@@ -11655,8 +11614,8 @@
       </c>
     </row>
     <row r="54" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B54" s="170"/>
-      <c r="C54" s="172"/>
+      <c r="B54" s="172"/>
+      <c r="C54" s="169"/>
       <c r="E54" s="77" t="s">
         <v>263</v>
       </c>
@@ -11685,8 +11644,8 @@
       <c r="R54" s="36"/>
     </row>
     <row r="55" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B55" s="170"/>
-      <c r="C55" s="172"/>
+      <c r="B55" s="172"/>
+      <c r="C55" s="169"/>
       <c r="E55" s="77" t="s">
         <v>335</v>
       </c>
@@ -11715,8 +11674,8 @@
       <c r="R55" s="36"/>
     </row>
     <row r="56" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B56" s="170"/>
-      <c r="C56" s="172" t="s">
+      <c r="B56" s="172"/>
+      <c r="C56" s="169" t="s">
         <v>37</v>
       </c>
       <c r="D56" s="1" t="s">
@@ -11766,8 +11725,8 @@
       </c>
     </row>
     <row r="57" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B57" s="170"/>
-      <c r="C57" s="172"/>
+      <c r="B57" s="172"/>
+      <c r="C57" s="169"/>
       <c r="E57" s="77" t="s">
         <v>263</v>
       </c>
@@ -11796,8 +11755,8 @@
       <c r="R57" s="36"/>
     </row>
     <row r="58" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B58" s="170"/>
-      <c r="C58" s="172" t="s">
+      <c r="B58" s="172"/>
+      <c r="C58" s="169" t="s">
         <v>36</v>
       </c>
       <c r="D58" s="1" t="s">
@@ -11847,8 +11806,8 @@
       </c>
     </row>
     <row r="59" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B59" s="170"/>
-      <c r="C59" s="172"/>
+      <c r="B59" s="172"/>
+      <c r="C59" s="169"/>
       <c r="E59" s="77" t="s">
         <v>263</v>
       </c>
@@ -11877,8 +11836,8 @@
       <c r="R59" s="36"/>
     </row>
     <row r="60" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B60" s="170"/>
-      <c r="C60" s="172" t="s">
+      <c r="B60" s="172"/>
+      <c r="C60" s="169" t="s">
         <v>12</v>
       </c>
       <c r="D60" s="1" t="s">
@@ -11928,8 +11887,8 @@
       </c>
     </row>
     <row r="61" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B61" s="170"/>
-      <c r="C61" s="172"/>
+      <c r="B61" s="172"/>
+      <c r="C61" s="169"/>
       <c r="E61" s="77" t="s">
         <v>263</v>
       </c>
@@ -11958,7 +11917,7 @@
       <c r="R61" s="36"/>
     </row>
     <row r="62" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B62" s="170"/>
+      <c r="B62" s="172"/>
       <c r="C62" s="85" t="s">
         <v>19</v>
       </c>
@@ -11983,8 +11942,8 @@
       <c r="R62" s="36"/>
     </row>
     <row r="63" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B63" s="170"/>
-      <c r="C63" s="172" t="s">
+      <c r="B63" s="172"/>
+      <c r="C63" s="169" t="s">
         <v>13</v>
       </c>
       <c r="D63" s="1" t="s">
@@ -12034,8 +11993,8 @@
       </c>
     </row>
     <row r="64" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B64" s="170"/>
-      <c r="C64" s="172"/>
+      <c r="B64" s="172"/>
+      <c r="C64" s="169"/>
       <c r="E64" s="77" t="s">
         <v>263</v>
       </c>
@@ -12064,8 +12023,8 @@
       <c r="R64" s="36"/>
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B65" s="170"/>
-      <c r="C65" s="172" t="s">
+      <c r="B65" s="172"/>
+      <c r="C65" s="169" t="s">
         <v>14</v>
       </c>
       <c r="D65" s="1" t="s">
@@ -12115,8 +12074,8 @@
       </c>
     </row>
     <row r="66" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B66" s="170"/>
-      <c r="C66" s="172"/>
+      <c r="B66" s="172"/>
+      <c r="C66" s="169"/>
       <c r="E66" s="77" t="s">
         <v>263</v>
       </c>
@@ -12145,8 +12104,8 @@
       <c r="R66" s="36"/>
     </row>
     <row r="67" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B67" s="170"/>
-      <c r="C67" s="172"/>
+      <c r="B67" s="172"/>
+      <c r="C67" s="169"/>
       <c r="E67" s="77" t="s">
         <v>335</v>
       </c>
@@ -12175,8 +12134,8 @@
       <c r="R67" s="36"/>
     </row>
     <row r="68" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B68" s="170"/>
-      <c r="C68" s="172"/>
+      <c r="B68" s="172"/>
+      <c r="C68" s="169"/>
       <c r="E68" s="77" t="s">
         <v>32</v>
       </c>
@@ -12205,8 +12164,8 @@
       <c r="R68" s="36"/>
     </row>
     <row r="69" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B69" s="170"/>
-      <c r="C69" s="172" t="s">
+      <c r="B69" s="172"/>
+      <c r="C69" s="169" t="s">
         <v>38</v>
       </c>
       <c r="D69" s="1" t="s">
@@ -12256,8 +12215,8 @@
       </c>
     </row>
     <row r="70" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B70" s="170"/>
-      <c r="C70" s="172"/>
+      <c r="B70" s="172"/>
+      <c r="C70" s="169"/>
       <c r="E70" s="77" t="s">
         <v>263</v>
       </c>
@@ -12286,8 +12245,8 @@
       <c r="R70" s="36"/>
     </row>
     <row r="71" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B71" s="170"/>
-      <c r="C71" s="172" t="s">
+      <c r="B71" s="172"/>
+      <c r="C71" s="169" t="s">
         <v>20</v>
       </c>
       <c r="D71" s="1" t="s">
@@ -12337,8 +12296,8 @@
       </c>
     </row>
     <row r="72" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B72" s="170"/>
-      <c r="C72" s="172"/>
+      <c r="B72" s="172"/>
+      <c r="C72" s="169"/>
       <c r="E72" s="77" t="s">
         <v>263</v>
       </c>
@@ -12367,8 +12326,8 @@
       <c r="R72" s="36"/>
     </row>
     <row r="73" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B73" s="170"/>
-      <c r="C73" s="172"/>
+      <c r="B73" s="172"/>
+      <c r="C73" s="169"/>
       <c r="E73" s="77" t="s">
         <v>335</v>
       </c>
@@ -12397,7 +12356,7 @@
       <c r="R73" s="36"/>
     </row>
     <row r="74" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B74" s="170"/>
+      <c r="B74" s="172"/>
       <c r="C74" s="85" t="s">
         <v>33</v>
       </c>
@@ -12422,7 +12381,7 @@
       <c r="R74" s="36"/>
     </row>
     <row r="75" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B75" s="170"/>
+      <c r="B75" s="172"/>
       <c r="C75" s="85" t="s">
         <v>39</v>
       </c>
@@ -12447,8 +12406,8 @@
       <c r="R75" s="36"/>
     </row>
     <row r="76" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B76" s="170"/>
-      <c r="C76" s="172" t="s">
+      <c r="B76" s="172"/>
+      <c r="C76" s="169" t="s">
         <v>41</v>
       </c>
       <c r="D76" s="1" t="s">
@@ -12498,8 +12457,8 @@
       </c>
     </row>
     <row r="77" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B77" s="170"/>
-      <c r="C77" s="172"/>
+      <c r="B77" s="172"/>
+      <c r="C77" s="169"/>
       <c r="E77" s="77" t="s">
         <v>263</v>
       </c>
@@ -12528,8 +12487,8 @@
       <c r="R77" s="36"/>
     </row>
     <row r="78" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B78" s="170"/>
-      <c r="C78" s="172" t="s">
+      <c r="B78" s="172"/>
+      <c r="C78" s="169" t="s">
         <v>42</v>
       </c>
       <c r="D78" s="1" t="s">
@@ -12579,8 +12538,8 @@
       </c>
     </row>
     <row r="79" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B79" s="170"/>
-      <c r="C79" s="172"/>
+      <c r="B79" s="172"/>
+      <c r="C79" s="169"/>
       <c r="E79" s="77" t="s">
         <v>263</v>
       </c>
@@ -12609,8 +12568,8 @@
       <c r="R79" s="36"/>
     </row>
     <row r="80" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B80" s="170"/>
-      <c r="C80" s="172" t="s">
+      <c r="B80" s="172"/>
+      <c r="C80" s="169" t="s">
         <v>15</v>
       </c>
       <c r="D80" s="1" t="s">
@@ -12661,7 +12620,7 @@
     </row>
     <row r="81" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B81" s="64"/>
-      <c r="C81" s="173"/>
+      <c r="C81" s="170"/>
       <c r="E81" s="77" t="s">
         <v>263</v>
       </c>
@@ -12690,7 +12649,7 @@
       <c r="R81" s="36"/>
     </row>
     <row r="82" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B82" s="169" t="s">
+      <c r="B82" s="171" t="s">
         <v>81</v>
       </c>
       <c r="C82" s="85" t="s">
@@ -12717,8 +12676,8 @@
       <c r="R82" s="36"/>
     </row>
     <row r="83" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B83" s="170"/>
-      <c r="C83" s="172" t="s">
+      <c r="B83" s="172"/>
+      <c r="C83" s="169" t="s">
         <v>16</v>
       </c>
       <c r="D83" s="1" t="s">
@@ -12766,8 +12725,8 @@
       </c>
     </row>
     <row r="84" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B84" s="170"/>
-      <c r="C84" s="172"/>
+      <c r="B84" s="172"/>
+      <c r="C84" s="169"/>
       <c r="E84" s="77" t="s">
         <v>263</v>
       </c>
@@ -12794,8 +12753,8 @@
       <c r="R84" s="36"/>
     </row>
     <row r="85" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B85" s="170"/>
-      <c r="C85" s="172"/>
+      <c r="B85" s="172"/>
+      <c r="C85" s="169"/>
       <c r="E85" s="77" t="s">
         <v>335</v>
       </c>
@@ -12822,8 +12781,8 @@
       <c r="R85" s="36"/>
     </row>
     <row r="86" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B86" s="170"/>
-      <c r="C86" s="172" t="s">
+      <c r="B86" s="172"/>
+      <c r="C86" s="169" t="s">
         <v>17</v>
       </c>
       <c r="D86" s="1" t="s">
@@ -12871,8 +12830,8 @@
       </c>
     </row>
     <row r="87" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B87" s="170"/>
-      <c r="C87" s="172"/>
+      <c r="B87" s="172"/>
+      <c r="C87" s="169"/>
       <c r="E87" s="77" t="s">
         <v>263</v>
       </c>
@@ -12899,8 +12858,8 @@
       <c r="R87" s="36"/>
     </row>
     <row r="88" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B88" s="170"/>
-      <c r="C88" s="172"/>
+      <c r="B88" s="172"/>
+      <c r="C88" s="169"/>
       <c r="E88" s="77" t="s">
         <v>335</v>
       </c>
@@ -12927,8 +12886,8 @@
       <c r="R88" s="36"/>
     </row>
     <row r="89" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B89" s="170"/>
-      <c r="C89" s="172"/>
+      <c r="B89" s="172"/>
+      <c r="C89" s="169"/>
       <c r="E89" s="77" t="s">
         <v>32</v>
       </c>
@@ -12955,8 +12914,8 @@
       <c r="R89" s="36"/>
     </row>
     <row r="90" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B90" s="170"/>
-      <c r="C90" s="172" t="s">
+      <c r="B90" s="172"/>
+      <c r="C90" s="169" t="s">
         <v>34</v>
       </c>
       <c r="D90" s="1" t="s">
@@ -13006,8 +12965,8 @@
       </c>
     </row>
     <row r="91" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B91" s="170"/>
-      <c r="C91" s="172"/>
+      <c r="B91" s="172"/>
+      <c r="C91" s="169"/>
       <c r="E91" s="77" t="s">
         <v>263</v>
       </c>
@@ -13036,8 +12995,8 @@
       <c r="R91" s="36"/>
     </row>
     <row r="92" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B92" s="170"/>
-      <c r="C92" s="172"/>
+      <c r="B92" s="172"/>
+      <c r="C92" s="169"/>
       <c r="E92" s="77" t="s">
         <v>335</v>
       </c>
@@ -13066,7 +13025,7 @@
       <c r="R92" s="36"/>
     </row>
     <row r="93" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B93" s="170"/>
+      <c r="B93" s="172"/>
       <c r="C93" s="85" t="s">
         <v>35</v>
       </c>
@@ -13091,8 +13050,8 @@
       <c r="R93" s="36"/>
     </row>
     <row r="94" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B94" s="170"/>
-      <c r="C94" s="172" t="s">
+      <c r="B94" s="172"/>
+      <c r="C94" s="169" t="s">
         <v>18</v>
       </c>
       <c r="D94" s="1" t="s">
@@ -13142,8 +13101,8 @@
       </c>
     </row>
     <row r="95" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B95" s="170"/>
-      <c r="C95" s="172"/>
+      <c r="B95" s="172"/>
+      <c r="C95" s="169"/>
       <c r="E95" s="77" t="s">
         <v>263</v>
       </c>
@@ -13172,8 +13131,8 @@
       <c r="R95" s="36"/>
     </row>
     <row r="96" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B96" s="170"/>
-      <c r="C96" s="172"/>
+      <c r="B96" s="172"/>
+      <c r="C96" s="169"/>
       <c r="E96" s="77" t="s">
         <v>335</v>
       </c>
@@ -13202,8 +13161,8 @@
       <c r="R96" s="36"/>
     </row>
     <row r="97" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B97" s="170"/>
-      <c r="C97" s="172"/>
+      <c r="B97" s="172"/>
+      <c r="C97" s="169"/>
       <c r="E97" s="77" t="s">
         <v>32</v>
       </c>
@@ -13232,8 +13191,8 @@
       <c r="R97" s="36"/>
     </row>
     <row r="98" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B98" s="170"/>
-      <c r="C98" s="172" t="s">
+      <c r="B98" s="172"/>
+      <c r="C98" s="169" t="s">
         <v>37</v>
       </c>
       <c r="D98" s="1" t="s">
@@ -13281,8 +13240,8 @@
       </c>
     </row>
     <row r="99" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B99" s="170"/>
-      <c r="C99" s="172"/>
+      <c r="B99" s="172"/>
+      <c r="C99" s="169"/>
       <c r="E99" s="77" t="s">
         <v>263</v>
       </c>
@@ -13309,8 +13268,8 @@
       <c r="R99" s="36"/>
     </row>
     <row r="100" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B100" s="170"/>
-      <c r="C100" s="172"/>
+      <c r="B100" s="172"/>
+      <c r="C100" s="169"/>
       <c r="E100" s="77" t="s">
         <v>335</v>
       </c>
@@ -13337,8 +13296,8 @@
       <c r="R100" s="36"/>
     </row>
     <row r="101" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B101" s="170"/>
-      <c r="C101" s="172" t="s">
+      <c r="B101" s="172"/>
+      <c r="C101" s="169" t="s">
         <v>36</v>
       </c>
       <c r="D101" s="1" t="s">
@@ -13388,8 +13347,8 @@
       </c>
     </row>
     <row r="102" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B102" s="170"/>
-      <c r="C102" s="172"/>
+      <c r="B102" s="172"/>
+      <c r="C102" s="169"/>
       <c r="E102" s="77" t="s">
         <v>263</v>
       </c>
@@ -13418,8 +13377,8 @@
       <c r="R102" s="36"/>
     </row>
     <row r="103" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B103" s="170"/>
-      <c r="C103" s="172" t="s">
+      <c r="B103" s="172"/>
+      <c r="C103" s="169" t="s">
         <v>12</v>
       </c>
       <c r="D103" s="1" t="s">
@@ -13467,8 +13426,8 @@
       </c>
     </row>
     <row r="104" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B104" s="170"/>
-      <c r="C104" s="172"/>
+      <c r="B104" s="172"/>
+      <c r="C104" s="169"/>
       <c r="E104" s="77" t="s">
         <v>263</v>
       </c>
@@ -13495,8 +13454,8 @@
       <c r="R104" s="36"/>
     </row>
     <row r="105" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B105" s="170"/>
-      <c r="C105" s="172"/>
+      <c r="B105" s="172"/>
+      <c r="C105" s="169"/>
       <c r="E105" s="77" t="s">
         <v>335</v>
       </c>
@@ -13523,8 +13482,8 @@
       <c r="R105" s="36"/>
     </row>
     <row r="106" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B106" s="170"/>
-      <c r="C106" s="172" t="s">
+      <c r="B106" s="172"/>
+      <c r="C106" s="169" t="s">
         <v>19</v>
       </c>
       <c r="D106" s="1" t="s">
@@ -13574,8 +13533,8 @@
       </c>
     </row>
     <row r="107" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B107" s="170"/>
-      <c r="C107" s="172"/>
+      <c r="B107" s="172"/>
+      <c r="C107" s="169"/>
       <c r="E107" s="77" t="s">
         <v>263</v>
       </c>
@@ -13604,8 +13563,8 @@
       <c r="R107" s="36"/>
     </row>
     <row r="108" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B108" s="170"/>
-      <c r="C108" s="172"/>
+      <c r="B108" s="172"/>
+      <c r="C108" s="169"/>
       <c r="E108" s="77" t="s">
         <v>32</v>
       </c>
@@ -13634,8 +13593,8 @@
       <c r="R108" s="36"/>
     </row>
     <row r="109" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B109" s="170"/>
-      <c r="C109" s="172" t="s">
+      <c r="B109" s="172"/>
+      <c r="C109" s="169" t="s">
         <v>13</v>
       </c>
       <c r="D109" s="1" t="s">
@@ -13683,8 +13642,8 @@
       </c>
     </row>
     <row r="110" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B110" s="170"/>
-      <c r="C110" s="172"/>
+      <c r="B110" s="172"/>
+      <c r="C110" s="169"/>
       <c r="E110" s="77" t="s">
         <v>263</v>
       </c>
@@ -13711,8 +13670,8 @@
       <c r="R110" s="36"/>
     </row>
     <row r="111" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B111" s="170"/>
-      <c r="C111" s="172"/>
+      <c r="B111" s="172"/>
+      <c r="C111" s="169"/>
       <c r="E111" s="77" t="s">
         <v>335</v>
       </c>
@@ -13739,8 +13698,8 @@
       <c r="R111" s="36"/>
     </row>
     <row r="112" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B112" s="170"/>
-      <c r="C112" s="172" t="s">
+      <c r="B112" s="172"/>
+      <c r="C112" s="169" t="s">
         <v>14</v>
       </c>
       <c r="D112" s="1" t="s">
@@ -13788,8 +13747,8 @@
       </c>
     </row>
     <row r="113" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B113" s="170"/>
-      <c r="C113" s="172"/>
+      <c r="B113" s="172"/>
+      <c r="C113" s="169"/>
       <c r="E113" s="77" t="s">
         <v>263</v>
       </c>
@@ -13816,8 +13775,8 @@
       <c r="R113" s="36"/>
     </row>
     <row r="114" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B114" s="170"/>
-      <c r="C114" s="172"/>
+      <c r="B114" s="172"/>
+      <c r="C114" s="169"/>
       <c r="E114" s="77" t="s">
         <v>335</v>
       </c>
@@ -13844,8 +13803,8 @@
       <c r="R114" s="36"/>
     </row>
     <row r="115" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B115" s="170"/>
-      <c r="C115" s="172" t="s">
+      <c r="B115" s="172"/>
+      <c r="C115" s="169" t="s">
         <v>38</v>
       </c>
       <c r="D115" s="1" t="s">
@@ -13893,8 +13852,8 @@
       </c>
     </row>
     <row r="116" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B116" s="170"/>
-      <c r="C116" s="172"/>
+      <c r="B116" s="172"/>
+      <c r="C116" s="169"/>
       <c r="E116" s="77" t="s">
         <v>263</v>
       </c>
@@ -13921,8 +13880,8 @@
       <c r="R116" s="36"/>
     </row>
     <row r="117" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B117" s="170"/>
-      <c r="C117" s="172" t="s">
+      <c r="B117" s="172"/>
+      <c r="C117" s="169" t="s">
         <v>20</v>
       </c>
       <c r="D117" s="1" t="s">
@@ -13972,8 +13931,8 @@
       </c>
     </row>
     <row r="118" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B118" s="170"/>
-      <c r="C118" s="172"/>
+      <c r="B118" s="172"/>
+      <c r="C118" s="169"/>
       <c r="E118" s="77" t="s">
         <v>263</v>
       </c>
@@ -14002,8 +13961,8 @@
       <c r="R118" s="36"/>
     </row>
     <row r="119" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B119" s="170"/>
-      <c r="C119" s="172"/>
+      <c r="B119" s="172"/>
+      <c r="C119" s="169"/>
       <c r="E119" s="77" t="s">
         <v>335</v>
       </c>
@@ -14032,8 +13991,8 @@
       <c r="R119" s="36"/>
     </row>
     <row r="120" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B120" s="170"/>
-      <c r="C120" s="172" t="s">
+      <c r="B120" s="172"/>
+      <c r="C120" s="169" t="s">
         <v>33</v>
       </c>
       <c r="D120" s="1" t="s">
@@ -14081,8 +14040,8 @@
       </c>
     </row>
     <row r="121" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B121" s="170"/>
-      <c r="C121" s="172"/>
+      <c r="B121" s="172"/>
+      <c r="C121" s="169"/>
       <c r="E121" s="77" t="s">
         <v>263</v>
       </c>
@@ -14109,8 +14068,8 @@
       <c r="R121" s="36"/>
     </row>
     <row r="122" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B122" s="170"/>
-      <c r="C122" s="172"/>
+      <c r="B122" s="172"/>
+      <c r="C122" s="169"/>
       <c r="E122" s="77" t="s">
         <v>335</v>
       </c>
@@ -14137,8 +14096,8 @@
       <c r="R122" s="36"/>
     </row>
     <row r="123" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B123" s="170"/>
-      <c r="C123" s="172" t="s">
+      <c r="B123" s="172"/>
+      <c r="C123" s="169" t="s">
         <v>39</v>
       </c>
       <c r="D123" s="1" t="s">
@@ -14186,8 +14145,8 @@
       </c>
     </row>
     <row r="124" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B124" s="170"/>
-      <c r="C124" s="172"/>
+      <c r="B124" s="172"/>
+      <c r="C124" s="169"/>
       <c r="E124" s="77" t="s">
         <v>263</v>
       </c>
@@ -14214,8 +14173,8 @@
       <c r="R124" s="36"/>
     </row>
     <row r="125" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B125" s="170"/>
-      <c r="C125" s="172" t="s">
+      <c r="B125" s="172"/>
+      <c r="C125" s="169" t="s">
         <v>41</v>
       </c>
       <c r="D125" s="1" t="s">
@@ -14263,8 +14222,8 @@
       </c>
     </row>
     <row r="126" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B126" s="170"/>
-      <c r="C126" s="172"/>
+      <c r="B126" s="172"/>
+      <c r="C126" s="169"/>
       <c r="E126" s="77" t="s">
         <v>263</v>
       </c>
@@ -14291,8 +14250,8 @@
       <c r="R126" s="36"/>
     </row>
     <row r="127" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B127" s="170"/>
-      <c r="C127" s="172" t="s">
+      <c r="B127" s="172"/>
+      <c r="C127" s="169" t="s">
         <v>42</v>
       </c>
       <c r="D127" s="1" t="s">
@@ -14342,8 +14301,8 @@
       </c>
     </row>
     <row r="128" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B128" s="170"/>
-      <c r="C128" s="172"/>
+      <c r="B128" s="172"/>
+      <c r="C128" s="169"/>
       <c r="E128" s="77" t="s">
         <v>263</v>
       </c>
@@ -14372,8 +14331,8 @@
       <c r="R128" s="36"/>
     </row>
     <row r="129" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B129" s="170"/>
-      <c r="C129" s="172" t="s">
+      <c r="B129" s="172"/>
+      <c r="C129" s="169" t="s">
         <v>15</v>
       </c>
       <c r="D129" s="1" t="s">
@@ -14424,7 +14383,7 @@
     </row>
     <row r="130" spans="2:18" x14ac:dyDescent="0.2">
       <c r="B130" s="63"/>
-      <c r="C130" s="173"/>
+      <c r="C130" s="170"/>
       <c r="E130" s="77" t="s">
         <v>263</v>
       </c>
@@ -14453,7 +14412,7 @@
       <c r="R130" s="36"/>
     </row>
     <row r="131" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B131" s="169" t="s">
+      <c r="B131" s="171" t="s">
         <v>82</v>
       </c>
       <c r="C131" s="174" t="s">
@@ -14504,8 +14463,8 @@
       </c>
     </row>
     <row r="132" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B132" s="170"/>
-      <c r="C132" s="172"/>
+      <c r="B132" s="172"/>
+      <c r="C132" s="169"/>
       <c r="E132" s="77" t="s">
         <v>263</v>
       </c>
@@ -14532,8 +14491,8 @@
       <c r="R132" s="36"/>
     </row>
     <row r="133" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B133" s="170"/>
-      <c r="C133" s="172" t="s">
+      <c r="B133" s="172"/>
+      <c r="C133" s="169" t="s">
         <v>16</v>
       </c>
       <c r="D133" s="1" t="s">
@@ -14581,8 +14540,8 @@
       </c>
     </row>
     <row r="134" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B134" s="170"/>
-      <c r="C134" s="172"/>
+      <c r="B134" s="172"/>
+      <c r="C134" s="169"/>
       <c r="E134" s="77" t="s">
         <v>32</v>
       </c>
@@ -14611,8 +14570,8 @@
       <c r="R134" s="36"/>
     </row>
     <row r="135" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B135" s="170"/>
-      <c r="C135" s="172" t="s">
+      <c r="B135" s="172"/>
+      <c r="C135" s="169" t="s">
         <v>17</v>
       </c>
       <c r="D135" s="1" t="s">
@@ -14662,8 +14621,8 @@
       </c>
     </row>
     <row r="136" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B136" s="170"/>
-      <c r="C136" s="172"/>
+      <c r="B136" s="172"/>
+      <c r="C136" s="169"/>
       <c r="E136" s="77" t="s">
         <v>263</v>
       </c>
@@ -14692,8 +14651,8 @@
       <c r="R136" s="36"/>
     </row>
     <row r="137" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B137" s="170"/>
-      <c r="C137" s="172"/>
+      <c r="B137" s="172"/>
+      <c r="C137" s="169"/>
       <c r="E137" s="77" t="s">
         <v>32</v>
       </c>
@@ -14722,8 +14681,8 @@
       <c r="R137" s="36"/>
     </row>
     <row r="138" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B138" s="170"/>
-      <c r="C138" s="172" t="s">
+      <c r="B138" s="172"/>
+      <c r="C138" s="169" t="s">
         <v>34</v>
       </c>
       <c r="D138" s="1" t="s">
@@ -14773,8 +14732,8 @@
       </c>
     </row>
     <row r="139" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B139" s="170"/>
-      <c r="C139" s="172"/>
+      <c r="B139" s="172"/>
+      <c r="C139" s="169"/>
       <c r="E139" s="77" t="s">
         <v>263</v>
       </c>
@@ -14803,8 +14762,8 @@
       <c r="R139" s="36"/>
     </row>
     <row r="140" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B140" s="170"/>
-      <c r="C140" s="172"/>
+      <c r="B140" s="172"/>
+      <c r="C140" s="169"/>
       <c r="E140" s="77" t="s">
         <v>32</v>
       </c>
@@ -14833,8 +14792,8 @@
       <c r="R140" s="36"/>
     </row>
     <row r="141" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B141" s="170"/>
-      <c r="C141" s="172" t="s">
+      <c r="B141" s="172"/>
+      <c r="C141" s="169" t="s">
         <v>35</v>
       </c>
       <c r="D141" s="1" t="s">
@@ -14880,8 +14839,8 @@
       </c>
     </row>
     <row r="142" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B142" s="170"/>
-      <c r="C142" s="172"/>
+      <c r="B142" s="172"/>
+      <c r="C142" s="169"/>
       <c r="E142" s="77" t="s">
         <v>32</v>
       </c>
@@ -14908,8 +14867,8 @@
       <c r="R142" s="36"/>
     </row>
     <row r="143" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B143" s="170"/>
-      <c r="C143" s="172"/>
+      <c r="B143" s="172"/>
+      <c r="C143" s="169"/>
       <c r="E143" s="77" t="s">
         <v>335</v>
       </c>
@@ -14936,8 +14895,8 @@
       <c r="R143" s="36"/>
     </row>
     <row r="144" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B144" s="170"/>
-      <c r="C144" s="172" t="s">
+      <c r="B144" s="172"/>
+      <c r="C144" s="169" t="s">
         <v>18</v>
       </c>
       <c r="D144" s="1" t="s">
@@ -14985,8 +14944,8 @@
       </c>
     </row>
     <row r="145" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B145" s="170"/>
-      <c r="C145" s="172"/>
+      <c r="B145" s="172"/>
+      <c r="C145" s="169"/>
       <c r="E145" s="77" t="s">
         <v>32</v>
       </c>
@@ -15015,10 +14974,10 @@
       <c r="R145" s="36"/>
     </row>
     <row r="146" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B146" s="170"/>
-      <c r="C146" s="172"/>
+      <c r="B146" s="172"/>
+      <c r="C146" s="169"/>
       <c r="E146" s="77" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="F146" s="36">
         <v>-3.074E-2</v>
@@ -15045,8 +15004,8 @@
       <c r="R146" s="36"/>
     </row>
     <row r="147" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B147" s="170"/>
-      <c r="C147" s="172" t="s">
+      <c r="B147" s="172"/>
+      <c r="C147" s="169" t="s">
         <v>37</v>
       </c>
       <c r="D147" s="1" t="s">
@@ -15096,8 +15055,8 @@
       </c>
     </row>
     <row r="148" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B148" s="170"/>
-      <c r="C148" s="172"/>
+      <c r="B148" s="172"/>
+      <c r="C148" s="169"/>
       <c r="E148" s="77" t="s">
         <v>263</v>
       </c>
@@ -15126,8 +15085,8 @@
       <c r="R148" s="36"/>
     </row>
     <row r="149" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B149" s="170"/>
-      <c r="C149" s="172"/>
+      <c r="B149" s="172"/>
+      <c r="C149" s="169"/>
       <c r="E149" s="77" t="s">
         <v>32</v>
       </c>
@@ -15156,8 +15115,8 @@
       <c r="R149" s="36"/>
     </row>
     <row r="150" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B150" s="170"/>
-      <c r="C150" s="172" t="s">
+      <c r="B150" s="172"/>
+      <c r="C150" s="169" t="s">
         <v>36</v>
       </c>
       <c r="D150" s="1" t="s">
@@ -15207,8 +15166,8 @@
       </c>
     </row>
     <row r="151" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B151" s="170"/>
-      <c r="C151" s="172"/>
+      <c r="B151" s="172"/>
+      <c r="C151" s="169"/>
       <c r="E151" s="77" t="s">
         <v>263</v>
       </c>
@@ -15237,8 +15196,8 @@
       <c r="R151" s="36"/>
     </row>
     <row r="152" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B152" s="170"/>
-      <c r="C152" s="172"/>
+      <c r="B152" s="172"/>
+      <c r="C152" s="169"/>
       <c r="E152" s="77" t="s">
         <v>32</v>
       </c>
@@ -15267,10 +15226,10 @@
       <c r="R152" s="36"/>
     </row>
     <row r="153" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B153" s="170"/>
-      <c r="C153" s="172"/>
+      <c r="B153" s="172"/>
+      <c r="C153" s="169"/>
       <c r="E153" s="77" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="F153" s="36">
         <v>-1.6080000000000001E-2</v>
@@ -15297,8 +15256,8 @@
       <c r="R153" s="36"/>
     </row>
     <row r="154" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B154" s="170"/>
-      <c r="C154" s="172" t="s">
+      <c r="B154" s="172"/>
+      <c r="C154" s="169" t="s">
         <v>12</v>
       </c>
       <c r="D154" s="1" t="s">
@@ -15348,8 +15307,8 @@
       </c>
     </row>
     <row r="155" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B155" s="170"/>
-      <c r="C155" s="172"/>
+      <c r="B155" s="172"/>
+      <c r="C155" s="169"/>
       <c r="E155" s="1" t="s">
         <v>263</v>
       </c>
@@ -15378,7 +15337,7 @@
       <c r="R155" s="36"/>
     </row>
     <row r="156" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B156" s="170"/>
+      <c r="B156" s="172"/>
       <c r="C156" s="85"/>
       <c r="E156" s="1" t="s">
         <v>335</v>
@@ -15408,7 +15367,7 @@
       <c r="R156" s="36"/>
     </row>
     <row r="157" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B157" s="170"/>
+      <c r="B157" s="172"/>
       <c r="C157" s="85"/>
       <c r="E157" s="1" t="s">
         <v>32</v>
@@ -15438,10 +15397,10 @@
       <c r="R157" s="36"/>
     </row>
     <row r="158" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B158" s="170"/>
+      <c r="B158" s="172"/>
       <c r="C158" s="85"/>
       <c r="E158" s="1" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F158" s="36">
         <v>0.41599000000000003</v>
@@ -15468,8 +15427,8 @@
       <c r="R158" s="36"/>
     </row>
     <row r="159" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B159" s="170"/>
-      <c r="C159" s="172" t="s">
+      <c r="B159" s="172"/>
+      <c r="C159" s="169" t="s">
         <v>19</v>
       </c>
       <c r="D159" s="1" t="s">
@@ -15519,8 +15478,8 @@
       </c>
     </row>
     <row r="160" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B160" s="170"/>
-      <c r="C160" s="172"/>
+      <c r="B160" s="172"/>
+      <c r="C160" s="169"/>
       <c r="E160" s="77" t="s">
         <v>263</v>
       </c>
@@ -15549,8 +15508,8 @@
       <c r="R160" s="36"/>
     </row>
     <row r="161" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B161" s="170"/>
-      <c r="C161" s="172" t="s">
+      <c r="B161" s="172"/>
+      <c r="C161" s="169" t="s">
         <v>13</v>
       </c>
       <c r="D161" s="1" t="s">
@@ -15600,8 +15559,8 @@
       </c>
     </row>
     <row r="162" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B162" s="170"/>
-      <c r="C162" s="172"/>
+      <c r="B162" s="172"/>
+      <c r="C162" s="169"/>
       <c r="E162" s="77" t="s">
         <v>263</v>
       </c>
@@ -15630,8 +15589,8 @@
       <c r="R162" s="36"/>
     </row>
     <row r="163" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B163" s="170"/>
-      <c r="C163" s="172"/>
+      <c r="B163" s="172"/>
+      <c r="C163" s="169"/>
       <c r="E163" s="77" t="s">
         <v>32</v>
       </c>
@@ -15660,8 +15619,8 @@
       <c r="R163" s="36"/>
     </row>
     <row r="164" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B164" s="170"/>
-      <c r="C164" s="172" t="s">
+      <c r="B164" s="172"/>
+      <c r="C164" s="169" t="s">
         <v>14</v>
       </c>
       <c r="D164" s="1" t="s">
@@ -15686,7 +15645,7 @@
         <v>7.9399999999999991E-3</v>
       </c>
       <c r="K164" s="88" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L164" s="36">
         <v>1039.6247578713901</v>
@@ -15711,8 +15670,8 @@
       </c>
     </row>
     <row r="165" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B165" s="170"/>
-      <c r="C165" s="172"/>
+      <c r="B165" s="172"/>
+      <c r="C165" s="169"/>
       <c r="E165" s="77" t="s">
         <v>263</v>
       </c>
@@ -15741,8 +15700,8 @@
       <c r="R165" s="36"/>
     </row>
     <row r="166" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B166" s="170"/>
-      <c r="C166" s="172"/>
+      <c r="B166" s="172"/>
+      <c r="C166" s="169"/>
       <c r="E166" s="77" t="s">
         <v>32</v>
       </c>
@@ -15771,8 +15730,8 @@
       <c r="R166" s="36"/>
     </row>
     <row r="167" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B167" s="170"/>
-      <c r="C167" s="172"/>
+      <c r="B167" s="172"/>
+      <c r="C167" s="169"/>
       <c r="E167" s="77" t="s">
         <v>392</v>
       </c>
@@ -15801,8 +15760,8 @@
       <c r="R167" s="36"/>
     </row>
     <row r="168" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B168" s="170"/>
-      <c r="C168" s="172"/>
+      <c r="B168" s="172"/>
+      <c r="C168" s="169"/>
       <c r="E168" s="77" t="s">
         <v>393</v>
       </c>
@@ -15831,8 +15790,8 @@
       <c r="R168" s="36"/>
     </row>
     <row r="169" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B169" s="170"/>
-      <c r="C169" s="172"/>
+      <c r="B169" s="172"/>
+      <c r="C169" s="169"/>
       <c r="E169" s="77" t="s">
         <v>394</v>
       </c>
@@ -15861,8 +15820,8 @@
       <c r="R169" s="36"/>
     </row>
     <row r="170" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B170" s="170"/>
-      <c r="C170" s="172"/>
+      <c r="B170" s="172"/>
+      <c r="C170" s="169"/>
       <c r="E170" s="77" t="s">
         <v>395</v>
       </c>
@@ -15891,8 +15850,8 @@
       <c r="R170" s="36"/>
     </row>
     <row r="171" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B171" s="170"/>
-      <c r="C171" s="172"/>
+      <c r="B171" s="172"/>
+      <c r="C171" s="169"/>
       <c r="E171" s="77" t="s">
         <v>396</v>
       </c>
@@ -15921,8 +15880,8 @@
       <c r="R171" s="36"/>
     </row>
     <row r="172" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B172" s="170"/>
-      <c r="C172" s="172" t="s">
+      <c r="B172" s="172"/>
+      <c r="C172" s="169" t="s">
         <v>38</v>
       </c>
       <c r="D172" s="1" t="s">
@@ -15972,8 +15931,8 @@
       </c>
     </row>
     <row r="173" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B173" s="170"/>
-      <c r="C173" s="172"/>
+      <c r="B173" s="172"/>
+      <c r="C173" s="169"/>
       <c r="E173" s="77" t="s">
         <v>263</v>
       </c>
@@ -16002,8 +15961,8 @@
       <c r="R173" s="36"/>
     </row>
     <row r="174" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B174" s="170"/>
-      <c r="C174" s="172"/>
+      <c r="B174" s="172"/>
+      <c r="C174" s="169"/>
       <c r="E174" s="77" t="s">
         <v>32</v>
       </c>
@@ -16032,8 +15991,8 @@
       <c r="R174" s="36"/>
     </row>
     <row r="175" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B175" s="170"/>
-      <c r="C175" s="172" t="s">
+      <c r="B175" s="172"/>
+      <c r="C175" s="169" t="s">
         <v>20</v>
       </c>
       <c r="D175" s="1" t="s">
@@ -16083,8 +16042,8 @@
       </c>
     </row>
     <row r="176" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B176" s="170"/>
-      <c r="C176" s="172"/>
+      <c r="B176" s="172"/>
+      <c r="C176" s="169"/>
       <c r="E176" s="77" t="s">
         <v>263</v>
       </c>
@@ -16113,8 +16072,8 @@
       <c r="R176" s="36"/>
     </row>
     <row r="177" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B177" s="170"/>
-      <c r="C177" s="172"/>
+      <c r="B177" s="172"/>
+      <c r="C177" s="169"/>
       <c r="E177" s="77" t="s">
         <v>32</v>
       </c>
@@ -16143,8 +16102,8 @@
       <c r="R177" s="36"/>
     </row>
     <row r="178" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B178" s="170"/>
-      <c r="C178" s="172"/>
+      <c r="B178" s="172"/>
+      <c r="C178" s="169"/>
       <c r="E178" s="77" t="s">
         <v>335</v>
       </c>
@@ -16173,8 +16132,8 @@
       <c r="R178" s="36"/>
     </row>
     <row r="179" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B179" s="170"/>
-      <c r="C179" s="172" t="s">
+      <c r="B179" s="172"/>
+      <c r="C179" s="169" t="s">
         <v>33</v>
       </c>
       <c r="D179" s="1" t="s">
@@ -16199,7 +16158,7 @@
         <v>3.3000000000000002E-9</v>
       </c>
       <c r="K179" s="88" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="L179" s="36">
         <v>243.89788410026199</v>
@@ -16224,8 +16183,8 @@
       </c>
     </row>
     <row r="180" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B180" s="170"/>
-      <c r="C180" s="172"/>
+      <c r="B180" s="172"/>
+      <c r="C180" s="169"/>
       <c r="E180" s="77" t="s">
         <v>263</v>
       </c>
@@ -16254,8 +16213,8 @@
       <c r="R180" s="36"/>
     </row>
     <row r="181" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B181" s="170"/>
-      <c r="C181" s="172"/>
+      <c r="B181" s="172"/>
+      <c r="C181" s="169"/>
       <c r="E181" s="77" t="s">
         <v>32</v>
       </c>
@@ -16284,8 +16243,8 @@
       <c r="R181" s="36"/>
     </row>
     <row r="182" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B182" s="170"/>
-      <c r="C182" s="172"/>
+      <c r="B182" s="172"/>
+      <c r="C182" s="169"/>
       <c r="E182" s="77" t="s">
         <v>392</v>
       </c>
@@ -16314,8 +16273,8 @@
       <c r="R182" s="36"/>
     </row>
     <row r="183" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B183" s="170"/>
-      <c r="C183" s="172"/>
+      <c r="B183" s="172"/>
+      <c r="C183" s="169"/>
       <c r="E183" s="77" t="s">
         <v>393</v>
       </c>
@@ -16344,8 +16303,8 @@
       <c r="R183" s="36"/>
     </row>
     <row r="184" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B184" s="170"/>
-      <c r="C184" s="172"/>
+      <c r="B184" s="172"/>
+      <c r="C184" s="169"/>
       <c r="E184" s="77" t="s">
         <v>394</v>
       </c>
@@ -16374,8 +16333,8 @@
       <c r="R184" s="36"/>
     </row>
     <row r="185" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B185" s="170"/>
-      <c r="C185" s="172"/>
+      <c r="B185" s="172"/>
+      <c r="C185" s="169"/>
       <c r="E185" s="77" t="s">
         <v>395</v>
       </c>
@@ -16404,8 +16363,8 @@
       <c r="R185" s="36"/>
     </row>
     <row r="186" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B186" s="170"/>
-      <c r="C186" s="172"/>
+      <c r="B186" s="172"/>
+      <c r="C186" s="169"/>
       <c r="E186" s="77" t="s">
         <v>396</v>
       </c>
@@ -16434,8 +16393,8 @@
       <c r="R186" s="36"/>
     </row>
     <row r="187" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B187" s="170"/>
-      <c r="C187" s="172" t="s">
+      <c r="B187" s="172"/>
+      <c r="C187" s="169" t="s">
         <v>39</v>
       </c>
       <c r="D187" s="1" t="s">
@@ -16483,8 +16442,8 @@
       </c>
     </row>
     <row r="188" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B188" s="170"/>
-      <c r="C188" s="172"/>
+      <c r="B188" s="172"/>
+      <c r="C188" s="169"/>
       <c r="E188" s="77" t="s">
         <v>263</v>
       </c>
@@ -16511,8 +16470,8 @@
       <c r="R188" s="36"/>
     </row>
     <row r="189" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B189" s="170"/>
-      <c r="C189" s="172" t="s">
+      <c r="B189" s="172"/>
+      <c r="C189" s="169" t="s">
         <v>41</v>
       </c>
       <c r="D189" s="1" t="s">
@@ -16562,8 +16521,8 @@
       </c>
     </row>
     <row r="190" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B190" s="170"/>
-      <c r="C190" s="172"/>
+      <c r="B190" s="172"/>
+      <c r="C190" s="169"/>
       <c r="E190" s="77" t="s">
         <v>263</v>
       </c>
@@ -16592,8 +16551,8 @@
       <c r="R190" s="36"/>
     </row>
     <row r="191" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B191" s="170"/>
-      <c r="C191" s="172"/>
+      <c r="B191" s="172"/>
+      <c r="C191" s="169"/>
       <c r="E191" s="77" t="s">
         <v>335</v>
       </c>
@@ -16622,8 +16581,8 @@
       <c r="R191" s="36"/>
     </row>
     <row r="192" spans="2:18" x14ac:dyDescent="0.2">
-      <c r="B192" s="170"/>
-      <c r="C192" s="172" t="s">
+      <c r="B192" s="172"/>
+      <c r="C192" s="169" t="s">
         <v>42</v>
       </c>
       <c r="D192" s="1" t="s">
@@ -16673,8 +16632,8 @@
       </c>
     </row>
     <row r="193" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B193" s="170"/>
-      <c r="C193" s="172"/>
+      <c r="B193" s="172"/>
+      <c r="C193" s="169"/>
       <c r="E193" s="77" t="s">
         <v>263</v>
       </c>
@@ -16703,8 +16662,8 @@
       <c r="R193" s="36"/>
     </row>
     <row r="194" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B194" s="170"/>
-      <c r="C194" s="172"/>
+      <c r="B194" s="172"/>
+      <c r="C194" s="169"/>
       <c r="E194" s="77" t="s">
         <v>32</v>
       </c>
@@ -16733,8 +16692,8 @@
       <c r="R194" s="36"/>
     </row>
     <row r="195" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B195" s="170"/>
-      <c r="C195" s="172"/>
+      <c r="B195" s="172"/>
+      <c r="C195" s="169"/>
       <c r="E195" s="77" t="s">
         <v>335</v>
       </c>
@@ -16763,8 +16722,8 @@
       <c r="R195" s="36"/>
     </row>
     <row r="196" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B196" s="170"/>
-      <c r="C196" s="172" t="s">
+      <c r="B196" s="172"/>
+      <c r="C196" s="169" t="s">
         <v>15</v>
       </c>
       <c r="D196" s="1" t="s">
@@ -16814,8 +16773,8 @@
       </c>
     </row>
     <row r="197" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B197" s="170"/>
-      <c r="C197" s="172"/>
+      <c r="B197" s="172"/>
+      <c r="C197" s="169"/>
       <c r="E197" s="1" t="s">
         <v>263</v>
       </c>
@@ -16844,8 +16803,8 @@
       <c r="R197" s="36"/>
     </row>
     <row r="198" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B198" s="170"/>
-      <c r="C198" s="172"/>
+      <c r="B198" s="172"/>
+      <c r="C198" s="169"/>
       <c r="E198" s="1" t="s">
         <v>335</v>
       </c>
@@ -16874,8 +16833,8 @@
       <c r="R198" s="36"/>
     </row>
     <row r="199" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B199" s="170"/>
-      <c r="C199" s="172"/>
+      <c r="B199" s="172"/>
+      <c r="C199" s="169"/>
       <c r="E199" s="1" t="s">
         <v>32</v>
       </c>
@@ -16904,11 +16863,11 @@
       <c r="R199" s="36"/>
     </row>
     <row r="200" spans="2:40" x14ac:dyDescent="0.2">
-      <c r="B200" s="171"/>
-      <c r="C200" s="173"/>
+      <c r="B200" s="173"/>
+      <c r="C200" s="170"/>
       <c r="D200" s="13"/>
       <c r="E200" s="13" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="F200" s="87">
         <v>0.17069000000000001</v>
@@ -16935,28 +16894,28 @@
       <c r="R200" s="87"/>
     </row>
     <row r="206" spans="2:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="U206" s="164" t="s">
+      <c r="U206" s="152" t="s">
         <v>349</v>
       </c>
-      <c r="V206" s="164"/>
-      <c r="W206" s="164"/>
-      <c r="X206" s="164"/>
-      <c r="Y206" s="164"/>
-      <c r="Z206" s="164"/>
-      <c r="AA206" s="164"/>
-      <c r="AB206" s="164"/>
-      <c r="AC206" s="164"/>
-      <c r="AD206" s="164"/>
-      <c r="AE206" s="164"/>
-      <c r="AF206" s="164"/>
-      <c r="AG206" s="164"/>
-      <c r="AH206" s="164"/>
-      <c r="AI206" s="164"/>
-      <c r="AJ206" s="164"/>
-      <c r="AK206" s="164"/>
-      <c r="AL206" s="164"/>
-      <c r="AM206" s="164"/>
-      <c r="AN206" s="164"/>
+      <c r="V206" s="152"/>
+      <c r="W206" s="152"/>
+      <c r="X206" s="152"/>
+      <c r="Y206" s="152"/>
+      <c r="Z206" s="152"/>
+      <c r="AA206" s="152"/>
+      <c r="AB206" s="152"/>
+      <c r="AC206" s="152"/>
+      <c r="AD206" s="152"/>
+      <c r="AE206" s="152"/>
+      <c r="AF206" s="152"/>
+      <c r="AG206" s="152"/>
+      <c r="AH206" s="152"/>
+      <c r="AI206" s="152"/>
+      <c r="AJ206" s="152"/>
+      <c r="AK206" s="152"/>
+      <c r="AL206" s="152"/>
+      <c r="AM206" s="152"/>
+      <c r="AN206" s="152"/>
     </row>
     <row r="207" spans="2:40" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="U207" s="13" t="s">
@@ -17231,28 +17190,28 @@
       <c r="AN211" s="13"/>
     </row>
     <row r="213" spans="21:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="U213" s="164" t="s">
+      <c r="U213" s="152" t="s">
         <v>350</v>
       </c>
-      <c r="V213" s="164"/>
-      <c r="W213" s="164"/>
-      <c r="X213" s="164"/>
-      <c r="Y213" s="164"/>
-      <c r="Z213" s="164"/>
-      <c r="AA213" s="164"/>
-      <c r="AB213" s="164"/>
-      <c r="AC213" s="164"/>
-      <c r="AD213" s="164"/>
-      <c r="AE213" s="164"/>
-      <c r="AF213" s="164"/>
-      <c r="AG213" s="164"/>
-      <c r="AH213" s="164"/>
-      <c r="AI213" s="164"/>
-      <c r="AJ213" s="164"/>
-      <c r="AK213" s="164"/>
-      <c r="AL213" s="164"/>
-      <c r="AM213" s="164"/>
-      <c r="AN213" s="164"/>
+      <c r="V213" s="152"/>
+      <c r="W213" s="152"/>
+      <c r="X213" s="152"/>
+      <c r="Y213" s="152"/>
+      <c r="Z213" s="152"/>
+      <c r="AA213" s="152"/>
+      <c r="AB213" s="152"/>
+      <c r="AC213" s="152"/>
+      <c r="AD213" s="152"/>
+      <c r="AE213" s="152"/>
+      <c r="AF213" s="152"/>
+      <c r="AG213" s="152"/>
+      <c r="AH213" s="152"/>
+      <c r="AI213" s="152"/>
+      <c r="AJ213" s="152"/>
+      <c r="AK213" s="152"/>
+      <c r="AL213" s="152"/>
+      <c r="AM213" s="152"/>
+      <c r="AN213" s="152"/>
     </row>
     <row r="214" spans="21:40" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="U214" s="13" t="s">
@@ -17542,28 +17501,28 @@
       </c>
     </row>
     <row r="221" spans="21:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="U221" s="164" t="s">
+      <c r="U221" s="152" t="s">
         <v>352</v>
       </c>
-      <c r="V221" s="164"/>
-      <c r="W221" s="164"/>
-      <c r="X221" s="164"/>
-      <c r="Y221" s="164"/>
-      <c r="Z221" s="164"/>
-      <c r="AA221" s="164"/>
-      <c r="AB221" s="164"/>
-      <c r="AC221" s="164"/>
-      <c r="AD221" s="164"/>
-      <c r="AE221" s="164"/>
-      <c r="AF221" s="164"/>
-      <c r="AG221" s="164"/>
-      <c r="AH221" s="164"/>
-      <c r="AI221" s="164"/>
-      <c r="AJ221" s="164"/>
-      <c r="AK221" s="164"/>
-      <c r="AL221" s="164"/>
-      <c r="AM221" s="164"/>
-      <c r="AN221" s="164"/>
+      <c r="V221" s="152"/>
+      <c r="W221" s="152"/>
+      <c r="X221" s="152"/>
+      <c r="Y221" s="152"/>
+      <c r="Z221" s="152"/>
+      <c r="AA221" s="152"/>
+      <c r="AB221" s="152"/>
+      <c r="AC221" s="152"/>
+      <c r="AD221" s="152"/>
+      <c r="AE221" s="152"/>
+      <c r="AF221" s="152"/>
+      <c r="AG221" s="152"/>
+      <c r="AH221" s="152"/>
+      <c r="AI221" s="152"/>
+      <c r="AJ221" s="152"/>
+      <c r="AK221" s="152"/>
+      <c r="AL221" s="152"/>
+      <c r="AM221" s="152"/>
+      <c r="AN221" s="152"/>
     </row>
     <row r="222" spans="21:40" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="U222" s="13" t="s">
@@ -17840,28 +17799,28 @@
       <c r="AN226" s="26"/>
     </row>
     <row r="229" spans="21:40" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="U229" s="164" t="s">
+      <c r="U229" s="152" t="s">
         <v>355</v>
       </c>
-      <c r="V229" s="164"/>
-      <c r="W229" s="164"/>
-      <c r="X229" s="164"/>
-      <c r="Y229" s="164"/>
-      <c r="Z229" s="164"/>
-      <c r="AA229" s="164"/>
-      <c r="AB229" s="164"/>
-      <c r="AC229" s="164"/>
-      <c r="AD229" s="164"/>
-      <c r="AE229" s="164"/>
-      <c r="AF229" s="164"/>
-      <c r="AG229" s="164"/>
-      <c r="AH229" s="164"/>
-      <c r="AI229" s="164"/>
-      <c r="AJ229" s="164"/>
-      <c r="AK229" s="164"/>
-      <c r="AL229" s="164"/>
-      <c r="AM229" s="164"/>
-      <c r="AN229" s="164"/>
+      <c r="V229" s="152"/>
+      <c r="W229" s="152"/>
+      <c r="X229" s="152"/>
+      <c r="Y229" s="152"/>
+      <c r="Z229" s="152"/>
+      <c r="AA229" s="152"/>
+      <c r="AB229" s="152"/>
+      <c r="AC229" s="152"/>
+      <c r="AD229" s="152"/>
+      <c r="AE229" s="152"/>
+      <c r="AF229" s="152"/>
+      <c r="AG229" s="152"/>
+      <c r="AH229" s="152"/>
+      <c r="AI229" s="152"/>
+      <c r="AJ229" s="152"/>
+      <c r="AK229" s="152"/>
+      <c r="AL229" s="152"/>
+      <c r="AM229" s="152"/>
+      <c r="AN229" s="152"/>
     </row>
     <row r="230" spans="21:40" ht="17" thickTop="1" x14ac:dyDescent="0.2">
       <c r="U230" s="13" t="s">
@@ -18255,14 +18214,14 @@
         <v>273</v>
       </c>
       <c r="AA236" s="25" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="AB236" s="1" t="s">
         <v>273</v>
       </c>
       <c r="AC236" s="25"/>
       <c r="AD236" s="25" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="AE236" s="1" t="s">
         <v>273</v>
@@ -18292,7 +18251,7 @@
         <v>273</v>
       </c>
       <c r="AN236" s="25" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
     </row>
     <row r="237" spans="21:40" s="25" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
@@ -18336,7 +18295,7 @@
         <v>343</v>
       </c>
       <c r="AL237" s="26" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="AM237" s="26"/>
       <c r="AN237" s="26" t="s">
@@ -18346,40 +18305,32 @@
   </sheetData>
   <dataConsolidate/>
   <mergeCells count="71">
-    <mergeCell ref="U229:AN229"/>
-    <mergeCell ref="C189:C191"/>
-    <mergeCell ref="C192:C195"/>
-    <mergeCell ref="C196:C200"/>
-    <mergeCell ref="U206:AN206"/>
-    <mergeCell ref="U213:AN213"/>
-    <mergeCell ref="U221:AN221"/>
-    <mergeCell ref="C161:C163"/>
-    <mergeCell ref="C164:C171"/>
-    <mergeCell ref="C172:C174"/>
-    <mergeCell ref="C175:C178"/>
-    <mergeCell ref="C179:C186"/>
-    <mergeCell ref="C187:C188"/>
-    <mergeCell ref="C141:C143"/>
-    <mergeCell ref="C144:C146"/>
-    <mergeCell ref="C147:C149"/>
-    <mergeCell ref="C150:C153"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="C159:C160"/>
-    <mergeCell ref="C120:C122"/>
-    <mergeCell ref="C123:C124"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="C127:C128"/>
-    <mergeCell ref="C129:C130"/>
-    <mergeCell ref="B131:B200"/>
-    <mergeCell ref="C131:C132"/>
-    <mergeCell ref="C133:C134"/>
-    <mergeCell ref="C135:C137"/>
-    <mergeCell ref="C138:C140"/>
-    <mergeCell ref="C103:C105"/>
-    <mergeCell ref="C106:C108"/>
-    <mergeCell ref="C109:C111"/>
-    <mergeCell ref="C112:C114"/>
-    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="B3:S3"/>
+    <mergeCell ref="B5:B35"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C19:C20"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C71:C73"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="B36:B80"/>
+    <mergeCell ref="C36:C39"/>
+    <mergeCell ref="C40:C41"/>
+    <mergeCell ref="C42:C45"/>
+    <mergeCell ref="C46:C49"/>
+    <mergeCell ref="C50:C52"/>
+    <mergeCell ref="C53:C55"/>
+    <mergeCell ref="C56:C57"/>
+    <mergeCell ref="C58:C59"/>
+    <mergeCell ref="C60:C61"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="C69:C70"/>
     <mergeCell ref="C117:C119"/>
     <mergeCell ref="C76:C77"/>
     <mergeCell ref="C78:C79"/>
@@ -18391,32 +18342,40 @@
     <mergeCell ref="C94:C97"/>
     <mergeCell ref="C98:C100"/>
     <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C73"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B36:B80"/>
-    <mergeCell ref="C36:C39"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="C42:C45"/>
-    <mergeCell ref="C46:C49"/>
-    <mergeCell ref="C50:C52"/>
-    <mergeCell ref="C53:C55"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="B3:S3"/>
-    <mergeCell ref="B5:B35"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C19:C20"/>
-    <mergeCell ref="C21:C22"/>
-    <mergeCell ref="C23:C24"/>
-    <mergeCell ref="C25:C26"/>
+    <mergeCell ref="C103:C105"/>
+    <mergeCell ref="C106:C108"/>
+    <mergeCell ref="C109:C111"/>
+    <mergeCell ref="C112:C114"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="B131:B200"/>
+    <mergeCell ref="C131:C132"/>
+    <mergeCell ref="C133:C134"/>
+    <mergeCell ref="C135:C137"/>
+    <mergeCell ref="C138:C140"/>
+    <mergeCell ref="C120:C122"/>
+    <mergeCell ref="C123:C124"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="C127:C128"/>
+    <mergeCell ref="C129:C130"/>
+    <mergeCell ref="C187:C188"/>
+    <mergeCell ref="C141:C143"/>
+    <mergeCell ref="C144:C146"/>
+    <mergeCell ref="C147:C149"/>
+    <mergeCell ref="C150:C153"/>
+    <mergeCell ref="C154:C155"/>
+    <mergeCell ref="C159:C160"/>
+    <mergeCell ref="C161:C163"/>
+    <mergeCell ref="C164:C171"/>
+    <mergeCell ref="C172:C174"/>
+    <mergeCell ref="C175:C178"/>
+    <mergeCell ref="C179:C186"/>
+    <mergeCell ref="U229:AN229"/>
+    <mergeCell ref="C189:C191"/>
+    <mergeCell ref="C192:C195"/>
+    <mergeCell ref="C196:C200"/>
+    <mergeCell ref="U206:AN206"/>
+    <mergeCell ref="U213:AN213"/>
+    <mergeCell ref="U221:AN221"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -18443,14 +18402,14 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="164" t="s">
+      <c r="B2" s="152" t="s">
         <v>86</v>
       </c>
-      <c r="C2" s="164"/>
-      <c r="D2" s="164"/>
-      <c r="E2" s="164"/>
-      <c r="F2" s="164"/>
-      <c r="G2" s="164"/>
+      <c r="C2" s="152"/>
+      <c r="D2" s="152"/>
+      <c r="E2" s="152"/>
+      <c r="F2" s="152"/>
+      <c r="G2" s="152"/>
       <c r="H2" s="54"/>
     </row>
     <row r="3" spans="2:8" ht="17" thickTop="1" x14ac:dyDescent="0.2">
@@ -18474,7 +18433,7 @@
       </c>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="157" t="s">
+      <c r="B4" s="161" t="s">
         <v>79</v>
       </c>
       <c r="C4" s="40" t="s">
@@ -18488,7 +18447,7 @@
       <c r="G4" s="40"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="158"/>
+      <c r="B5" s="162"/>
       <c r="C5" s="1" t="s">
         <v>34</v>
       </c>
@@ -18497,7 +18456,7 @@
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="158"/>
+      <c r="B6" s="162"/>
       <c r="C6" s="1" t="s">
         <v>14</v>
       </c>
@@ -18506,7 +18465,7 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="158"/>
+      <c r="B7" s="162"/>
       <c r="C7" s="1" t="s">
         <v>38</v>
       </c>
@@ -18515,7 +18474,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="159"/>
+      <c r="B8" s="154"/>
       <c r="C8" s="13" t="s">
         <v>42</v>
       </c>
@@ -18527,7 +18486,7 @@
       <c r="G8" s="13"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="157" t="s">
+      <c r="B9" s="161" t="s">
         <v>80</v>
       </c>
       <c r="C9" s="40" t="s">
@@ -18541,7 +18500,7 @@
       <c r="G9" s="40"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="158"/>
+      <c r="B10" s="162"/>
       <c r="C10" s="1" t="s">
         <v>13</v>
       </c>
@@ -18553,7 +18512,7 @@
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="158"/>
+      <c r="B11" s="162"/>
       <c r="C11" s="1" t="s">
         <v>16</v>
       </c>
@@ -18565,7 +18524,7 @@
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="158"/>
+      <c r="B12" s="162"/>
       <c r="C12" s="1" t="s">
         <v>36</v>
       </c>
@@ -18574,7 +18533,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="159"/>
+      <c r="B13" s="154"/>
       <c r="C13" s="13" t="s">
         <v>42</v>
       </c>
@@ -18586,7 +18545,7 @@
       <c r="G13" s="13"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="157" t="s">
+      <c r="B14" s="161" t="s">
         <v>81</v>
       </c>
       <c r="C14" s="41" t="s">
@@ -18602,7 +18561,7 @@
       <c r="G14" s="40"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="158"/>
+      <c r="B15" s="162"/>
       <c r="C15" s="1" t="s">
         <v>17</v>
       </c>
@@ -18614,7 +18573,7 @@
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="158"/>
+      <c r="B16" s="162"/>
       <c r="C16" s="1" t="s">
         <v>37</v>
       </c>
@@ -18629,7 +18588,7 @@
       </c>
     </row>
     <row r="17" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B17" s="158"/>
+      <c r="B17" s="162"/>
       <c r="C17" s="1" t="s">
         <v>20</v>
       </c>
@@ -18641,7 +18600,7 @@
       </c>
     </row>
     <row r="18" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B18" s="159"/>
+      <c r="B18" s="154"/>
       <c r="C18" s="13" t="s">
         <v>13</v>
       </c>
@@ -18655,7 +18614,7 @@
       <c r="G18" s="13"/>
     </row>
     <row r="19" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B19" s="158" t="s">
+      <c r="B19" s="162" t="s">
         <v>82</v>
       </c>
       <c r="C19" s="39" t="s">
@@ -18666,7 +18625,7 @@
       </c>
     </row>
     <row r="20" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B20" s="158"/>
+      <c r="B20" s="162"/>
       <c r="C20" s="1" t="s">
         <v>13</v>
       </c>
@@ -18675,7 +18634,7 @@
       </c>
     </row>
     <row r="21" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B21" s="158"/>
+      <c r="B21" s="162"/>
       <c r="C21" s="1" t="s">
         <v>34</v>
       </c>
@@ -18684,7 +18643,7 @@
       </c>
     </row>
     <row r="22" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B22" s="158"/>
+      <c r="B22" s="162"/>
       <c r="C22" s="1" t="s">
         <v>38</v>
       </c>
@@ -18693,7 +18652,7 @@
       </c>
     </row>
     <row r="23" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="B23" s="159"/>
+      <c r="B23" s="154"/>
       <c r="C23" s="13" t="s">
         <v>15</v>
       </c>
@@ -18705,18 +18664,18 @@
       <c r="G23" s="13"/>
     </row>
     <row r="30" spans="2:20" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="J30" s="164" t="s">
+      <c r="J30" s="152" t="s">
         <v>274</v>
       </c>
-      <c r="K30" s="164"/>
-      <c r="L30" s="164"/>
-      <c r="M30" s="164"/>
-      <c r="N30" s="164"/>
-      <c r="O30" s="164"/>
-      <c r="P30" s="164"/>
-      <c r="Q30" s="164"/>
-      <c r="R30" s="164"/>
-      <c r="S30" s="164"/>
+      <c r="K30" s="152"/>
+      <c r="L30" s="152"/>
+      <c r="M30" s="152"/>
+      <c r="N30" s="152"/>
+      <c r="O30" s="152"/>
+      <c r="P30" s="152"/>
+      <c r="Q30" s="152"/>
+      <c r="R30" s="152"/>
+      <c r="S30" s="152"/>
     </row>
     <row r="31" spans="2:20" ht="18" thickTop="1" x14ac:dyDescent="0.2">
       <c r="J31" s="55" t="s">
@@ -18751,7 +18710,7 @@
       </c>
     </row>
     <row r="32" spans="2:20" x14ac:dyDescent="0.2">
-      <c r="J32" s="169" t="s">
+      <c r="J32" s="171" t="s">
         <v>79</v>
       </c>
       <c r="K32" s="14" t="s">
@@ -18765,7 +18724,7 @@
       </c>
     </row>
     <row r="33" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J33" s="170"/>
+      <c r="J33" s="172"/>
       <c r="K33" s="14" t="s">
         <v>16</v>
       </c>
@@ -18774,7 +18733,7 @@
       </c>
     </row>
     <row r="34" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J34" s="170"/>
+      <c r="J34" s="172"/>
       <c r="K34" s="14" t="s">
         <v>17</v>
       </c>
@@ -18783,7 +18742,7 @@
       </c>
     </row>
     <row r="35" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J35" s="170"/>
+      <c r="J35" s="172"/>
       <c r="K35" s="14" t="s">
         <v>34</v>
       </c>
@@ -18792,7 +18751,7 @@
       </c>
     </row>
     <row r="36" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J36" s="170"/>
+      <c r="J36" s="172"/>
       <c r="K36" s="14" t="s">
         <v>35</v>
       </c>
@@ -18801,7 +18760,7 @@
       </c>
     </row>
     <row r="37" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J37" s="170"/>
+      <c r="J37" s="172"/>
       <c r="K37" s="14" t="s">
         <v>18</v>
       </c>
@@ -18813,7 +18772,7 @@
       </c>
     </row>
     <row r="38" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J38" s="170"/>
+      <c r="J38" s="172"/>
       <c r="K38" s="14" t="s">
         <v>37</v>
       </c>
@@ -18822,7 +18781,7 @@
       </c>
     </row>
     <row r="39" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J39" s="170"/>
+      <c r="J39" s="172"/>
       <c r="K39" s="14" t="s">
         <v>36</v>
       </c>
@@ -18831,7 +18790,7 @@
       </c>
     </row>
     <row r="40" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J40" s="170"/>
+      <c r="J40" s="172"/>
       <c r="K40" s="14" t="s">
         <v>12</v>
       </c>
@@ -18843,7 +18802,7 @@
       </c>
     </row>
     <row r="41" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J41" s="170"/>
+      <c r="J41" s="172"/>
       <c r="K41" s="14" t="s">
         <v>19</v>
       </c>
@@ -18855,7 +18814,7 @@
       </c>
     </row>
     <row r="42" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J42" s="170"/>
+      <c r="J42" s="172"/>
       <c r="K42" s="14" t="s">
         <v>13</v>
       </c>
@@ -18867,7 +18826,7 @@
       </c>
     </row>
     <row r="43" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J43" s="170"/>
+      <c r="J43" s="172"/>
       <c r="K43" s="14" t="s">
         <v>14</v>
       </c>
@@ -18876,7 +18835,7 @@
       </c>
     </row>
     <row r="44" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J44" s="170"/>
+      <c r="J44" s="172"/>
       <c r="K44" s="14" t="s">
         <v>38</v>
       </c>
@@ -18885,7 +18844,7 @@
       </c>
     </row>
     <row r="45" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J45" s="170"/>
+      <c r="J45" s="172"/>
       <c r="K45" s="14" t="s">
         <v>20</v>
       </c>
@@ -18897,7 +18856,7 @@
       </c>
     </row>
     <row r="46" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J46" s="170"/>
+      <c r="J46" s="172"/>
       <c r="K46" s="14" t="s">
         <v>33</v>
       </c>
@@ -18906,7 +18865,7 @@
       </c>
     </row>
     <row r="47" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J47" s="170"/>
+      <c r="J47" s="172"/>
       <c r="K47" s="14" t="s">
         <v>39</v>
       </c>
@@ -18918,7 +18877,7 @@
       </c>
     </row>
     <row r="48" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J48" s="170"/>
+      <c r="J48" s="172"/>
       <c r="K48" s="14" t="s">
         <v>41</v>
       </c>
@@ -18927,7 +18886,7 @@
       </c>
     </row>
     <row r="49" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J49" s="170"/>
+      <c r="J49" s="172"/>
       <c r="K49" s="14" t="s">
         <v>42</v>
       </c>
@@ -18936,7 +18895,7 @@
       </c>
     </row>
     <row r="50" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J50" s="170"/>
+      <c r="J50" s="172"/>
       <c r="K50" s="15" t="s">
         <v>15</v>
       </c>
@@ -18945,7 +18904,7 @@
       </c>
     </row>
     <row r="51" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J51" s="169" t="s">
+      <c r="J51" s="171" t="s">
         <v>80</v>
       </c>
       <c r="K51" s="14" t="s">
@@ -18956,7 +18915,7 @@
       </c>
     </row>
     <row r="52" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J52" s="170"/>
+      <c r="J52" s="172"/>
       <c r="K52" s="14" t="s">
         <v>16</v>
       </c>
@@ -18965,7 +18924,7 @@
       </c>
     </row>
     <row r="53" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J53" s="170"/>
+      <c r="J53" s="172"/>
       <c r="K53" s="14" t="s">
         <v>17</v>
       </c>
@@ -18974,7 +18933,7 @@
       </c>
     </row>
     <row r="54" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J54" s="170"/>
+      <c r="J54" s="172"/>
       <c r="K54" s="14" t="s">
         <v>34</v>
       </c>
@@ -18983,7 +18942,7 @@
       </c>
     </row>
     <row r="55" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J55" s="170"/>
+      <c r="J55" s="172"/>
       <c r="K55" s="14" t="s">
         <v>35</v>
       </c>
@@ -18992,7 +18951,7 @@
       </c>
     </row>
     <row r="56" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J56" s="170"/>
+      <c r="J56" s="172"/>
       <c r="K56" s="14" t="s">
         <v>18</v>
       </c>
@@ -19001,7 +18960,7 @@
       </c>
     </row>
     <row r="57" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J57" s="170"/>
+      <c r="J57" s="172"/>
       <c r="K57" s="14" t="s">
         <v>37</v>
       </c>
@@ -19013,7 +18972,7 @@
       </c>
     </row>
     <row r="58" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J58" s="170"/>
+      <c r="J58" s="172"/>
       <c r="K58" s="14" t="s">
         <v>36</v>
       </c>
@@ -19022,7 +18981,7 @@
       </c>
     </row>
     <row r="59" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J59" s="170"/>
+      <c r="J59" s="172"/>
       <c r="K59" s="14" t="s">
         <v>12</v>
       </c>
@@ -19034,7 +18993,7 @@
       </c>
     </row>
     <row r="60" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J60" s="170"/>
+      <c r="J60" s="172"/>
       <c r="K60" s="14" t="s">
         <v>19</v>
       </c>
@@ -19043,7 +19002,7 @@
       </c>
     </row>
     <row r="61" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J61" s="170"/>
+      <c r="J61" s="172"/>
       <c r="K61" s="14" t="s">
         <v>13</v>
       </c>
@@ -19055,7 +19014,7 @@
       </c>
     </row>
     <row r="62" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J62" s="170"/>
+      <c r="J62" s="172"/>
       <c r="K62" s="14" t="s">
         <v>14</v>
       </c>
@@ -19064,7 +19023,7 @@
       </c>
     </row>
     <row r="63" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J63" s="170"/>
+      <c r="J63" s="172"/>
       <c r="K63" s="14" t="s">
         <v>38</v>
       </c>
@@ -19076,7 +19035,7 @@
       </c>
     </row>
     <row r="64" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J64" s="170"/>
+      <c r="J64" s="172"/>
       <c r="K64" s="14" t="s">
         <v>20</v>
       </c>
@@ -19088,7 +19047,7 @@
       </c>
     </row>
     <row r="65" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J65" s="170"/>
+      <c r="J65" s="172"/>
       <c r="K65" s="14" t="s">
         <v>33</v>
       </c>
@@ -19100,7 +19059,7 @@
       </c>
     </row>
     <row r="66" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J66" s="170"/>
+      <c r="J66" s="172"/>
       <c r="K66" s="14" t="s">
         <v>39</v>
       </c>
@@ -19112,7 +19071,7 @@
       </c>
     </row>
     <row r="67" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J67" s="170"/>
+      <c r="J67" s="172"/>
       <c r="K67" s="14" t="s">
         <v>41</v>
       </c>
@@ -19121,7 +19080,7 @@
       </c>
     </row>
     <row r="68" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J68" s="170"/>
+      <c r="J68" s="172"/>
       <c r="K68" s="14" t="s">
         <v>42</v>
       </c>
@@ -19133,7 +19092,7 @@
       </c>
     </row>
     <row r="69" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J69" s="170"/>
+      <c r="J69" s="172"/>
       <c r="K69" s="15" t="s">
         <v>15</v>
       </c>
@@ -19142,7 +19101,7 @@
       </c>
     </row>
     <row r="70" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J70" s="169" t="s">
+      <c r="J70" s="171" t="s">
         <v>81</v>
       </c>
       <c r="K70" s="14" t="s">
@@ -19156,7 +19115,7 @@
       </c>
     </row>
     <row r="71" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J71" s="170"/>
+      <c r="J71" s="172"/>
       <c r="K71" s="14" t="s">
         <v>16</v>
       </c>
@@ -19165,7 +19124,7 @@
       </c>
     </row>
     <row r="72" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J72" s="170"/>
+      <c r="J72" s="172"/>
       <c r="K72" s="14" t="s">
         <v>17</v>
       </c>
@@ -19177,7 +19136,7 @@
       </c>
     </row>
     <row r="73" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J73" s="170"/>
+      <c r="J73" s="172"/>
       <c r="K73" s="14" t="s">
         <v>34</v>
       </c>
@@ -19186,7 +19145,7 @@
       </c>
     </row>
     <row r="74" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J74" s="170"/>
+      <c r="J74" s="172"/>
       <c r="K74" s="14" t="s">
         <v>35</v>
       </c>
@@ -19195,7 +19154,7 @@
       </c>
     </row>
     <row r="75" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J75" s="170"/>
+      <c r="J75" s="172"/>
       <c r="K75" s="14" t="s">
         <v>18</v>
       </c>
@@ -19207,7 +19166,7 @@
       </c>
     </row>
     <row r="76" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J76" s="170"/>
+      <c r="J76" s="172"/>
       <c r="K76" s="14" t="s">
         <v>37</v>
       </c>
@@ -19216,7 +19175,7 @@
       </c>
     </row>
     <row r="77" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J77" s="170"/>
+      <c r="J77" s="172"/>
       <c r="K77" s="14" t="s">
         <v>36</v>
       </c>
@@ -19228,7 +19187,7 @@
       </c>
     </row>
     <row r="78" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J78" s="170"/>
+      <c r="J78" s="172"/>
       <c r="K78" s="14" t="s">
         <v>12</v>
       </c>
@@ -19237,7 +19196,7 @@
       </c>
     </row>
     <row r="79" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J79" s="170"/>
+      <c r="J79" s="172"/>
       <c r="K79" s="14" t="s">
         <v>19</v>
       </c>
@@ -19249,7 +19208,7 @@
       </c>
     </row>
     <row r="80" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J80" s="170"/>
+      <c r="J80" s="172"/>
       <c r="K80" s="14" t="s">
         <v>13</v>
       </c>
@@ -19261,7 +19220,7 @@
       </c>
     </row>
     <row r="81" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J81" s="170"/>
+      <c r="J81" s="172"/>
       <c r="K81" s="14" t="s">
         <v>14</v>
       </c>
@@ -19273,7 +19232,7 @@
       </c>
     </row>
     <row r="82" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J82" s="170"/>
+      <c r="J82" s="172"/>
       <c r="K82" s="14" t="s">
         <v>38</v>
       </c>
@@ -19288,7 +19247,7 @@
       </c>
     </row>
     <row r="83" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J83" s="170"/>
+      <c r="J83" s="172"/>
       <c r="K83" s="14" t="s">
         <v>20</v>
       </c>
@@ -19297,7 +19256,7 @@
       </c>
     </row>
     <row r="84" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J84" s="170"/>
+      <c r="J84" s="172"/>
       <c r="K84" s="14" t="s">
         <v>33</v>
       </c>
@@ -19306,7 +19265,7 @@
       </c>
     </row>
     <row r="85" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J85" s="170"/>
+      <c r="J85" s="172"/>
       <c r="K85" s="14" t="s">
         <v>39</v>
       </c>
@@ -19315,7 +19274,7 @@
       </c>
     </row>
     <row r="86" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J86" s="170"/>
+      <c r="J86" s="172"/>
       <c r="K86" s="14" t="s">
         <v>41</v>
       </c>
@@ -19330,7 +19289,7 @@
       </c>
     </row>
     <row r="87" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J87" s="170"/>
+      <c r="J87" s="172"/>
       <c r="K87" s="14" t="s">
         <v>42</v>
       </c>
@@ -19339,7 +19298,7 @@
       </c>
     </row>
     <row r="88" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J88" s="170"/>
+      <c r="J88" s="172"/>
       <c r="K88" s="15" t="s">
         <v>15</v>
       </c>
@@ -19351,7 +19310,7 @@
       </c>
     </row>
     <row r="89" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J89" s="169" t="s">
+      <c r="J89" s="171" t="s">
         <v>82</v>
       </c>
       <c r="K89" s="14" t="s">
@@ -19359,125 +19318,125 @@
       </c>
     </row>
     <row r="90" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J90" s="170"/>
+      <c r="J90" s="172"/>
       <c r="K90" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="91" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J91" s="170"/>
+      <c r="J91" s="172"/>
       <c r="K91" s="14" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="92" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J92" s="170"/>
+      <c r="J92" s="172"/>
       <c r="K92" s="14" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="93" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J93" s="170"/>
+      <c r="J93" s="172"/>
       <c r="K93" s="14" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="94" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J94" s="170"/>
+      <c r="J94" s="172"/>
       <c r="K94" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="95" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J95" s="170"/>
+      <c r="J95" s="172"/>
       <c r="K95" s="14" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="96" spans="10:20" x14ac:dyDescent="0.2">
-      <c r="J96" s="170"/>
+      <c r="J96" s="172"/>
       <c r="K96" s="14" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="97" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J97" s="170"/>
+      <c r="J97" s="172"/>
       <c r="K97" s="14" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="98" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J98" s="170"/>
+      <c r="J98" s="172"/>
       <c r="K98" s="14" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="99" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J99" s="170"/>
+      <c r="J99" s="172"/>
       <c r="K99" s="14" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="100" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J100" s="170"/>
+      <c r="J100" s="172"/>
       <c r="K100" s="14" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="101" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J101" s="170"/>
+      <c r="J101" s="172"/>
       <c r="K101" s="14" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="102" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J102" s="170"/>
+      <c r="J102" s="172"/>
       <c r="K102" s="14" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="103" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J103" s="170"/>
+      <c r="J103" s="172"/>
       <c r="K103" s="14" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="104" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J104" s="170"/>
+      <c r="J104" s="172"/>
       <c r="K104" s="14" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="105" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J105" s="170"/>
+      <c r="J105" s="172"/>
       <c r="K105" s="14" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="106" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J106" s="170"/>
+      <c r="J106" s="172"/>
       <c r="K106" s="14" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="107" spans="10:11" x14ac:dyDescent="0.2">
-      <c r="J107" s="170"/>
+      <c r="J107" s="172"/>
       <c r="K107" s="15" t="s">
         <v>15</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="J89:J107"/>
+    <mergeCell ref="J70:J88"/>
+    <mergeCell ref="J32:J50"/>
+    <mergeCell ref="J51:J69"/>
+    <mergeCell ref="J30:S30"/>
     <mergeCell ref="B2:G2"/>
     <mergeCell ref="B4:B8"/>
     <mergeCell ref="B9:B13"/>
     <mergeCell ref="B14:B18"/>
     <mergeCell ref="B19:B23"/>
-    <mergeCell ref="J89:J107"/>
-    <mergeCell ref="J70:J88"/>
-    <mergeCell ref="J32:J50"/>
-    <mergeCell ref="J51:J69"/>
-    <mergeCell ref="J30:S30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
demographics summaries and correlation modeling
</commit_message>
<xml_diff>
--- a/Figures/summaries_csvs/model_summary.xlsx
+++ b/Figures/summaries_csvs/model_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kunalpalawat/Documents/GitHub/project-harvest-fork/Figures/summaries_csvs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFC8D1E3-623A-2443-BD84-D3454FD68662}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C68F66EC-9317-F347-9D2D-4ED07A813D27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" activeTab="4" xr2:uid="{BBA561B4-B8F2-A543-83D5-E4C6EA31C59C}"/>
   </bookViews>
@@ -22786,7 +22786,7 @@
   <dimension ref="B2:S49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>